<commit_message>
Commit Kedua Penyusunan Denah Wisuda USK 163
Hasil Penyusunan Pertama Denah Wisuda USK Periode 163 Hari ke 3, Jum'at 22 November 2024 (Penambahan Kursi Kosong di nomor 362)
</commit_message>
<xml_diff>
--- a/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
+++ b/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data Hary\Denah Wisuda 163\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2240FAE-3C52-472C-97CF-D50D6465BCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665E2EC3-4570-41C9-A874-04A3A555FBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3596,33 +3596,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3724,6 +3697,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4080,8 +4080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="Y41" sqref="Y41"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34:V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4097,49 +4097,49 @@
     <row r="1" spans="1:46" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="227" t="s">
+      <c r="C1" s="264" t="s">
         <v>763</v>
       </c>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
-      <c r="K1" s="228"/>
-      <c r="L1" s="228"/>
-      <c r="M1" s="228"/>
-      <c r="N1" s="228"/>
-      <c r="O1" s="228"/>
-      <c r="P1" s="228"/>
-      <c r="Q1" s="228"/>
-      <c r="R1" s="228"/>
-      <c r="S1" s="228"/>
-      <c r="T1" s="228"/>
-      <c r="U1" s="228"/>
-      <c r="V1" s="228"/>
-      <c r="W1" s="228"/>
-      <c r="X1" s="228"/>
-      <c r="Y1" s="228"/>
-      <c r="Z1" s="228"/>
-      <c r="AA1" s="228"/>
-      <c r="AB1" s="228"/>
-      <c r="AC1" s="228"/>
-      <c r="AD1" s="228"/>
-      <c r="AE1" s="228"/>
-      <c r="AF1" s="228"/>
-      <c r="AG1" s="228"/>
-      <c r="AH1" s="228"/>
-      <c r="AI1" s="228"/>
-      <c r="AJ1" s="228"/>
-      <c r="AK1" s="228"/>
-      <c r="AL1" s="228"/>
-      <c r="AM1" s="228"/>
-      <c r="AN1" s="228"/>
-      <c r="AO1" s="228"/>
-      <c r="AP1" s="228"/>
-      <c r="AQ1" s="229"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="265"/>
+      <c r="M1" s="265"/>
+      <c r="N1" s="265"/>
+      <c r="O1" s="265"/>
+      <c r="P1" s="265"/>
+      <c r="Q1" s="265"/>
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="265"/>
+      <c r="V1" s="265"/>
+      <c r="W1" s="265"/>
+      <c r="X1" s="265"/>
+      <c r="Y1" s="265"/>
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="265"/>
+      <c r="AD1" s="265"/>
+      <c r="AE1" s="265"/>
+      <c r="AF1" s="265"/>
+      <c r="AG1" s="265"/>
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
+      <c r="AK1" s="265"/>
+      <c r="AL1" s="265"/>
+      <c r="AM1" s="265"/>
+      <c r="AN1" s="265"/>
+      <c r="AO1" s="265"/>
+      <c r="AP1" s="265"/>
+      <c r="AQ1" s="266"/>
       <c r="AR1" s="33"/>
       <c r="AS1" s="179"/>
     </row>
@@ -4148,45 +4148,45 @@
       <c r="B2" s="33"/>
       <c r="C2" s="128"/>
       <c r="D2" s="129"/>
-      <c r="E2" s="230" t="s">
+      <c r="E2" s="267" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="230"/>
-      <c r="G2" s="230"/>
-      <c r="H2" s="230"/>
-      <c r="I2" s="230"/>
-      <c r="J2" s="230"/>
-      <c r="K2" s="230"/>
-      <c r="L2" s="230"/>
-      <c r="M2" s="230"/>
-      <c r="N2" s="230"/>
-      <c r="O2" s="230"/>
-      <c r="P2" s="230"/>
-      <c r="Q2" s="230"/>
-      <c r="R2" s="230"/>
-      <c r="S2" s="230"/>
-      <c r="T2" s="230"/>
-      <c r="U2" s="230"/>
-      <c r="V2" s="230"/>
-      <c r="W2" s="230"/>
-      <c r="X2" s="230"/>
-      <c r="Y2" s="230"/>
-      <c r="Z2" s="230"/>
-      <c r="AA2" s="230"/>
-      <c r="AB2" s="230"/>
-      <c r="AC2" s="230"/>
-      <c r="AD2" s="230"/>
-      <c r="AE2" s="230"/>
-      <c r="AF2" s="230"/>
-      <c r="AG2" s="230"/>
-      <c r="AH2" s="230"/>
-      <c r="AI2" s="230"/>
-      <c r="AJ2" s="230"/>
-      <c r="AK2" s="230"/>
-      <c r="AL2" s="230"/>
-      <c r="AM2" s="230"/>
-      <c r="AN2" s="230"/>
-      <c r="AO2" s="230"/>
+      <c r="F2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="267"/>
+      <c r="J2" s="267"/>
+      <c r="K2" s="267"/>
+      <c r="L2" s="267"/>
+      <c r="M2" s="267"/>
+      <c r="N2" s="267"/>
+      <c r="O2" s="267"/>
+      <c r="P2" s="267"/>
+      <c r="Q2" s="267"/>
+      <c r="R2" s="267"/>
+      <c r="S2" s="267"/>
+      <c r="T2" s="267"/>
+      <c r="U2" s="267"/>
+      <c r="V2" s="267"/>
+      <c r="W2" s="267"/>
+      <c r="X2" s="267"/>
+      <c r="Y2" s="267"/>
+      <c r="Z2" s="267"/>
+      <c r="AA2" s="267"/>
+      <c r="AB2" s="267"/>
+      <c r="AC2" s="267"/>
+      <c r="AD2" s="267"/>
+      <c r="AE2" s="267"/>
+      <c r="AF2" s="267"/>
+      <c r="AG2" s="267"/>
+      <c r="AH2" s="267"/>
+      <c r="AI2" s="267"/>
+      <c r="AJ2" s="267"/>
+      <c r="AK2" s="267"/>
+      <c r="AL2" s="267"/>
+      <c r="AM2" s="267"/>
+      <c r="AN2" s="267"/>
+      <c r="AO2" s="267"/>
       <c r="AP2" s="129"/>
       <c r="AQ2" s="130"/>
       <c r="AR2" s="33"/>
@@ -4472,7 +4472,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="123"/>
-      <c r="C7" s="249" t="s">
+      <c r="C7" s="240" t="s">
         <v>772</v>
       </c>
       <c r="D7" s="191" t="s">
@@ -4868,10 +4868,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="147"/>
-      <c r="C10" s="250" t="s">
+      <c r="C10" s="241" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="251" t="s">
+      <c r="D10" s="242" t="s">
         <v>773</v>
       </c>
       <c r="E10" s="192" t="s">
@@ -4889,10 +4889,10 @@
       <c r="I10" s="192" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="253" t="s">
+      <c r="J10" s="244" t="s">
         <v>774</v>
       </c>
-      <c r="K10" s="252" t="s">
+      <c r="K10" s="243" t="s">
         <v>775</v>
       </c>
       <c r="L10" s="200" t="s">
@@ -4910,38 +4910,38 @@
       <c r="P10" s="200" t="s">
         <v>98</v>
       </c>
-      <c r="Q10" s="256" t="s">
+      <c r="Q10" s="247" t="s">
         <v>776</v>
       </c>
-      <c r="R10" s="255" t="s">
+      <c r="R10" s="246" t="s">
         <v>100</v>
       </c>
-      <c r="S10" s="255" t="s">
+      <c r="S10" s="246" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="255" t="s">
+      <c r="T10" s="246" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="255" t="s">
+      <c r="U10" s="246" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="255" t="s">
+      <c r="V10" s="246" t="s">
         <v>58</v>
       </c>
       <c r="W10" s="137"/>
-      <c r="X10" s="255" t="s">
+      <c r="X10" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Y10" s="255" t="s">
+      <c r="Y10" s="246" t="s">
         <v>57</v>
       </c>
-      <c r="Z10" s="255" t="s">
+      <c r="Z10" s="246" t="s">
         <v>56</v>
       </c>
-      <c r="AA10" s="255" t="s">
+      <c r="AA10" s="246" t="s">
         <v>101</v>
       </c>
-      <c r="AB10" s="257" t="s">
+      <c r="AB10" s="248" t="s">
         <v>145</v>
       </c>
       <c r="AC10" s="193" t="s">
@@ -5135,7 +5135,7 @@
       <c r="A12" s="133">
         <v>6</v>
       </c>
-      <c r="B12" s="270"/>
+      <c r="B12" s="261"/>
       <c r="C12" s="193">
         <v>120</v>
       </c>
@@ -6469,11 +6469,11 @@
       <c r="K22" s="113"/>
       <c r="L22" s="113"/>
       <c r="M22" s="113"/>
-      <c r="N22" s="231" t="s">
+      <c r="N22" s="268" t="s">
         <v>575</v>
       </c>
-      <c r="O22" s="231"/>
-      <c r="P22" s="231"/>
+      <c r="O22" s="268"/>
+      <c r="P22" s="268"/>
       <c r="Q22" s="113"/>
       <c r="R22" s="113"/>
       <c r="S22" s="113"/>
@@ -6487,11 +6487,11 @@
       <c r="AA22" s="113"/>
       <c r="AB22" s="113"/>
       <c r="AC22" s="113"/>
-      <c r="AD22" s="231" t="s">
+      <c r="AD22" s="268" t="s">
         <v>575</v>
       </c>
-      <c r="AE22" s="231"/>
-      <c r="AF22" s="231"/>
+      <c r="AE22" s="268"/>
+      <c r="AF22" s="268"/>
       <c r="AG22" s="113"/>
       <c r="AH22" s="113"/>
       <c r="AI22" s="113"/>
@@ -6508,34 +6508,34 @@
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" s="225"/>
-      <c r="B23" s="258">
+      <c r="B23" s="249">
         <v>385</v>
       </c>
-      <c r="C23" s="258">
+      <c r="C23" s="249">
         <v>386</v>
       </c>
-      <c r="D23" s="258">
+      <c r="D23" s="249">
         <v>387</v>
       </c>
-      <c r="E23" s="258">
+      <c r="E23" s="249">
         <v>388</v>
       </c>
-      <c r="F23" s="258">
+      <c r="F23" s="249">
         <v>389</v>
       </c>
-      <c r="G23" s="258">
+      <c r="G23" s="249">
         <v>390</v>
       </c>
-      <c r="H23" s="258">
+      <c r="H23" s="249">
         <v>391</v>
       </c>
-      <c r="I23" s="258">
+      <c r="I23" s="249">
         <v>392</v>
       </c>
-      <c r="J23" s="258">
+      <c r="J23" s="249">
         <v>393</v>
       </c>
-      <c r="K23" s="258">
+      <c r="K23" s="249">
         <v>394</v>
       </c>
       <c r="L23" s="149"/>
@@ -6585,68 +6585,68 @@
       </c>
       <c r="AG23" s="149"/>
       <c r="AH23" s="149"/>
-      <c r="AI23" s="262">
+      <c r="AI23" s="253">
         <v>394</v>
       </c>
-      <c r="AJ23" s="262">
+      <c r="AJ23" s="253">
         <v>393</v>
       </c>
-      <c r="AK23" s="262">
+      <c r="AK23" s="253">
         <v>392</v>
       </c>
-      <c r="AL23" s="262">
+      <c r="AL23" s="253">
         <v>391</v>
       </c>
-      <c r="AM23" s="262">
+      <c r="AM23" s="253">
         <v>390</v>
       </c>
-      <c r="AN23" s="262">
+      <c r="AN23" s="253">
         <v>389</v>
       </c>
-      <c r="AO23" s="262">
+      <c r="AO23" s="253">
         <v>388</v>
       </c>
-      <c r="AP23" s="262">
+      <c r="AP23" s="253">
         <v>387</v>
       </c>
-      <c r="AQ23" s="262">
+      <c r="AQ23" s="253">
         <v>386</v>
       </c>
-      <c r="AR23" s="262">
+      <c r="AR23" s="253">
         <v>385</v>
       </c>
       <c r="AS23" s="179"/>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="123"/>
-      <c r="B24" s="262">
+      <c r="B24" s="253">
         <v>395</v>
       </c>
-      <c r="C24" s="262">
+      <c r="C24" s="253">
         <v>396</v>
       </c>
-      <c r="D24" s="262">
+      <c r="D24" s="253">
         <v>397</v>
       </c>
-      <c r="E24" s="262">
+      <c r="E24" s="253">
         <v>398</v>
       </c>
-      <c r="F24" s="262">
+      <c r="F24" s="253">
         <v>399</v>
       </c>
-      <c r="G24" s="262">
+      <c r="G24" s="253">
         <v>400</v>
       </c>
-      <c r="H24" s="262">
+      <c r="H24" s="253">
         <v>401</v>
       </c>
-      <c r="I24" s="262">
+      <c r="I24" s="253">
         <v>402</v>
       </c>
-      <c r="J24" s="262">
+      <c r="J24" s="253">
         <v>403</v>
       </c>
-      <c r="K24" s="262">
+      <c r="K24" s="253">
         <v>404</v>
       </c>
       <c r="L24" s="149"/>
@@ -6676,68 +6676,68 @@
       </c>
       <c r="AG24" s="149"/>
       <c r="AH24" s="149"/>
-      <c r="AI24" s="262">
+      <c r="AI24" s="253">
         <v>404</v>
       </c>
-      <c r="AJ24" s="262">
+      <c r="AJ24" s="253">
         <v>403</v>
       </c>
-      <c r="AK24" s="262">
+      <c r="AK24" s="253">
         <v>402</v>
       </c>
-      <c r="AL24" s="262">
+      <c r="AL24" s="253">
         <v>401</v>
       </c>
-      <c r="AM24" s="262">
+      <c r="AM24" s="253">
         <v>400</v>
       </c>
-      <c r="AN24" s="262">
+      <c r="AN24" s="253">
         <v>399</v>
       </c>
-      <c r="AO24" s="262">
+      <c r="AO24" s="253">
         <v>398</v>
       </c>
-      <c r="AP24" s="262">
+      <c r="AP24" s="253">
         <v>397</v>
       </c>
-      <c r="AQ24" s="262">
+      <c r="AQ24" s="253">
         <v>396</v>
       </c>
-      <c r="AR24" s="262">
+      <c r="AR24" s="253">
         <v>395</v>
       </c>
       <c r="AS24" s="179"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="124"/>
-      <c r="B25" s="263">
+      <c r="B25" s="254">
         <v>405</v>
       </c>
-      <c r="C25" s="263">
+      <c r="C25" s="254">
         <v>406</v>
       </c>
-      <c r="D25" s="263">
+      <c r="D25" s="254">
         <v>407</v>
       </c>
-      <c r="E25" s="263">
+      <c r="E25" s="254">
         <v>408</v>
       </c>
-      <c r="F25" s="263">
+      <c r="F25" s="254">
         <v>409</v>
       </c>
-      <c r="G25" s="263">
+      <c r="G25" s="254">
         <v>410</v>
       </c>
-      <c r="H25" s="263">
+      <c r="H25" s="254">
         <v>411</v>
       </c>
-      <c r="I25" s="263">
+      <c r="I25" s="254">
         <v>412</v>
       </c>
-      <c r="J25" s="263">
+      <c r="J25" s="254">
         <v>413</v>
       </c>
-      <c r="K25" s="263">
+      <c r="K25" s="254">
         <v>414</v>
       </c>
       <c r="L25" s="149"/>
@@ -6767,74 +6767,74 @@
       </c>
       <c r="AG25" s="149"/>
       <c r="AH25" s="149"/>
-      <c r="AI25" s="263">
+      <c r="AI25" s="254">
         <v>414</v>
       </c>
-      <c r="AJ25" s="263">
+      <c r="AJ25" s="254">
         <v>413</v>
       </c>
-      <c r="AK25" s="263">
+      <c r="AK25" s="254">
         <v>412</v>
       </c>
-      <c r="AL25" s="263">
+      <c r="AL25" s="254">
         <v>411</v>
       </c>
-      <c r="AM25" s="263">
+      <c r="AM25" s="254">
         <v>410</v>
       </c>
-      <c r="AN25" s="263">
+      <c r="AN25" s="254">
         <v>409</v>
       </c>
-      <c r="AO25" s="263">
+      <c r="AO25" s="254">
         <v>408</v>
       </c>
-      <c r="AP25" s="263">
+      <c r="AP25" s="254">
         <v>407</v>
       </c>
-      <c r="AQ25" s="263">
+      <c r="AQ25" s="254">
         <v>406</v>
       </c>
-      <c r="AR25" s="263">
+      <c r="AR25" s="254">
         <v>405</v>
       </c>
       <c r="AS25" s="179"/>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="123"/>
-      <c r="B26" s="264">
+      <c r="B26" s="255">
         <v>415</v>
       </c>
-      <c r="C26" s="264">
+      <c r="C26" s="255">
         <v>416</v>
       </c>
-      <c r="D26" s="264">
+      <c r="D26" s="255">
         <v>417</v>
       </c>
-      <c r="E26" s="264">
+      <c r="E26" s="255">
         <v>418</v>
       </c>
-      <c r="F26" s="264">
+      <c r="F26" s="255">
         <v>419</v>
       </c>
-      <c r="G26" s="264">
+      <c r="G26" s="255">
         <v>420</v>
       </c>
-      <c r="H26" s="264">
+      <c r="H26" s="255">
         <v>421</v>
       </c>
-      <c r="I26" s="264">
+      <c r="I26" s="255">
         <v>422</v>
       </c>
-      <c r="J26" s="264">
+      <c r="J26" s="255">
         <v>423</v>
       </c>
-      <c r="K26" s="264">
+      <c r="K26" s="255">
         <v>424</v>
       </c>
-      <c r="L26" s="264">
+      <c r="L26" s="255">
         <v>425</v>
       </c>
-      <c r="M26" s="264">
+      <c r="M26" s="255">
         <v>426</v>
       </c>
       <c r="N26" s="155">
@@ -6888,80 +6888,80 @@
       <c r="AF26" s="157">
         <v>4</v>
       </c>
-      <c r="AG26" s="262">
+      <c r="AG26" s="253">
         <v>426</v>
       </c>
-      <c r="AH26" s="266">
+      <c r="AH26" s="257">
         <v>425</v>
       </c>
-      <c r="AI26" s="262">
+      <c r="AI26" s="253">
         <v>424</v>
       </c>
-      <c r="AJ26" s="266">
+      <c r="AJ26" s="257">
         <v>423</v>
       </c>
-      <c r="AK26" s="262">
+      <c r="AK26" s="253">
         <v>422</v>
       </c>
-      <c r="AL26" s="266">
+      <c r="AL26" s="257">
         <v>421</v>
       </c>
-      <c r="AM26" s="262">
+      <c r="AM26" s="253">
         <v>420</v>
       </c>
-      <c r="AN26" s="266">
+      <c r="AN26" s="257">
         <v>419</v>
       </c>
-      <c r="AO26" s="262">
+      <c r="AO26" s="253">
         <v>418</v>
       </c>
-      <c r="AP26" s="266">
+      <c r="AP26" s="257">
         <v>417</v>
       </c>
-      <c r="AQ26" s="262">
+      <c r="AQ26" s="253">
         <v>416</v>
       </c>
-      <c r="AR26" s="266">
+      <c r="AR26" s="257">
         <v>415</v>
       </c>
       <c r="AS26" s="179"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="115"/>
-      <c r="B27" s="264">
+      <c r="B27" s="255">
         <v>427</v>
       </c>
-      <c r="C27" s="264">
+      <c r="C27" s="255">
         <v>428</v>
       </c>
-      <c r="D27" s="264">
+      <c r="D27" s="255">
         <v>429</v>
       </c>
-      <c r="E27" s="264">
+      <c r="E27" s="255">
         <v>430</v>
       </c>
-      <c r="F27" s="264">
+      <c r="F27" s="255">
         <v>431</v>
       </c>
-      <c r="G27" s="264">
+      <c r="G27" s="255">
         <v>432</v>
       </c>
-      <c r="H27" s="264">
+      <c r="H27" s="255">
         <v>433</v>
       </c>
-      <c r="I27" s="264">
+      <c r="I27" s="255">
         <v>434</v>
       </c>
-      <c r="J27" s="264">
+      <c r="J27" s="255">
         <v>435</v>
       </c>
-      <c r="K27" s="264">
+      <c r="K27" s="255">
         <v>436</v>
       </c>
-      <c r="L27" s="264">
+      <c r="L27" s="255">
         <v>437</v>
       </c>
-      <c r="M27" s="264">
+      <c r="M27" s="255">
         <v>438</v>
       </c>
       <c r="N27" s="155">
@@ -7015,80 +7015,80 @@
       <c r="AF27" s="157">
         <v>5</v>
       </c>
-      <c r="AG27" s="262">
+      <c r="AG27" s="253">
         <v>438</v>
       </c>
-      <c r="AH27" s="266">
+      <c r="AH27" s="257">
         <v>437</v>
       </c>
-      <c r="AI27" s="262">
+      <c r="AI27" s="253">
         <v>436</v>
       </c>
-      <c r="AJ27" s="262">
+      <c r="AJ27" s="253">
         <v>435</v>
       </c>
-      <c r="AK27" s="262">
+      <c r="AK27" s="253">
         <v>434</v>
       </c>
-      <c r="AL27" s="262">
+      <c r="AL27" s="253">
         <v>433</v>
       </c>
-      <c r="AM27" s="262">
+      <c r="AM27" s="253">
         <v>432</v>
       </c>
-      <c r="AN27" s="262">
+      <c r="AN27" s="253">
         <v>431</v>
       </c>
-      <c r="AO27" s="267" t="s">
+      <c r="AO27" s="258" t="s">
         <v>758</v>
       </c>
-      <c r="AP27" s="262">
+      <c r="AP27" s="253">
         <v>429</v>
       </c>
-      <c r="AQ27" s="262">
+      <c r="AQ27" s="253">
         <v>428</v>
       </c>
-      <c r="AR27" s="262">
+      <c r="AR27" s="253">
         <v>427</v>
       </c>
       <c r="AS27" s="179"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="119"/>
-      <c r="B28" s="264">
+      <c r="B28" s="255">
         <v>439</v>
       </c>
-      <c r="C28" s="264">
+      <c r="C28" s="255">
         <v>440</v>
       </c>
-      <c r="D28" s="264">
+      <c r="D28" s="255">
         <v>441</v>
       </c>
-      <c r="E28" s="264">
+      <c r="E28" s="255">
         <v>442</v>
       </c>
-      <c r="F28" s="264">
+      <c r="F28" s="255">
         <v>443</v>
       </c>
-      <c r="G28" s="264">
+      <c r="G28" s="255">
         <v>444</v>
       </c>
-      <c r="H28" s="264">
+      <c r="H28" s="255">
         <v>445</v>
       </c>
-      <c r="I28" s="264">
+      <c r="I28" s="255">
         <v>446</v>
       </c>
-      <c r="J28" s="264">
+      <c r="J28" s="255">
         <v>447</v>
       </c>
-      <c r="K28" s="264">
+      <c r="K28" s="255">
         <v>448</v>
       </c>
-      <c r="L28" s="264">
+      <c r="L28" s="255">
         <v>449</v>
       </c>
-      <c r="M28" s="264">
+      <c r="M28" s="255">
         <v>450</v>
       </c>
       <c r="N28" s="155">
@@ -7142,80 +7142,80 @@
       <c r="AF28" s="157">
         <v>6</v>
       </c>
-      <c r="AG28" s="262">
+      <c r="AG28" s="253">
         <v>450</v>
       </c>
-      <c r="AH28" s="266">
+      <c r="AH28" s="257">
         <v>449</v>
       </c>
-      <c r="AI28" s="262">
+      <c r="AI28" s="253">
         <v>448</v>
       </c>
-      <c r="AJ28" s="262">
+      <c r="AJ28" s="253">
         <v>447</v>
       </c>
-      <c r="AK28" s="262">
+      <c r="AK28" s="253">
         <v>446</v>
       </c>
-      <c r="AL28" s="262">
+      <c r="AL28" s="253">
         <v>445</v>
       </c>
-      <c r="AM28" s="262">
+      <c r="AM28" s="253">
         <v>444</v>
       </c>
-      <c r="AN28" s="262">
+      <c r="AN28" s="253">
         <v>443</v>
       </c>
-      <c r="AO28" s="262">
+      <c r="AO28" s="253">
         <v>442</v>
       </c>
-      <c r="AP28" s="262">
+      <c r="AP28" s="253">
         <v>441</v>
       </c>
-      <c r="AQ28" s="262">
+      <c r="AQ28" s="253">
         <v>440</v>
       </c>
-      <c r="AR28" s="262">
+      <c r="AR28" s="253">
         <v>439</v>
       </c>
       <c r="AS28" s="180"/>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="127"/>
-      <c r="B29" s="265">
+      <c r="B29" s="256">
         <v>451</v>
       </c>
-      <c r="C29" s="265">
+      <c r="C29" s="256">
         <v>452</v>
       </c>
-      <c r="D29" s="265">
+      <c r="D29" s="256">
         <v>453</v>
       </c>
-      <c r="E29" s="265">
+      <c r="E29" s="256">
         <v>454</v>
       </c>
-      <c r="F29" s="265">
+      <c r="F29" s="256">
         <v>455</v>
       </c>
-      <c r="G29" s="265">
+      <c r="G29" s="256">
         <v>456</v>
       </c>
-      <c r="H29" s="265">
+      <c r="H29" s="256">
         <v>457</v>
       </c>
-      <c r="I29" s="265">
+      <c r="I29" s="256">
         <v>458</v>
       </c>
-      <c r="J29" s="265">
+      <c r="J29" s="256">
         <v>459</v>
       </c>
-      <c r="K29" s="265">
+      <c r="K29" s="256">
         <v>460</v>
       </c>
-      <c r="L29" s="265">
+      <c r="L29" s="256">
         <v>461</v>
       </c>
-      <c r="M29" s="265">
+      <c r="M29" s="256">
         <v>462</v>
       </c>
       <c r="N29" s="155">
@@ -7236,14 +7236,14 @@
       <c r="S29" s="193">
         <v>325</v>
       </c>
-      <c r="T29" s="259" t="s">
+      <c r="T29" s="253">
+        <v>326</v>
+      </c>
+      <c r="U29" s="250" t="s">
         <v>779</v>
       </c>
-      <c r="U29" s="271" t="s">
+      <c r="V29" s="262" t="s">
         <v>364</v>
-      </c>
-      <c r="V29" s="195">
-        <v>322</v>
       </c>
       <c r="W29" s="154"/>
       <c r="X29" s="195">
@@ -7274,77 +7274,77 @@
       <c r="AG29" s="194">
         <v>462</v>
       </c>
-      <c r="AH29" s="268">
+      <c r="AH29" s="259">
         <v>461</v>
       </c>
       <c r="AI29" s="194">
         <v>460</v>
       </c>
-      <c r="AJ29" s="268">
+      <c r="AJ29" s="259">
         <v>459</v>
       </c>
       <c r="AK29" s="194">
         <v>458</v>
       </c>
-      <c r="AL29" s="268">
+      <c r="AL29" s="259">
         <v>457</v>
       </c>
       <c r="AM29" s="194">
         <v>456</v>
       </c>
-      <c r="AN29" s="268">
+      <c r="AN29" s="259">
         <v>455</v>
       </c>
       <c r="AO29" s="194">
         <v>454</v>
       </c>
-      <c r="AP29" s="268">
+      <c r="AP29" s="259">
         <v>453</v>
       </c>
       <c r="AQ29" s="194">
         <v>452</v>
       </c>
-      <c r="AR29" s="268">
+      <c r="AR29" s="259">
         <v>451</v>
       </c>
       <c r="AS29" s="179"/>
     </row>
     <row r="30" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="115"/>
-      <c r="B30" s="262">
+      <c r="B30" s="253">
         <v>463</v>
       </c>
-      <c r="C30" s="262">
+      <c r="C30" s="253">
         <v>464</v>
       </c>
-      <c r="D30" s="262">
+      <c r="D30" s="253">
         <v>465</v>
       </c>
-      <c r="E30" s="262">
+      <c r="E30" s="253">
         <v>466</v>
       </c>
-      <c r="F30" s="262">
+      <c r="F30" s="253">
         <v>467</v>
       </c>
-      <c r="G30" s="262">
+      <c r="G30" s="253">
         <v>468</v>
       </c>
-      <c r="H30" s="262">
+      <c r="H30" s="253">
         <v>469</v>
       </c>
-      <c r="I30" s="262">
+      <c r="I30" s="253">
         <v>470</v>
       </c>
-      <c r="J30" s="262">
+      <c r="J30" s="253">
         <v>471</v>
       </c>
-      <c r="K30" s="262">
+      <c r="K30" s="253">
         <v>472</v>
       </c>
-      <c r="L30" s="262">
+      <c r="L30" s="253">
         <v>473</v>
       </c>
-      <c r="M30" s="262">
+      <c r="M30" s="253">
         <v>474</v>
       </c>
       <c r="N30" s="113">
@@ -7398,79 +7398,79 @@
       <c r="AF30" s="160">
         <v>8</v>
       </c>
-      <c r="AG30" s="262">
+      <c r="AG30" s="253">
         <v>474</v>
       </c>
-      <c r="AH30" s="266">
+      <c r="AH30" s="257">
         <v>473</v>
       </c>
-      <c r="AI30" s="262">
+      <c r="AI30" s="253">
         <v>472</v>
       </c>
-      <c r="AJ30" s="262">
+      <c r="AJ30" s="253">
         <v>471</v>
       </c>
-      <c r="AK30" s="262">
+      <c r="AK30" s="253">
         <v>470</v>
       </c>
-      <c r="AL30" s="262">
+      <c r="AL30" s="253">
         <v>469</v>
       </c>
-      <c r="AM30" s="262">
+      <c r="AM30" s="253">
         <v>468</v>
       </c>
-      <c r="AN30" s="262">
+      <c r="AN30" s="253">
         <v>467</v>
       </c>
-      <c r="AO30" s="262">
+      <c r="AO30" s="253">
         <v>466</v>
       </c>
-      <c r="AP30" s="262">
+      <c r="AP30" s="253">
         <v>465</v>
       </c>
-      <c r="AQ30" s="262">
+      <c r="AQ30" s="253">
         <v>464</v>
       </c>
-      <c r="AR30" s="262">
+      <c r="AR30" s="253">
         <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="115"/>
-      <c r="B31" s="262">
+      <c r="B31" s="253">
         <v>475</v>
       </c>
-      <c r="C31" s="262">
+      <c r="C31" s="253">
         <v>476</v>
       </c>
-      <c r="D31" s="262">
+      <c r="D31" s="253">
         <v>477</v>
       </c>
-      <c r="E31" s="262">
+      <c r="E31" s="253">
         <v>478</v>
       </c>
-      <c r="F31" s="262">
+      <c r="F31" s="253">
         <v>479</v>
       </c>
-      <c r="G31" s="262">
+      <c r="G31" s="253">
         <v>480</v>
       </c>
-      <c r="H31" s="262">
+      <c r="H31" s="253">
         <v>481</v>
       </c>
-      <c r="I31" s="262">
+      <c r="I31" s="253">
         <v>482</v>
       </c>
-      <c r="J31" s="262">
+      <c r="J31" s="253">
         <v>483</v>
       </c>
-      <c r="K31" s="262">
+      <c r="K31" s="253">
         <v>484</v>
       </c>
-      <c r="L31" s="262">
+      <c r="L31" s="253">
         <v>485</v>
       </c>
-      <c r="M31" s="262">
+      <c r="M31" s="253">
         <v>486</v>
       </c>
       <c r="N31" s="155">
@@ -7524,79 +7524,79 @@
       <c r="AF31" s="186">
         <v>9</v>
       </c>
-      <c r="AG31" s="262">
+      <c r="AG31" s="253">
         <v>486</v>
       </c>
-      <c r="AH31" s="266">
+      <c r="AH31" s="257">
         <v>485</v>
       </c>
-      <c r="AI31" s="262">
+      <c r="AI31" s="253">
         <v>484</v>
       </c>
-      <c r="AJ31" s="262">
+      <c r="AJ31" s="253">
         <v>483</v>
       </c>
-      <c r="AK31" s="262">
+      <c r="AK31" s="253">
         <v>482</v>
       </c>
-      <c r="AL31" s="262">
+      <c r="AL31" s="253">
         <v>481</v>
       </c>
-      <c r="AM31" s="262">
+      <c r="AM31" s="253">
         <v>480</v>
       </c>
-      <c r="AN31" s="262">
+      <c r="AN31" s="253">
         <v>479</v>
       </c>
-      <c r="AO31" s="262">
+      <c r="AO31" s="253">
         <v>478</v>
       </c>
-      <c r="AP31" s="262">
+      <c r="AP31" s="253">
         <v>477</v>
       </c>
-      <c r="AQ31" s="262">
+      <c r="AQ31" s="253">
         <v>476</v>
       </c>
-      <c r="AR31" s="262">
+      <c r="AR31" s="253">
         <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="115"/>
-      <c r="B32" s="262">
+      <c r="B32" s="253">
         <v>487</v>
       </c>
-      <c r="C32" s="262">
+      <c r="C32" s="253">
         <v>488</v>
       </c>
-      <c r="D32" s="262">
+      <c r="D32" s="253">
         <v>489</v>
       </c>
-      <c r="E32" s="262">
+      <c r="E32" s="253">
         <v>490</v>
       </c>
-      <c r="F32" s="262">
+      <c r="F32" s="253">
         <v>491</v>
       </c>
-      <c r="G32" s="262">
+      <c r="G32" s="253">
         <v>492</v>
       </c>
-      <c r="H32" s="262">
+      <c r="H32" s="253">
         <v>493</v>
       </c>
-      <c r="I32" s="262">
+      <c r="I32" s="253">
         <v>494</v>
       </c>
-      <c r="J32" s="262">
+      <c r="J32" s="253">
         <v>495</v>
       </c>
-      <c r="K32" s="262">
+      <c r="K32" s="253">
         <v>496</v>
       </c>
-      <c r="L32" s="262">
+      <c r="L32" s="253">
         <v>497</v>
       </c>
-      <c r="M32" s="262">
+      <c r="M32" s="253">
         <v>498</v>
       </c>
       <c r="N32" s="185">
@@ -7650,79 +7650,79 @@
       <c r="AF32" s="186">
         <v>10</v>
       </c>
-      <c r="AG32" s="262">
+      <c r="AG32" s="253">
         <v>498</v>
       </c>
-      <c r="AH32" s="266">
+      <c r="AH32" s="257">
         <v>497</v>
       </c>
-      <c r="AI32" s="262">
+      <c r="AI32" s="253">
         <v>496</v>
       </c>
-      <c r="AJ32" s="262">
+      <c r="AJ32" s="253">
         <v>495</v>
       </c>
-      <c r="AK32" s="262">
+      <c r="AK32" s="253">
         <v>494</v>
       </c>
-      <c r="AL32" s="262">
+      <c r="AL32" s="253">
         <v>493</v>
       </c>
-      <c r="AM32" s="262">
+      <c r="AM32" s="253">
         <v>492</v>
       </c>
-      <c r="AN32" s="262">
+      <c r="AN32" s="253">
         <v>491</v>
       </c>
-      <c r="AO32" s="262">
+      <c r="AO32" s="253">
         <v>490</v>
       </c>
-      <c r="AP32" s="262">
+      <c r="AP32" s="253">
         <v>489</v>
       </c>
-      <c r="AQ32" s="262">
+      <c r="AQ32" s="253">
         <v>488</v>
       </c>
-      <c r="AR32" s="262">
+      <c r="AR32" s="253">
         <v>487</v>
       </c>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
-      <c r="B33" s="262">
+      <c r="B33" s="253">
         <v>499</v>
       </c>
-      <c r="C33" s="262">
+      <c r="C33" s="253">
         <v>500</v>
       </c>
-      <c r="D33" s="262">
+      <c r="D33" s="253">
         <v>501</v>
       </c>
-      <c r="E33" s="262">
+      <c r="E33" s="253">
         <v>502</v>
       </c>
-      <c r="F33" s="262">
+      <c r="F33" s="253">
         <v>503</v>
       </c>
-      <c r="G33" s="262">
+      <c r="G33" s="253">
         <v>504</v>
       </c>
-      <c r="H33" s="262">
+      <c r="H33" s="253">
         <v>505</v>
       </c>
-      <c r="I33" s="262">
+      <c r="I33" s="253">
         <v>506</v>
       </c>
-      <c r="J33" s="262">
+      <c r="J33" s="253">
         <v>507</v>
       </c>
-      <c r="K33" s="262">
+      <c r="K33" s="253">
         <v>508</v>
       </c>
-      <c r="L33" s="262">
+      <c r="L33" s="253">
         <v>509</v>
       </c>
-      <c r="M33" s="262">
+      <c r="M33" s="253">
         <v>510</v>
       </c>
       <c r="N33" s="187">
@@ -7776,37 +7776,37 @@
       <c r="AF33" s="186">
         <v>11</v>
       </c>
-      <c r="AG33" s="262">
+      <c r="AG33" s="253">
         <v>510</v>
       </c>
-      <c r="AH33" s="268">
+      <c r="AH33" s="259">
         <v>509</v>
       </c>
-      <c r="AI33" s="262">
+      <c r="AI33" s="253">
         <v>508</v>
       </c>
       <c r="AJ33" s="194">
         <v>507</v>
       </c>
-      <c r="AK33" s="262">
+      <c r="AK33" s="253">
         <v>506</v>
       </c>
       <c r="AL33" s="194">
         <v>505</v>
       </c>
-      <c r="AM33" s="262">
+      <c r="AM33" s="253">
         <v>504</v>
       </c>
       <c r="AN33" s="194">
         <v>503</v>
       </c>
-      <c r="AO33" s="262">
+      <c r="AO33" s="253">
         <v>502</v>
       </c>
       <c r="AP33" s="194">
         <v>501</v>
       </c>
-      <c r="AQ33" s="262">
+      <c r="AQ33" s="253">
         <v>500</v>
       </c>
       <c r="AR33" s="194">
@@ -7816,40 +7816,40 @@
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="115"/>
-      <c r="B34" s="262">
+      <c r="B34" s="253">
         <v>511</v>
       </c>
-      <c r="C34" s="262">
+      <c r="C34" s="253">
         <v>512</v>
       </c>
-      <c r="D34" s="262">
+      <c r="D34" s="253">
         <v>513</v>
       </c>
-      <c r="E34" s="262">
+      <c r="E34" s="253">
         <v>514</v>
       </c>
-      <c r="F34" s="262">
+      <c r="F34" s="253">
         <v>515</v>
       </c>
-      <c r="G34" s="262">
+      <c r="G34" s="253">
         <v>516</v>
       </c>
-      <c r="H34" s="262">
+      <c r="H34" s="253">
         <v>517</v>
       </c>
-      <c r="I34" s="262">
+      <c r="I34" s="253">
         <v>518</v>
       </c>
-      <c r="J34" s="262">
+      <c r="J34" s="253">
         <v>519</v>
       </c>
-      <c r="K34" s="262">
+      <c r="K34" s="253">
         <v>520</v>
       </c>
-      <c r="L34" s="262">
+      <c r="L34" s="253">
         <v>521</v>
       </c>
-      <c r="M34" s="262">
+      <c r="M34" s="253">
         <v>522</v>
       </c>
       <c r="N34" s="187">
@@ -7859,11 +7859,11 @@
       <c r="P34" s="195">
         <v>363</v>
       </c>
-      <c r="Q34" s="260" t="s">
+      <c r="Q34" s="195">
+        <v>364</v>
+      </c>
+      <c r="R34" s="251" t="s">
         <v>778</v>
-      </c>
-      <c r="R34" s="201">
-        <v>361</v>
       </c>
       <c r="S34" s="201">
         <v>360</v>
@@ -7887,53 +7887,53 @@
       <c r="Z34" s="201">
         <v>359</v>
       </c>
-      <c r="AA34" s="258">
+      <c r="AA34" s="201">
         <v>360</v>
       </c>
-      <c r="AB34" s="258">
+      <c r="AB34" s="249">
         <v>361</v>
       </c>
-      <c r="AC34" s="258">
+      <c r="AC34" s="249">
         <v>362</v>
       </c>
-      <c r="AD34" s="258">
+      <c r="AD34" s="249">
         <v>363</v>
       </c>
       <c r="AE34" s="115"/>
       <c r="AF34" s="186">
         <v>12</v>
       </c>
-      <c r="AG34" s="262">
+      <c r="AG34" s="253">
         <v>522</v>
       </c>
-      <c r="AH34" s="268">
+      <c r="AH34" s="259">
         <v>521</v>
       </c>
-      <c r="AI34" s="262">
+      <c r="AI34" s="253">
         <v>520</v>
       </c>
       <c r="AJ34" s="194">
         <v>519</v>
       </c>
-      <c r="AK34" s="262">
+      <c r="AK34" s="253">
         <v>518</v>
       </c>
       <c r="AL34" s="194">
         <v>517</v>
       </c>
-      <c r="AM34" s="262">
+      <c r="AM34" s="253">
         <v>516</v>
       </c>
       <c r="AN34" s="194">
         <v>515</v>
       </c>
-      <c r="AO34" s="262">
+      <c r="AO34" s="253">
         <v>514</v>
       </c>
       <c r="AP34" s="194">
         <v>513</v>
       </c>
-      <c r="AQ34" s="262">
+      <c r="AQ34" s="253">
         <v>512</v>
       </c>
       <c r="AR34" s="194">
@@ -7943,124 +7943,124 @@
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="115"/>
-      <c r="B35" s="262">
+      <c r="B35" s="253">
         <v>523</v>
       </c>
-      <c r="C35" s="262">
+      <c r="C35" s="253">
         <v>524</v>
       </c>
-      <c r="D35" s="262">
+      <c r="D35" s="253">
         <v>525</v>
       </c>
-      <c r="E35" s="262">
+      <c r="E35" s="253">
         <v>526</v>
       </c>
-      <c r="F35" s="262">
+      <c r="F35" s="253">
         <v>527</v>
       </c>
-      <c r="G35" s="262">
+      <c r="G35" s="253">
         <v>528</v>
       </c>
-      <c r="H35" s="262">
+      <c r="H35" s="253">
         <v>529</v>
       </c>
-      <c r="I35" s="262">
+      <c r="I35" s="253">
         <v>530</v>
       </c>
-      <c r="J35" s="262">
+      <c r="J35" s="253">
         <v>531</v>
       </c>
-      <c r="K35" s="262">
+      <c r="K35" s="253">
         <v>532</v>
       </c>
-      <c r="L35" s="262">
+      <c r="L35" s="253">
         <v>533</v>
       </c>
-      <c r="M35" s="262">
+      <c r="M35" s="253">
         <v>534</v>
       </c>
       <c r="N35" s="187">
         <v>13</v>
       </c>
       <c r="O35" s="141"/>
-      <c r="P35" s="258">
+      <c r="P35" s="249">
         <v>370</v>
       </c>
-      <c r="Q35" s="258">
+      <c r="Q35" s="249">
         <v>369</v>
       </c>
-      <c r="R35" s="258">
+      <c r="R35" s="249">
         <v>368</v>
       </c>
-      <c r="S35" s="258">
+      <c r="S35" s="249">
         <v>367</v>
       </c>
-      <c r="T35" s="262">
+      <c r="T35" s="253">
         <v>366</v>
       </c>
-      <c r="U35" s="262">
+      <c r="U35" s="253">
         <v>365</v>
       </c>
-      <c r="V35" s="262">
+      <c r="V35" s="253">
         <v>364</v>
       </c>
       <c r="W35" s="167"/>
-      <c r="X35" s="262">
+      <c r="X35" s="253">
         <v>364</v>
       </c>
-      <c r="Y35" s="262">
+      <c r="Y35" s="253">
         <v>365</v>
       </c>
-      <c r="Z35" s="262">
+      <c r="Z35" s="253">
         <v>366</v>
       </c>
-      <c r="AA35" s="262">
+      <c r="AA35" s="253">
         <v>367</v>
       </c>
-      <c r="AB35" s="262">
+      <c r="AB35" s="253">
         <v>368</v>
       </c>
-      <c r="AC35" s="262">
+      <c r="AC35" s="253">
         <v>369</v>
       </c>
-      <c r="AD35" s="262">
+      <c r="AD35" s="253">
         <v>370</v>
       </c>
       <c r="AE35" s="115"/>
       <c r="AF35" s="186">
         <v>13</v>
       </c>
-      <c r="AG35" s="262">
+      <c r="AG35" s="253">
         <v>534</v>
       </c>
-      <c r="AH35" s="268">
+      <c r="AH35" s="259">
         <v>533</v>
       </c>
-      <c r="AI35" s="262">
+      <c r="AI35" s="253">
         <v>532</v>
       </c>
       <c r="AJ35" s="194">
         <v>531</v>
       </c>
-      <c r="AK35" s="262">
+      <c r="AK35" s="253">
         <v>530</v>
       </c>
       <c r="AL35" s="194">
         <v>529</v>
       </c>
-      <c r="AM35" s="262">
+      <c r="AM35" s="253">
         <v>528</v>
       </c>
       <c r="AN35" s="194">
         <v>527</v>
       </c>
-      <c r="AO35" s="262">
+      <c r="AO35" s="253">
         <v>526</v>
       </c>
       <c r="AP35" s="194">
         <v>525</v>
       </c>
-      <c r="AQ35" s="262">
+      <c r="AQ35" s="253">
         <v>524</v>
       </c>
       <c r="AR35" s="194">
@@ -8070,87 +8070,87 @@
     </row>
     <row r="36" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="115"/>
-      <c r="B36" s="262">
+      <c r="B36" s="253">
         <v>535</v>
       </c>
-      <c r="C36" s="262">
+      <c r="C36" s="253">
         <v>536</v>
       </c>
-      <c r="D36" s="262">
+      <c r="D36" s="253">
         <v>537</v>
       </c>
-      <c r="E36" s="262">
+      <c r="E36" s="253">
         <v>538</v>
       </c>
-      <c r="F36" s="262">
+      <c r="F36" s="253">
         <v>539</v>
       </c>
-      <c r="G36" s="262">
+      <c r="G36" s="253">
         <v>540</v>
       </c>
-      <c r="H36" s="262">
+      <c r="H36" s="253">
         <v>541</v>
       </c>
-      <c r="I36" s="262">
+      <c r="I36" s="253">
         <v>542</v>
       </c>
-      <c r="J36" s="262">
+      <c r="J36" s="253">
         <v>543</v>
       </c>
-      <c r="K36" s="262">
+      <c r="K36" s="253">
         <v>544</v>
       </c>
-      <c r="L36" s="262">
+      <c r="L36" s="253">
         <v>545</v>
       </c>
-      <c r="M36" s="262">
+      <c r="M36" s="253">
         <v>546</v>
       </c>
       <c r="N36" s="187">
         <v>14</v>
       </c>
-      <c r="O36" s="269"/>
-      <c r="P36" s="262">
+      <c r="O36" s="260"/>
+      <c r="P36" s="253">
         <v>377</v>
       </c>
-      <c r="Q36" s="262">
+      <c r="Q36" s="253">
         <v>376</v>
       </c>
-      <c r="R36" s="262">
+      <c r="R36" s="253">
         <v>375</v>
       </c>
-      <c r="S36" s="262">
+      <c r="S36" s="253">
         <v>374</v>
       </c>
-      <c r="T36" s="262">
+      <c r="T36" s="253">
         <v>373</v>
       </c>
-      <c r="U36" s="262">
+      <c r="U36" s="253">
         <v>372</v>
       </c>
-      <c r="V36" s="262">
+      <c r="V36" s="253">
         <v>371</v>
       </c>
       <c r="W36" s="167"/>
-      <c r="X36" s="258">
+      <c r="X36" s="249">
         <v>371</v>
       </c>
-      <c r="Y36" s="258">
+      <c r="Y36" s="249">
         <v>372</v>
       </c>
-      <c r="Z36" s="258">
+      <c r="Z36" s="249">
         <v>373</v>
       </c>
-      <c r="AA36" s="258">
+      <c r="AA36" s="249">
         <v>374</v>
       </c>
-      <c r="AB36" s="258">
+      <c r="AB36" s="249">
         <v>375</v>
       </c>
-      <c r="AC36" s="258">
+      <c r="AC36" s="249">
         <v>376</v>
       </c>
-      <c r="AD36" s="258">
+      <c r="AD36" s="249">
         <v>377</v>
       </c>
       <c r="AE36" s="115"/>
@@ -8195,87 +8195,87 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37" s="115"/>
-      <c r="B37" s="262">
+      <c r="B37" s="253">
         <v>547</v>
       </c>
-      <c r="C37" s="262">
+      <c r="C37" s="253">
         <v>548</v>
       </c>
-      <c r="D37" s="262">
+      <c r="D37" s="253">
         <v>549</v>
       </c>
-      <c r="E37" s="262">
+      <c r="E37" s="253">
         <v>550</v>
       </c>
-      <c r="F37" s="262">
+      <c r="F37" s="253">
         <v>551</v>
       </c>
-      <c r="G37" s="262">
+      <c r="G37" s="253">
         <v>552</v>
       </c>
-      <c r="H37" s="262">
+      <c r="H37" s="253">
         <v>553</v>
       </c>
-      <c r="I37" s="262">
+      <c r="I37" s="253">
         <v>554</v>
       </c>
-      <c r="J37" s="262">
+      <c r="J37" s="253">
         <v>555</v>
       </c>
-      <c r="K37" s="262">
+      <c r="K37" s="253">
         <v>556</v>
       </c>
-      <c r="L37" s="262">
+      <c r="L37" s="253">
         <v>557</v>
       </c>
-      <c r="M37" s="262">
+      <c r="M37" s="253">
         <v>558</v>
       </c>
       <c r="N37" s="187">
         <v>15</v>
       </c>
       <c r="O37" s="141"/>
-      <c r="P37" s="258">
+      <c r="P37" s="249">
         <v>384</v>
       </c>
-      <c r="Q37" s="258">
+      <c r="Q37" s="249">
         <v>383</v>
       </c>
-      <c r="R37" s="258">
+      <c r="R37" s="249">
         <v>382</v>
       </c>
-      <c r="S37" s="258">
+      <c r="S37" s="249">
         <v>381</v>
       </c>
-      <c r="T37" s="258">
+      <c r="T37" s="249">
         <v>380</v>
       </c>
-      <c r="U37" s="258">
+      <c r="U37" s="249">
         <v>379</v>
       </c>
-      <c r="V37" s="258">
+      <c r="V37" s="249">
         <v>378</v>
       </c>
       <c r="W37" s="167"/>
-      <c r="X37" s="258">
+      <c r="X37" s="249">
         <v>378</v>
       </c>
-      <c r="Y37" s="258">
+      <c r="Y37" s="249">
         <v>379</v>
       </c>
-      <c r="Z37" s="258">
+      <c r="Z37" s="249">
         <v>380</v>
       </c>
-      <c r="AA37" s="258">
+      <c r="AA37" s="249">
         <v>381</v>
       </c>
-      <c r="AB37" s="258">
+      <c r="AB37" s="249">
         <v>382</v>
       </c>
-      <c r="AC37" s="258">
+      <c r="AC37" s="249">
         <v>383</v>
       </c>
-      <c r="AD37" s="262">
+      <c r="AD37" s="253">
         <v>384</v>
       </c>
       <c r="AE37" s="115"/>
@@ -8721,22 +8721,22 @@
       <c r="AQ47" s="115"/>
     </row>
     <row r="48" spans="1:45" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="236" t="s">
+      <c r="A48" s="227" t="s">
         <v>759</v>
       </c>
-      <c r="B48" s="242"/>
-      <c r="C48" s="237"/>
-      <c r="D48" s="237"/>
-      <c r="E48" s="237"/>
-      <c r="F48" s="237"/>
-      <c r="G48" s="237"/>
-      <c r="H48" s="237"/>
+      <c r="B48" s="233"/>
+      <c r="C48" s="228"/>
+      <c r="D48" s="228"/>
+      <c r="E48" s="228"/>
+      <c r="F48" s="228"/>
+      <c r="G48" s="228"/>
+      <c r="H48" s="228"/>
       <c r="I48" s="177"/>
       <c r="J48" s="177"/>
       <c r="K48" s="177"/>
       <c r="L48" s="177"/>
       <c r="M48" s="177"/>
-      <c r="N48" s="244" t="s">
+      <c r="N48" s="235" t="s">
         <v>759</v>
       </c>
       <c r="O48" s="207">
@@ -8745,17 +8745,17 @@
       <c r="P48" s="218" t="s">
         <v>766</v>
       </c>
-      <c r="Q48" s="245"/>
-      <c r="R48" s="246"/>
-      <c r="S48" s="247"/>
-      <c r="T48" s="247"/>
-      <c r="U48" s="247"/>
+      <c r="Q48" s="236"/>
+      <c r="R48" s="237"/>
+      <c r="S48" s="238"/>
+      <c r="T48" s="238"/>
+      <c r="U48" s="238"/>
       <c r="V48" s="143"/>
       <c r="W48" s="143"/>
       <c r="X48" s="143"/>
       <c r="Y48" s="143"/>
       <c r="Z48" s="115"/>
-      <c r="AA48" s="243" t="s">
+      <c r="AA48" s="234" t="s">
         <v>759</v>
       </c>
       <c r="AB48" s="219">
@@ -8764,10 +8764,10 @@
       <c r="AC48" s="218" t="s">
         <v>770</v>
       </c>
-      <c r="AD48" s="247"/>
-      <c r="AE48" s="247"/>
-      <c r="AF48" s="247"/>
-      <c r="AG48" s="247"/>
+      <c r="AD48" s="238"/>
+      <c r="AE48" s="238"/>
+      <c r="AF48" s="238"/>
+      <c r="AG48" s="238"/>
       <c r="AH48" s="217"/>
       <c r="AI48" s="217"/>
       <c r="AJ48" s="115"/>
@@ -8786,14 +8786,14 @@
       <c r="B49" s="206">
         <v>120</v>
       </c>
-      <c r="C49" s="240" t="s">
+      <c r="C49" s="231" t="s">
         <v>757</v>
       </c>
-      <c r="D49" s="241"/>
-      <c r="E49" s="241"/>
-      <c r="F49" s="241"/>
-      <c r="G49" s="241"/>
-      <c r="H49" s="241"/>
+      <c r="D49" s="232"/>
+      <c r="E49" s="232"/>
+      <c r="F49" s="232"/>
+      <c r="G49" s="232"/>
+      <c r="H49" s="232"/>
       <c r="I49" s="177"/>
       <c r="J49" s="177"/>
       <c r="K49" s="177"/>
@@ -8802,7 +8802,7 @@
       <c r="N49" s="223" t="s">
         <v>760</v>
       </c>
-      <c r="O49" s="254">
+      <c r="O49" s="245">
         <v>1</v>
       </c>
       <c r="P49" s="214" t="s">
@@ -8843,10 +8843,10 @@
       <c r="AQ49" s="115"/>
     </row>
     <row r="50" spans="1:43" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="235" t="s">
+      <c r="A50" s="226" t="s">
         <v>756</v>
       </c>
-      <c r="B50" s="242"/>
+      <c r="B50" s="233"/>
       <c r="C50" s="203"/>
       <c r="D50" s="204"/>
       <c r="E50" s="204"/>
@@ -8877,10 +8877,10 @@
       <c r="X50" s="143"/>
       <c r="Y50" s="143"/>
       <c r="Z50" s="115"/>
-      <c r="AA50" s="248" t="s">
+      <c r="AA50" s="239" t="s">
         <v>764</v>
       </c>
-      <c r="AB50" s="261">
+      <c r="AB50" s="252">
         <v>9</v>
       </c>
       <c r="AC50" s="215" t="s">
@@ -8912,13 +8912,13 @@
       <c r="K51" s="171"/>
       <c r="L51" s="171"/>
       <c r="M51" s="171"/>
-      <c r="N51" s="238" t="s">
+      <c r="N51" s="229" t="s">
         <v>756</v>
       </c>
       <c r="O51" s="208">
         <v>10</v>
       </c>
-      <c r="P51" s="239" t="s">
+      <c r="P51" s="230" t="s">
         <v>769</v>
       </c>
       <c r="Q51" s="143"/>
@@ -9126,50 +9126,50 @@
       <c r="AQ55" s="115"/>
     </row>
     <row r="56" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A56" s="233">
+      <c r="A56" s="270">
         <f>SUM(B48:B50,O48:O52,AB48:AB50)</f>
         <v>719</v>
       </c>
-      <c r="B56" s="233"/>
-      <c r="C56" s="233"/>
-      <c r="D56" s="233"/>
-      <c r="E56" s="233"/>
-      <c r="F56" s="233"/>
-      <c r="G56" s="233"/>
-      <c r="H56" s="233"/>
-      <c r="I56" s="233"/>
-      <c r="J56" s="233"/>
-      <c r="K56" s="233"/>
-      <c r="L56" s="233"/>
-      <c r="M56" s="233"/>
-      <c r="N56" s="233"/>
-      <c r="O56" s="234"/>
-      <c r="P56" s="233"/>
-      <c r="Q56" s="233"/>
-      <c r="R56" s="233"/>
-      <c r="S56" s="233"/>
-      <c r="T56" s="233"/>
-      <c r="U56" s="233"/>
-      <c r="V56" s="233"/>
-      <c r="W56" s="233"/>
-      <c r="X56" s="233"/>
-      <c r="Y56" s="233"/>
-      <c r="Z56" s="233"/>
-      <c r="AA56" s="233"/>
-      <c r="AB56" s="234"/>
-      <c r="AC56" s="233"/>
-      <c r="AD56" s="233"/>
-      <c r="AE56" s="233"/>
-      <c r="AF56" s="233"/>
-      <c r="AG56" s="233"/>
-      <c r="AH56" s="233"/>
-      <c r="AI56" s="233"/>
-      <c r="AJ56" s="233"/>
-      <c r="AK56" s="233"/>
+      <c r="B56" s="270"/>
+      <c r="C56" s="270"/>
+      <c r="D56" s="270"/>
+      <c r="E56" s="270"/>
+      <c r="F56" s="270"/>
+      <c r="G56" s="270"/>
+      <c r="H56" s="270"/>
+      <c r="I56" s="270"/>
+      <c r="J56" s="270"/>
+      <c r="K56" s="270"/>
+      <c r="L56" s="270"/>
+      <c r="M56" s="270"/>
+      <c r="N56" s="270"/>
+      <c r="O56" s="271"/>
+      <c r="P56" s="270"/>
+      <c r="Q56" s="270"/>
+      <c r="R56" s="270"/>
+      <c r="S56" s="270"/>
+      <c r="T56" s="270"/>
+      <c r="U56" s="270"/>
+      <c r="V56" s="270"/>
+      <c r="W56" s="270"/>
+      <c r="X56" s="270"/>
+      <c r="Y56" s="270"/>
+      <c r="Z56" s="270"/>
+      <c r="AA56" s="270"/>
+      <c r="AB56" s="271"/>
+      <c r="AC56" s="270"/>
+      <c r="AD56" s="270"/>
+      <c r="AE56" s="270"/>
+      <c r="AF56" s="270"/>
+      <c r="AG56" s="270"/>
+      <c r="AH56" s="270"/>
+      <c r="AI56" s="270"/>
+      <c r="AJ56" s="270"/>
+      <c r="AK56" s="270"/>
     </row>
     <row r="58" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H58" s="232"/>
-      <c r="I58" s="232"/>
+      <c r="H58" s="269"/>
+      <c r="I58" s="269"/>
     </row>
     <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AA60" s="13"/>
@@ -9187,8 +9187,8 @@
       <c r="AJ66" s="131"/>
     </row>
     <row r="67" spans="13:36" x14ac:dyDescent="0.2">
-      <c r="AI67" s="226"/>
-      <c r="AJ67" s="226"/>
+      <c r="AI67" s="263"/>
+      <c r="AJ67" s="263"/>
     </row>
     <row r="68" spans="13:36" x14ac:dyDescent="0.2">
       <c r="AI68" s="113"/>

</xml_diff>

<commit_message>
Commit 4 Penyusunan Denah Wisuda USK 163
Hasil Penyusunan Denah Wisuda USK Periode 163 Hari ke 3, Jum'at 22 November 2024 ( Mengatur Selingan dan Fullkan Nomor )
</commit_message>
<xml_diff>
--- a/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
+++ b/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data Hary\Denah Wisuda 163\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696890F-3D2C-4647-A066-5D317553E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D5F43F-299A-407C-A7F2-25773C6D4079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3073,17 +3073,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -3110,6 +3099,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -3516,9 +3518,6 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3540,7 +3539,7 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3591,13 +3590,10 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3677,9 +3673,6 @@
     <xf numFmtId="0" fontId="11" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3689,34 +3682,7 @@
     <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3756,6 +3722,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4113,7 +4115,7 @@
   <dimension ref="A1:AT81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A37" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="AQ29" sqref="AQ29"/>
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4129,49 +4131,49 @@
     <row r="1" spans="1:46" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="256" t="s">
+      <c r="C1" s="270" t="s">
         <v>762</v>
       </c>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
-      <c r="N1" s="257"/>
-      <c r="O1" s="257"/>
-      <c r="P1" s="257"/>
-      <c r="Q1" s="257"/>
-      <c r="R1" s="257"/>
-      <c r="S1" s="257"/>
-      <c r="T1" s="257"/>
-      <c r="U1" s="257"/>
-      <c r="V1" s="257"/>
-      <c r="W1" s="257"/>
-      <c r="X1" s="257"/>
-      <c r="Y1" s="257"/>
-      <c r="Z1" s="257"/>
-      <c r="AA1" s="257"/>
-      <c r="AB1" s="257"/>
-      <c r="AC1" s="257"/>
-      <c r="AD1" s="257"/>
-      <c r="AE1" s="257"/>
-      <c r="AF1" s="257"/>
-      <c r="AG1" s="257"/>
-      <c r="AH1" s="257"/>
-      <c r="AI1" s="257"/>
-      <c r="AJ1" s="257"/>
-      <c r="AK1" s="257"/>
-      <c r="AL1" s="257"/>
-      <c r="AM1" s="257"/>
-      <c r="AN1" s="257"/>
-      <c r="AO1" s="257"/>
-      <c r="AP1" s="257"/>
-      <c r="AQ1" s="258"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
+      <c r="Y1" s="271"/>
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="271"/>
+      <c r="AC1" s="271"/>
+      <c r="AD1" s="271"/>
+      <c r="AE1" s="271"/>
+      <c r="AF1" s="271"/>
+      <c r="AG1" s="271"/>
+      <c r="AH1" s="271"/>
+      <c r="AI1" s="271"/>
+      <c r="AJ1" s="271"/>
+      <c r="AK1" s="271"/>
+      <c r="AL1" s="271"/>
+      <c r="AM1" s="271"/>
+      <c r="AN1" s="271"/>
+      <c r="AO1" s="271"/>
+      <c r="AP1" s="271"/>
+      <c r="AQ1" s="272"/>
       <c r="AR1" s="33"/>
       <c r="AS1" s="178"/>
     </row>
@@ -4180,45 +4182,45 @@
       <c r="B2" s="33"/>
       <c r="C2" s="128"/>
       <c r="D2" s="129"/>
-      <c r="E2" s="259" t="s">
+      <c r="E2" s="273" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="259"/>
-      <c r="G2" s="259"/>
-      <c r="H2" s="259"/>
-      <c r="I2" s="259"/>
-      <c r="J2" s="259"/>
-      <c r="K2" s="259"/>
-      <c r="L2" s="259"/>
-      <c r="M2" s="259"/>
-      <c r="N2" s="259"/>
-      <c r="O2" s="259"/>
-      <c r="P2" s="259"/>
-      <c r="Q2" s="259"/>
-      <c r="R2" s="259"/>
-      <c r="S2" s="259"/>
-      <c r="T2" s="259"/>
-      <c r="U2" s="259"/>
-      <c r="V2" s="259"/>
-      <c r="W2" s="259"/>
-      <c r="X2" s="259"/>
-      <c r="Y2" s="259"/>
-      <c r="Z2" s="259"/>
-      <c r="AA2" s="259"/>
-      <c r="AB2" s="259"/>
-      <c r="AC2" s="259"/>
-      <c r="AD2" s="259"/>
-      <c r="AE2" s="259"/>
-      <c r="AF2" s="259"/>
-      <c r="AG2" s="259"/>
-      <c r="AH2" s="259"/>
-      <c r="AI2" s="259"/>
-      <c r="AJ2" s="259"/>
-      <c r="AK2" s="259"/>
-      <c r="AL2" s="259"/>
-      <c r="AM2" s="259"/>
-      <c r="AN2" s="259"/>
-      <c r="AO2" s="259"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="273"/>
+      <c r="I2" s="273"/>
+      <c r="J2" s="273"/>
+      <c r="K2" s="273"/>
+      <c r="L2" s="273"/>
+      <c r="M2" s="273"/>
+      <c r="N2" s="273"/>
+      <c r="O2" s="273"/>
+      <c r="P2" s="273"/>
+      <c r="Q2" s="273"/>
+      <c r="R2" s="273"/>
+      <c r="S2" s="273"/>
+      <c r="T2" s="273"/>
+      <c r="U2" s="273"/>
+      <c r="V2" s="273"/>
+      <c r="W2" s="273"/>
+      <c r="X2" s="273"/>
+      <c r="Y2" s="273"/>
+      <c r="Z2" s="273"/>
+      <c r="AA2" s="273"/>
+      <c r="AB2" s="273"/>
+      <c r="AC2" s="273"/>
+      <c r="AD2" s="273"/>
+      <c r="AE2" s="273"/>
+      <c r="AF2" s="273"/>
+      <c r="AG2" s="273"/>
+      <c r="AH2" s="273"/>
+      <c r="AI2" s="273"/>
+      <c r="AJ2" s="273"/>
+      <c r="AK2" s="273"/>
+      <c r="AL2" s="273"/>
+      <c r="AM2" s="273"/>
+      <c r="AN2" s="273"/>
+      <c r="AO2" s="273"/>
       <c r="AP2" s="129"/>
       <c r="AQ2" s="130"/>
       <c r="AR2" s="33"/>
@@ -4504,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="123"/>
-      <c r="C7" s="238" t="s">
+      <c r="C7" s="236" t="s">
         <v>771</v>
       </c>
       <c r="D7" s="190" t="s">
@@ -4534,13 +4536,13 @@
       <c r="L7" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="198" t="s">
+      <c r="M7" s="197" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="190" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="198" t="s">
+      <c r="O7" s="197" t="s">
         <v>21</v>
       </c>
       <c r="P7" s="190" t="s">
@@ -4886,10 +4888,12 @@
       <c r="AP9" s="190" t="s">
         <v>60</v>
       </c>
-      <c r="AQ9" s="190" t="s">
+      <c r="AQ9" s="278" t="s">
         <v>59</v>
       </c>
-      <c r="AR9" s="123"/>
+      <c r="AR9" s="279" t="s">
+        <v>761</v>
+      </c>
       <c r="AS9" s="51">
         <v>3</v>
       </c>
@@ -4900,10 +4904,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="147"/>
-      <c r="C10" s="239" t="s">
+      <c r="C10" s="237" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="240" t="s">
+      <c r="D10" s="238" t="s">
         <v>772</v>
       </c>
       <c r="E10" s="191" t="s">
@@ -4921,59 +4925,59 @@
       <c r="I10" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="242" t="s">
+      <c r="J10" s="240" t="s">
         <v>773</v>
       </c>
-      <c r="K10" s="241" t="s">
+      <c r="K10" s="239" t="s">
         <v>774</v>
       </c>
-      <c r="L10" s="199" t="s">
+      <c r="L10" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="199" t="s">
+      <c r="M10" s="198" t="s">
         <v>95</v>
       </c>
-      <c r="N10" s="199" t="s">
+      <c r="N10" s="198" t="s">
         <v>96</v>
       </c>
-      <c r="O10" s="199" t="s">
+      <c r="O10" s="198" t="s">
         <v>97</v>
       </c>
-      <c r="P10" s="199" t="s">
+      <c r="P10" s="198" t="s">
         <v>98</v>
       </c>
-      <c r="Q10" s="245" t="s">
+      <c r="Q10" s="243" t="s">
         <v>775</v>
       </c>
-      <c r="R10" s="244" t="s">
+      <c r="R10" s="242" t="s">
         <v>100</v>
       </c>
-      <c r="S10" s="244" t="s">
+      <c r="S10" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="244" t="s">
+      <c r="T10" s="242" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="244" t="s">
+      <c r="U10" s="242" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="244" t="s">
+      <c r="V10" s="242" t="s">
         <v>58</v>
       </c>
       <c r="W10" s="137"/>
-      <c r="X10" s="244" t="s">
+      <c r="X10" s="242" t="s">
         <v>58</v>
       </c>
-      <c r="Y10" s="244" t="s">
+      <c r="Y10" s="242" t="s">
         <v>57</v>
       </c>
-      <c r="Z10" s="244" t="s">
+      <c r="Z10" s="242" t="s">
         <v>56</v>
       </c>
-      <c r="AA10" s="244" t="s">
+      <c r="AA10" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="AB10" s="246" t="s">
+      <c r="AB10" s="244" t="s">
         <v>145</v>
       </c>
       <c r="AC10" s="192" t="s">
@@ -5155,7 +5159,7 @@
       <c r="AQ11" s="192" t="s">
         <v>108</v>
       </c>
-      <c r="AR11" s="196" t="s">
+      <c r="AR11" s="195" t="s">
         <v>537</v>
       </c>
       <c r="AS11" s="51">
@@ -5167,7 +5171,7 @@
       <c r="A12" s="133">
         <v>6</v>
       </c>
-      <c r="B12" s="252"/>
+      <c r="B12" s="249"/>
       <c r="C12" s="192">
         <v>120</v>
       </c>
@@ -5431,9 +5435,7 @@
       <c r="A14" s="133">
         <v>8</v>
       </c>
-      <c r="B14" s="220" t="s">
-        <v>761</v>
-      </c>
+      <c r="B14" s="119"/>
       <c r="C14" s="192">
         <v>160</v>
       </c>
@@ -6080,10 +6082,12 @@
       <c r="AP18" s="192" t="s">
         <v>269</v>
       </c>
-      <c r="AQ18" s="192" t="s">
+      <c r="AQ18" s="280" t="s">
         <v>268</v>
       </c>
-      <c r="AR18" s="119"/>
+      <c r="AR18" s="279" t="s">
+        <v>779</v>
+      </c>
       <c r="AS18" s="51">
         <v>12</v>
       </c>
@@ -6227,7 +6231,7 @@
       <c r="A20" s="133">
         <v>14</v>
       </c>
-      <c r="B20" s="197"/>
+      <c r="B20" s="196"/>
       <c r="C20" s="192">
         <v>280</v>
       </c>
@@ -6349,7 +6353,7 @@
       <c r="AQ20" s="192">
         <v>280</v>
       </c>
-      <c r="AR20" s="196" t="s">
+      <c r="AR20" s="195" t="s">
         <v>460</v>
       </c>
       <c r="AS20" s="51">
@@ -6419,11 +6423,11 @@
       <c r="U21" s="192">
         <v>282</v>
       </c>
-      <c r="V21" s="193">
+      <c r="V21" s="192">
         <v>281</v>
       </c>
       <c r="W21" s="118"/>
-      <c r="X21" s="193">
+      <c r="X21" s="192">
         <v>281</v>
       </c>
       <c r="Y21" s="192">
@@ -6503,11 +6507,11 @@
       <c r="K22" s="113"/>
       <c r="L22" s="113"/>
       <c r="M22" s="113"/>
-      <c r="N22" s="260" t="s">
+      <c r="N22" s="274" t="s">
         <v>575</v>
       </c>
-      <c r="O22" s="260"/>
-      <c r="P22" s="260"/>
+      <c r="O22" s="274"/>
+      <c r="P22" s="274"/>
       <c r="Q22" s="113"/>
       <c r="R22" s="113"/>
       <c r="S22" s="113"/>
@@ -6521,11 +6525,11 @@
       <c r="AA22" s="113"/>
       <c r="AB22" s="113"/>
       <c r="AC22" s="113"/>
-      <c r="AD22" s="260" t="s">
+      <c r="AD22" s="274" t="s">
         <v>575</v>
       </c>
-      <c r="AE22" s="260"/>
-      <c r="AF22" s="260"/>
+      <c r="AE22" s="274"/>
+      <c r="AF22" s="274"/>
       <c r="AG22" s="113"/>
       <c r="AH22" s="113"/>
       <c r="AI22" s="113"/>
@@ -6541,19 +6545,19 @@
       <c r="AS22" s="178"/>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A23" s="223"/>
-      <c r="B23" s="265"/>
-      <c r="C23" s="265"/>
-      <c r="D23" s="265"/>
-      <c r="E23" s="265"/>
-      <c r="F23" s="265"/>
-      <c r="G23" s="265"/>
-      <c r="H23" s="265"/>
-      <c r="I23" s="265"/>
-      <c r="J23" s="265"/>
-      <c r="K23" s="265"/>
-      <c r="L23" s="266"/>
-      <c r="M23" s="266"/>
+      <c r="A23" s="221"/>
+      <c r="B23" s="253"/>
+      <c r="C23" s="253"/>
+      <c r="D23" s="253"/>
+      <c r="E23" s="253"/>
+      <c r="F23" s="253"/>
+      <c r="G23" s="253"/>
+      <c r="H23" s="253"/>
+      <c r="I23" s="253"/>
+      <c r="J23" s="253"/>
+      <c r="K23" s="253"/>
+      <c r="L23" s="254"/>
+      <c r="M23" s="254"/>
       <c r="N23" s="154">
         <v>1</v>
       </c>
@@ -6597,34 +6601,34 @@
       <c r="AF23" s="156">
         <v>1</v>
       </c>
-      <c r="AG23" s="266"/>
-      <c r="AH23" s="266"/>
-      <c r="AI23" s="267"/>
-      <c r="AJ23" s="267"/>
-      <c r="AK23" s="267"/>
-      <c r="AL23" s="267"/>
-      <c r="AM23" s="267"/>
-      <c r="AN23" s="267"/>
-      <c r="AO23" s="267"/>
-      <c r="AP23" s="267"/>
-      <c r="AQ23" s="267"/>
-      <c r="AR23" s="267"/>
+      <c r="AG23" s="254"/>
+      <c r="AH23" s="254"/>
+      <c r="AI23" s="255"/>
+      <c r="AJ23" s="255"/>
+      <c r="AK23" s="255"/>
+      <c r="AL23" s="255"/>
+      <c r="AM23" s="255"/>
+      <c r="AN23" s="255"/>
+      <c r="AO23" s="255"/>
+      <c r="AP23" s="255"/>
+      <c r="AQ23" s="255"/>
+      <c r="AR23" s="255"/>
       <c r="AS23" s="178"/>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="123"/>
-      <c r="B24" s="267"/>
-      <c r="C24" s="267"/>
-      <c r="D24" s="267"/>
-      <c r="E24" s="267"/>
-      <c r="F24" s="267"/>
-      <c r="G24" s="267"/>
-      <c r="H24" s="267"/>
-      <c r="I24" s="267"/>
-      <c r="J24" s="267"/>
-      <c r="K24" s="267"/>
-      <c r="L24" s="266"/>
-      <c r="M24" s="266"/>
+      <c r="B24" s="255"/>
+      <c r="C24" s="255"/>
+      <c r="D24" s="255"/>
+      <c r="E24" s="255"/>
+      <c r="F24" s="255"/>
+      <c r="G24" s="255"/>
+      <c r="H24" s="255"/>
+      <c r="I24" s="255"/>
+      <c r="J24" s="255"/>
+      <c r="K24" s="255"/>
+      <c r="L24" s="254"/>
+      <c r="M24" s="254"/>
       <c r="N24" s="154">
         <v>2</v>
       </c>
@@ -6648,34 +6652,34 @@
       <c r="AF24" s="156">
         <v>2</v>
       </c>
-      <c r="AG24" s="266"/>
-      <c r="AH24" s="266"/>
-      <c r="AI24" s="267"/>
-      <c r="AJ24" s="267"/>
-      <c r="AK24" s="267"/>
-      <c r="AL24" s="267"/>
-      <c r="AM24" s="267"/>
-      <c r="AN24" s="267"/>
-      <c r="AO24" s="267"/>
-      <c r="AP24" s="267"/>
-      <c r="AQ24" s="267"/>
-      <c r="AR24" s="267"/>
+      <c r="AG24" s="254"/>
+      <c r="AH24" s="254"/>
+      <c r="AI24" s="255"/>
+      <c r="AJ24" s="255"/>
+      <c r="AK24" s="255"/>
+      <c r="AL24" s="255"/>
+      <c r="AM24" s="255"/>
+      <c r="AN24" s="255"/>
+      <c r="AO24" s="255"/>
+      <c r="AP24" s="255"/>
+      <c r="AQ24" s="255"/>
+      <c r="AR24" s="255"/>
       <c r="AS24" s="178"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="124"/>
-      <c r="B25" s="267"/>
-      <c r="C25" s="267"/>
-      <c r="D25" s="267"/>
-      <c r="E25" s="267"/>
-      <c r="F25" s="267"/>
-      <c r="G25" s="267"/>
-      <c r="H25" s="267"/>
-      <c r="I25" s="267"/>
-      <c r="J25" s="267"/>
-      <c r="K25" s="267"/>
-      <c r="L25" s="266"/>
-      <c r="M25" s="266"/>
+      <c r="B25" s="255"/>
+      <c r="C25" s="255"/>
+      <c r="D25" s="255"/>
+      <c r="E25" s="255"/>
+      <c r="F25" s="255"/>
+      <c r="G25" s="255"/>
+      <c r="H25" s="255"/>
+      <c r="I25" s="255"/>
+      <c r="J25" s="255"/>
+      <c r="K25" s="255"/>
+      <c r="L25" s="254"/>
+      <c r="M25" s="254"/>
       <c r="N25" s="154">
         <v>3</v>
       </c>
@@ -6699,34 +6703,34 @@
       <c r="AF25" s="156">
         <v>3</v>
       </c>
-      <c r="AG25" s="266"/>
-      <c r="AH25" s="266"/>
-      <c r="AI25" s="267"/>
-      <c r="AJ25" s="267"/>
-      <c r="AK25" s="267"/>
-      <c r="AL25" s="267"/>
-      <c r="AM25" s="267"/>
-      <c r="AN25" s="267"/>
-      <c r="AO25" s="267"/>
-      <c r="AP25" s="267"/>
-      <c r="AQ25" s="267"/>
-      <c r="AR25" s="267"/>
+      <c r="AG25" s="254"/>
+      <c r="AH25" s="254"/>
+      <c r="AI25" s="255"/>
+      <c r="AJ25" s="255"/>
+      <c r="AK25" s="255"/>
+      <c r="AL25" s="255"/>
+      <c r="AM25" s="255"/>
+      <c r="AN25" s="255"/>
+      <c r="AO25" s="255"/>
+      <c r="AP25" s="255"/>
+      <c r="AQ25" s="255"/>
+      <c r="AR25" s="255"/>
       <c r="AS25" s="178"/>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="123"/>
-      <c r="B26" s="268"/>
-      <c r="C26" s="268"/>
-      <c r="D26" s="268"/>
-      <c r="E26" s="268"/>
-      <c r="F26" s="268"/>
-      <c r="G26" s="268"/>
-      <c r="H26" s="268"/>
-      <c r="I26" s="268"/>
-      <c r="J26" s="268"/>
-      <c r="K26" s="268"/>
-      <c r="L26" s="268"/>
-      <c r="M26" s="268"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="256"/>
+      <c r="D26" s="256"/>
+      <c r="E26" s="256"/>
+      <c r="F26" s="256"/>
+      <c r="G26" s="256"/>
+      <c r="H26" s="256"/>
+      <c r="I26" s="256"/>
+      <c r="J26" s="256"/>
+      <c r="K26" s="256"/>
+      <c r="L26" s="256"/>
+      <c r="M26" s="256"/>
       <c r="N26" s="154">
         <v>4</v>
       </c>
@@ -6778,34 +6782,34 @@
       <c r="AF26" s="156">
         <v>4</v>
       </c>
-      <c r="AG26" s="267"/>
-      <c r="AH26" s="279"/>
-      <c r="AI26" s="267"/>
-      <c r="AJ26" s="279"/>
-      <c r="AK26" s="267"/>
-      <c r="AL26" s="279"/>
-      <c r="AM26" s="267"/>
-      <c r="AN26" s="279"/>
-      <c r="AO26" s="267"/>
-      <c r="AP26" s="279"/>
-      <c r="AQ26" s="267"/>
-      <c r="AR26" s="279"/>
+      <c r="AG26" s="255"/>
+      <c r="AH26" s="267"/>
+      <c r="AI26" s="255"/>
+      <c r="AJ26" s="267"/>
+      <c r="AK26" s="255"/>
+      <c r="AL26" s="267"/>
+      <c r="AM26" s="255"/>
+      <c r="AN26" s="267"/>
+      <c r="AO26" s="255"/>
+      <c r="AP26" s="267"/>
+      <c r="AQ26" s="255"/>
+      <c r="AR26" s="267"/>
       <c r="AS26" s="178"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="115"/>
-      <c r="B27" s="268"/>
-      <c r="C27" s="268"/>
-      <c r="D27" s="268"/>
-      <c r="E27" s="268"/>
-      <c r="F27" s="268"/>
-      <c r="G27" s="268"/>
-      <c r="H27" s="268"/>
-      <c r="I27" s="268"/>
-      <c r="J27" s="268"/>
-      <c r="K27" s="268"/>
-      <c r="L27" s="268"/>
-      <c r="M27" s="268"/>
+      <c r="B27" s="256"/>
+      <c r="C27" s="256"/>
+      <c r="D27" s="256"/>
+      <c r="E27" s="256"/>
+      <c r="F27" s="256"/>
+      <c r="G27" s="256"/>
+      <c r="H27" s="256"/>
+      <c r="I27" s="256"/>
+      <c r="J27" s="256"/>
+      <c r="K27" s="256"/>
+      <c r="L27" s="256"/>
+      <c r="M27" s="256"/>
       <c r="N27" s="154">
         <v>5</v>
       </c>
@@ -6857,34 +6861,34 @@
       <c r="AF27" s="156">
         <v>5</v>
       </c>
-      <c r="AG27" s="267"/>
-      <c r="AH27" s="279"/>
-      <c r="AI27" s="267"/>
-      <c r="AJ27" s="267"/>
-      <c r="AK27" s="267"/>
-      <c r="AL27" s="267"/>
-      <c r="AM27" s="267"/>
-      <c r="AN27" s="267"/>
-      <c r="AO27" s="280"/>
-      <c r="AP27" s="267"/>
-      <c r="AQ27" s="267"/>
-      <c r="AR27" s="267"/>
+      <c r="AG27" s="255"/>
+      <c r="AH27" s="267"/>
+      <c r="AI27" s="255"/>
+      <c r="AJ27" s="255"/>
+      <c r="AK27" s="255"/>
+      <c r="AL27" s="255"/>
+      <c r="AM27" s="255"/>
+      <c r="AN27" s="255"/>
+      <c r="AO27" s="268"/>
+      <c r="AP27" s="255"/>
+      <c r="AQ27" s="255"/>
+      <c r="AR27" s="255"/>
       <c r="AS27" s="178"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="119"/>
-      <c r="B28" s="268"/>
-      <c r="C28" s="268"/>
-      <c r="D28" s="268"/>
-      <c r="E28" s="268"/>
-      <c r="F28" s="268"/>
-      <c r="G28" s="268"/>
-      <c r="H28" s="268"/>
-      <c r="I28" s="268"/>
-      <c r="J28" s="268"/>
-      <c r="K28" s="268"/>
-      <c r="L28" s="268"/>
-      <c r="M28" s="268"/>
+      <c r="B28" s="256"/>
+      <c r="C28" s="256"/>
+      <c r="D28" s="256"/>
+      <c r="E28" s="256"/>
+      <c r="F28" s="256"/>
+      <c r="G28" s="256"/>
+      <c r="H28" s="256"/>
+      <c r="I28" s="256"/>
+      <c r="J28" s="256"/>
+      <c r="K28" s="256"/>
+      <c r="L28" s="256"/>
+      <c r="M28" s="256"/>
       <c r="N28" s="154">
         <v>6</v>
       </c>
@@ -6936,626 +6940,620 @@
       <c r="AF28" s="156">
         <v>6</v>
       </c>
-      <c r="AG28" s="267"/>
-      <c r="AH28" s="279"/>
-      <c r="AI28" s="267"/>
-      <c r="AJ28" s="267"/>
-      <c r="AK28" s="267"/>
-      <c r="AL28" s="267"/>
-      <c r="AM28" s="267"/>
-      <c r="AN28" s="267"/>
-      <c r="AO28" s="267"/>
-      <c r="AP28" s="267"/>
-      <c r="AQ28" s="267"/>
-      <c r="AR28" s="267"/>
+      <c r="AG28" s="255"/>
+      <c r="AH28" s="267"/>
+      <c r="AI28" s="255"/>
+      <c r="AJ28" s="255"/>
+      <c r="AK28" s="255"/>
+      <c r="AL28" s="255"/>
+      <c r="AM28" s="255"/>
+      <c r="AN28" s="255"/>
+      <c r="AO28" s="255"/>
+      <c r="AP28" s="255"/>
+      <c r="AQ28" s="255"/>
+      <c r="AR28" s="255"/>
       <c r="AS28" s="179"/>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="127"/>
-      <c r="B29" s="269"/>
-      <c r="C29" s="269"/>
-      <c r="D29" s="269"/>
-      <c r="E29" s="269"/>
-      <c r="F29" s="269"/>
-      <c r="G29" s="269"/>
-      <c r="H29" s="269"/>
-      <c r="I29" s="269"/>
-      <c r="J29" s="269"/>
-      <c r="K29" s="269"/>
-      <c r="L29" s="269"/>
-      <c r="M29" s="269"/>
+      <c r="B29" s="257"/>
+      <c r="C29" s="257"/>
+      <c r="D29" s="257"/>
+      <c r="E29" s="257"/>
+      <c r="F29" s="257"/>
+      <c r="G29" s="257"/>
+      <c r="H29" s="257"/>
+      <c r="I29" s="257"/>
+      <c r="J29" s="257"/>
+      <c r="K29" s="257"/>
+      <c r="L29" s="257"/>
+      <c r="M29" s="257"/>
       <c r="N29" s="154">
         <v>7</v>
       </c>
-      <c r="O29" s="220" t="s">
-        <v>779</v>
-      </c>
+      <c r="O29" s="113"/>
       <c r="P29" s="192">
         <v>328</v>
       </c>
       <c r="Q29" s="192">
         <v>327</v>
       </c>
-      <c r="R29" s="192">
+      <c r="R29" s="237">
         <v>326</v>
       </c>
-      <c r="S29" s="192">
+      <c r="S29" s="245" t="s">
+        <v>778</v>
+      </c>
+      <c r="T29" s="250" t="s">
+        <v>364</v>
+      </c>
+      <c r="U29" s="193">
+        <v>323</v>
+      </c>
+      <c r="V29" s="193">
+        <v>322</v>
+      </c>
+      <c r="W29" s="153"/>
+      <c r="X29" s="193">
+        <v>322</v>
+      </c>
+      <c r="Y29" s="193">
+        <v>323</v>
+      </c>
+      <c r="Z29" s="193">
+        <v>324</v>
+      </c>
+      <c r="AA29" s="193">
         <v>325</v>
       </c>
-      <c r="T29" s="250">
+      <c r="AB29" s="193">
         <v>326</v>
       </c>
-      <c r="U29" s="247" t="s">
-        <v>778</v>
-      </c>
-      <c r="V29" s="253" t="s">
-        <v>364</v>
-      </c>
-      <c r="W29" s="153"/>
-      <c r="X29" s="194">
-        <v>322</v>
-      </c>
-      <c r="Y29" s="194">
-        <v>323</v>
-      </c>
-      <c r="Z29" s="194">
-        <v>324</v>
-      </c>
-      <c r="AA29" s="194">
-        <v>325</v>
-      </c>
-      <c r="AB29" s="194">
-        <v>326</v>
-      </c>
-      <c r="AC29" s="194">
+      <c r="AC29" s="193">
         <v>327</v>
       </c>
-      <c r="AD29" s="194">
+      <c r="AD29" s="193">
         <v>328</v>
       </c>
       <c r="AE29" s="113"/>
       <c r="AF29" s="156">
         <v>7</v>
       </c>
-      <c r="AG29" s="276"/>
-      <c r="AH29" s="275"/>
-      <c r="AI29" s="276"/>
-      <c r="AJ29" s="275"/>
-      <c r="AK29" s="276"/>
-      <c r="AL29" s="275"/>
-      <c r="AM29" s="276"/>
-      <c r="AN29" s="275"/>
-      <c r="AO29" s="276"/>
-      <c r="AP29" s="275"/>
-      <c r="AQ29" s="276"/>
-      <c r="AR29" s="275"/>
+      <c r="AG29" s="264"/>
+      <c r="AH29" s="263"/>
+      <c r="AI29" s="264"/>
+      <c r="AJ29" s="263"/>
+      <c r="AK29" s="264"/>
+      <c r="AL29" s="263"/>
+      <c r="AM29" s="264"/>
+      <c r="AN29" s="263"/>
+      <c r="AO29" s="264"/>
+      <c r="AP29" s="263"/>
+      <c r="AQ29" s="264"/>
+      <c r="AR29" s="263"/>
       <c r="AS29" s="178"/>
     </row>
     <row r="30" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="115"/>
-      <c r="B30" s="267"/>
-      <c r="C30" s="267"/>
-      <c r="D30" s="267"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="267"/>
-      <c r="G30" s="267"/>
-      <c r="H30" s="267"/>
-      <c r="I30" s="267"/>
-      <c r="J30" s="267"/>
-      <c r="K30" s="267"/>
-      <c r="L30" s="267"/>
-      <c r="M30" s="267"/>
+      <c r="B30" s="255"/>
+      <c r="C30" s="255"/>
+      <c r="D30" s="255"/>
+      <c r="E30" s="255"/>
+      <c r="F30" s="255"/>
+      <c r="G30" s="255"/>
+      <c r="H30" s="255"/>
+      <c r="I30" s="255"/>
+      <c r="J30" s="255"/>
+      <c r="K30" s="255"/>
+      <c r="L30" s="255"/>
+      <c r="M30" s="255"/>
       <c r="N30" s="113">
         <v>8</v>
       </c>
-      <c r="O30" s="251"/>
-      <c r="P30" s="254">
+      <c r="O30" s="248"/>
+      <c r="P30" s="251">
         <v>335</v>
       </c>
-      <c r="Q30" s="194">
+      <c r="Q30" s="193">
         <v>334</v>
       </c>
-      <c r="R30" s="194">
+      <c r="R30" s="193">
         <v>333</v>
       </c>
-      <c r="S30" s="194">
+      <c r="S30" s="193">
         <v>332</v>
       </c>
-      <c r="T30" s="194">
+      <c r="T30" s="193">
         <v>331</v>
       </c>
-      <c r="U30" s="194">
+      <c r="U30" s="193">
         <v>330</v>
       </c>
-      <c r="V30" s="194">
+      <c r="V30" s="193">
         <v>329</v>
       </c>
       <c r="W30" s="162"/>
-      <c r="X30" s="194">
+      <c r="X30" s="193">
         <v>329</v>
       </c>
-      <c r="Y30" s="194">
+      <c r="Y30" s="193">
         <v>330</v>
       </c>
-      <c r="Z30" s="194">
+      <c r="Z30" s="193">
         <v>331</v>
       </c>
-      <c r="AA30" s="194">
+      <c r="AA30" s="193">
         <v>332</v>
       </c>
-      <c r="AB30" s="194">
+      <c r="AB30" s="193">
         <v>333</v>
       </c>
-      <c r="AC30" s="194">
+      <c r="AC30" s="193">
         <v>334</v>
       </c>
-      <c r="AD30" s="194">
+      <c r="AD30" s="193">
         <v>335</v>
       </c>
       <c r="AE30" s="113"/>
       <c r="AF30" s="159">
         <v>8</v>
       </c>
-      <c r="AG30" s="267"/>
-      <c r="AH30" s="279"/>
-      <c r="AI30" s="267"/>
-      <c r="AJ30" s="267"/>
-      <c r="AK30" s="267"/>
-      <c r="AL30" s="267"/>
-      <c r="AM30" s="267"/>
-      <c r="AN30" s="267"/>
-      <c r="AO30" s="267"/>
-      <c r="AP30" s="267"/>
-      <c r="AQ30" s="267"/>
-      <c r="AR30" s="267"/>
+      <c r="AG30" s="255"/>
+      <c r="AH30" s="267"/>
+      <c r="AI30" s="255"/>
+      <c r="AJ30" s="255"/>
+      <c r="AK30" s="255"/>
+      <c r="AL30" s="255"/>
+      <c r="AM30" s="255"/>
+      <c r="AN30" s="255"/>
+      <c r="AO30" s="255"/>
+      <c r="AP30" s="255"/>
+      <c r="AQ30" s="255"/>
+      <c r="AR30" s="255"/>
     </row>
     <row r="31" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="115"/>
-      <c r="B31" s="267"/>
-      <c r="C31" s="267"/>
-      <c r="D31" s="267"/>
-      <c r="E31" s="267"/>
-      <c r="F31" s="267"/>
-      <c r="G31" s="267"/>
-      <c r="H31" s="267"/>
-      <c r="I31" s="267"/>
-      <c r="J31" s="267"/>
-      <c r="K31" s="267"/>
-      <c r="L31" s="267"/>
-      <c r="M31" s="267"/>
+      <c r="B31" s="255"/>
+      <c r="C31" s="255"/>
+      <c r="D31" s="255"/>
+      <c r="E31" s="255"/>
+      <c r="F31" s="255"/>
+      <c r="G31" s="255"/>
+      <c r="H31" s="255"/>
+      <c r="I31" s="255"/>
+      <c r="J31" s="255"/>
+      <c r="K31" s="255"/>
+      <c r="L31" s="255"/>
+      <c r="M31" s="255"/>
       <c r="N31" s="154">
         <v>9</v>
       </c>
       <c r="O31" s="125"/>
-      <c r="P31" s="194">
+      <c r="P31" s="193">
         <v>342</v>
       </c>
-      <c r="Q31" s="194">
+      <c r="Q31" s="193">
         <v>341</v>
       </c>
-      <c r="R31" s="194">
+      <c r="R31" s="193">
         <v>340</v>
       </c>
-      <c r="S31" s="194">
+      <c r="S31" s="193">
         <v>339</v>
       </c>
-      <c r="T31" s="194">
+      <c r="T31" s="193">
         <v>338</v>
       </c>
-      <c r="U31" s="194">
+      <c r="U31" s="193">
         <v>337</v>
       </c>
-      <c r="V31" s="194">
+      <c r="V31" s="193">
         <v>336</v>
       </c>
       <c r="W31" s="163"/>
-      <c r="X31" s="194">
+      <c r="X31" s="193">
         <v>336</v>
       </c>
-      <c r="Y31" s="194">
+      <c r="Y31" s="193">
         <v>337</v>
       </c>
-      <c r="Z31" s="194">
+      <c r="Z31" s="193">
         <v>338</v>
       </c>
-      <c r="AA31" s="194">
+      <c r="AA31" s="193">
         <v>339</v>
       </c>
-      <c r="AB31" s="194">
+      <c r="AB31" s="193">
         <v>340</v>
       </c>
-      <c r="AC31" s="194">
+      <c r="AC31" s="193">
         <v>341</v>
       </c>
-      <c r="AD31" s="194">
+      <c r="AD31" s="193">
         <v>342</v>
       </c>
       <c r="AE31" s="115"/>
       <c r="AF31" s="185">
         <v>9</v>
       </c>
-      <c r="AG31" s="267"/>
-      <c r="AH31" s="279"/>
-      <c r="AI31" s="267"/>
-      <c r="AJ31" s="267"/>
-      <c r="AK31" s="267"/>
-      <c r="AL31" s="267"/>
-      <c r="AM31" s="267"/>
-      <c r="AN31" s="267"/>
-      <c r="AO31" s="267"/>
-      <c r="AP31" s="267"/>
-      <c r="AQ31" s="267"/>
-      <c r="AR31" s="267"/>
+      <c r="AG31" s="255"/>
+      <c r="AH31" s="267"/>
+      <c r="AI31" s="255"/>
+      <c r="AJ31" s="255"/>
+      <c r="AK31" s="255"/>
+      <c r="AL31" s="255"/>
+      <c r="AM31" s="255"/>
+      <c r="AN31" s="255"/>
+      <c r="AO31" s="255"/>
+      <c r="AP31" s="255"/>
+      <c r="AQ31" s="255"/>
+      <c r="AR31" s="255"/>
     </row>
     <row r="32" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="115"/>
-      <c r="B32" s="267"/>
-      <c r="C32" s="267"/>
-      <c r="D32" s="267"/>
-      <c r="E32" s="267"/>
-      <c r="F32" s="267"/>
-      <c r="G32" s="267"/>
-      <c r="H32" s="267"/>
-      <c r="I32" s="267"/>
-      <c r="J32" s="267"/>
-      <c r="K32" s="267"/>
-      <c r="L32" s="267"/>
-      <c r="M32" s="267"/>
+      <c r="B32" s="255"/>
+      <c r="C32" s="255"/>
+      <c r="D32" s="255"/>
+      <c r="E32" s="255"/>
+      <c r="F32" s="255"/>
+      <c r="G32" s="255"/>
+      <c r="H32" s="255"/>
+      <c r="I32" s="255"/>
+      <c r="J32" s="255"/>
+      <c r="K32" s="255"/>
+      <c r="L32" s="255"/>
+      <c r="M32" s="255"/>
       <c r="N32" s="184">
         <v>10</v>
       </c>
       <c r="O32" s="115"/>
-      <c r="P32" s="194">
+      <c r="P32" s="193">
         <v>349</v>
       </c>
-      <c r="Q32" s="194">
+      <c r="Q32" s="193">
         <v>348</v>
       </c>
-      <c r="R32" s="194">
+      <c r="R32" s="193">
         <v>347</v>
       </c>
-      <c r="S32" s="194">
+      <c r="S32" s="193">
         <v>346</v>
       </c>
-      <c r="T32" s="194">
+      <c r="T32" s="193">
         <v>345</v>
       </c>
-      <c r="U32" s="194">
+      <c r="U32" s="193">
         <v>344</v>
       </c>
-      <c r="V32" s="194">
+      <c r="V32" s="193">
         <v>343</v>
       </c>
       <c r="W32" s="163"/>
-      <c r="X32" s="194">
+      <c r="X32" s="193">
         <v>343</v>
       </c>
-      <c r="Y32" s="194">
+      <c r="Y32" s="193">
         <v>344</v>
       </c>
-      <c r="Z32" s="194">
+      <c r="Z32" s="193">
         <v>345</v>
       </c>
-      <c r="AA32" s="194">
+      <c r="AA32" s="193">
         <v>346</v>
       </c>
-      <c r="AB32" s="194">
+      <c r="AB32" s="193">
         <v>347</v>
       </c>
-      <c r="AC32" s="194">
+      <c r="AC32" s="193">
         <v>348</v>
       </c>
-      <c r="AD32" s="194">
+      <c r="AD32" s="193">
         <v>349</v>
       </c>
       <c r="AE32" s="115"/>
       <c r="AF32" s="185">
         <v>10</v>
       </c>
-      <c r="AG32" s="267"/>
-      <c r="AH32" s="279"/>
-      <c r="AI32" s="267"/>
-      <c r="AJ32" s="267"/>
-      <c r="AK32" s="267"/>
-      <c r="AL32" s="267"/>
-      <c r="AM32" s="267"/>
-      <c r="AN32" s="267"/>
-      <c r="AO32" s="267"/>
-      <c r="AP32" s="267"/>
-      <c r="AQ32" s="267"/>
-      <c r="AR32" s="267"/>
+      <c r="AG32" s="255"/>
+      <c r="AH32" s="267"/>
+      <c r="AI32" s="255"/>
+      <c r="AJ32" s="255"/>
+      <c r="AK32" s="255"/>
+      <c r="AL32" s="255"/>
+      <c r="AM32" s="255"/>
+      <c r="AN32" s="255"/>
+      <c r="AO32" s="255"/>
+      <c r="AP32" s="255"/>
+      <c r="AQ32" s="255"/>
+      <c r="AR32" s="255"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
-      <c r="B33" s="267"/>
-      <c r="C33" s="267"/>
-      <c r="D33" s="267"/>
-      <c r="E33" s="267"/>
-      <c r="F33" s="267"/>
-      <c r="G33" s="267"/>
-      <c r="H33" s="267"/>
-      <c r="I33" s="267"/>
-      <c r="J33" s="267"/>
-      <c r="K33" s="267"/>
-      <c r="L33" s="267"/>
-      <c r="M33" s="267"/>
+      <c r="B33" s="255"/>
+      <c r="C33" s="255"/>
+      <c r="D33" s="255"/>
+      <c r="E33" s="255"/>
+      <c r="F33" s="255"/>
+      <c r="G33" s="255"/>
+      <c r="H33" s="255"/>
+      <c r="I33" s="255"/>
+      <c r="J33" s="255"/>
+      <c r="K33" s="255"/>
+      <c r="L33" s="255"/>
+      <c r="M33" s="255"/>
       <c r="N33" s="186">
         <v>11</v>
       </c>
       <c r="O33" s="115"/>
-      <c r="P33" s="194">
+      <c r="P33" s="193">
         <v>356</v>
       </c>
-      <c r="Q33" s="194">
+      <c r="Q33" s="193">
         <v>355</v>
       </c>
-      <c r="R33" s="194">
+      <c r="R33" s="193">
         <v>354</v>
       </c>
-      <c r="S33" s="194">
+      <c r="S33" s="193">
         <v>353</v>
       </c>
-      <c r="T33" s="194">
+      <c r="T33" s="193">
         <v>352</v>
       </c>
-      <c r="U33" s="194">
+      <c r="U33" s="193">
         <v>351</v>
       </c>
-      <c r="V33" s="194">
+      <c r="V33" s="193">
         <v>350</v>
       </c>
       <c r="W33" s="163"/>
-      <c r="X33" s="264">
+      <c r="X33" s="252">
         <v>350</v>
       </c>
-      <c r="Y33" s="264">
+      <c r="Y33" s="252">
         <v>351</v>
       </c>
-      <c r="Z33" s="264">
+      <c r="Z33" s="193">
         <v>352</v>
       </c>
-      <c r="AA33" s="264">
+      <c r="AA33" s="193">
         <v>353</v>
       </c>
-      <c r="AB33" s="194">
+      <c r="AB33" s="193">
         <v>354</v>
       </c>
-      <c r="AC33" s="194">
+      <c r="AC33" s="193">
         <v>355</v>
       </c>
-      <c r="AD33" s="194">
+      <c r="AD33" s="193">
         <v>356</v>
       </c>
       <c r="AE33" s="115"/>
       <c r="AF33" s="185">
         <v>11</v>
       </c>
-      <c r="AG33" s="267"/>
-      <c r="AH33" s="275"/>
-      <c r="AI33" s="267"/>
-      <c r="AJ33" s="276"/>
-      <c r="AK33" s="267"/>
-      <c r="AL33" s="276"/>
-      <c r="AM33" s="267"/>
-      <c r="AN33" s="276"/>
-      <c r="AO33" s="267"/>
-      <c r="AP33" s="276"/>
-      <c r="AQ33" s="267"/>
-      <c r="AR33" s="276"/>
+      <c r="AG33" s="255"/>
+      <c r="AH33" s="263"/>
+      <c r="AI33" s="255"/>
+      <c r="AJ33" s="264"/>
+      <c r="AK33" s="255"/>
+      <c r="AL33" s="264"/>
+      <c r="AM33" s="255"/>
+      <c r="AN33" s="264"/>
+      <c r="AO33" s="255"/>
+      <c r="AP33" s="264"/>
+      <c r="AQ33" s="255"/>
+      <c r="AR33" s="264"/>
       <c r="AS33" s="181"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="115"/>
-      <c r="B34" s="267"/>
-      <c r="C34" s="267"/>
-      <c r="D34" s="267"/>
-      <c r="E34" s="267"/>
-      <c r="F34" s="267"/>
-      <c r="G34" s="267"/>
-      <c r="H34" s="267"/>
-      <c r="I34" s="267"/>
-      <c r="J34" s="267"/>
-      <c r="K34" s="267"/>
-      <c r="L34" s="267"/>
-      <c r="M34" s="267"/>
+      <c r="B34" s="255"/>
+      <c r="C34" s="255"/>
+      <c r="D34" s="255"/>
+      <c r="E34" s="255"/>
+      <c r="F34" s="255"/>
+      <c r="G34" s="255"/>
+      <c r="H34" s="255"/>
+      <c r="I34" s="255"/>
+      <c r="J34" s="255"/>
+      <c r="K34" s="255"/>
+      <c r="L34" s="255"/>
+      <c r="M34" s="255"/>
       <c r="N34" s="186">
         <v>12</v>
       </c>
       <c r="O34" s="141"/>
-      <c r="P34" s="194">
-        <v>363</v>
-      </c>
-      <c r="Q34" s="194">
-        <v>364</v>
-      </c>
-      <c r="R34" s="248" t="s">
+      <c r="P34" s="246" t="s">
         <v>777</v>
       </c>
-      <c r="S34" s="200">
+      <c r="Q34" s="199">
+        <v>362</v>
+      </c>
+      <c r="R34" s="199">
+        <v>361</v>
+      </c>
+      <c r="S34" s="199">
         <v>360</v>
       </c>
-      <c r="T34" s="200">
+      <c r="T34" s="199">
         <v>359</v>
       </c>
-      <c r="U34" s="200">
+      <c r="U34" s="199">
         <v>358</v>
       </c>
-      <c r="V34" s="200">
+      <c r="V34" s="199">
         <v>357</v>
       </c>
       <c r="W34" s="166"/>
-      <c r="X34" s="200">
+      <c r="X34" s="199">
         <v>357</v>
       </c>
-      <c r="Y34" s="200">
+      <c r="Y34" s="199">
         <v>358</v>
       </c>
-      <c r="Z34" s="200">
-        <v>359</v>
-      </c>
-      <c r="AA34" s="200">
-        <v>360</v>
-      </c>
-      <c r="AB34" s="265"/>
-      <c r="AC34" s="265"/>
-      <c r="AD34" s="265"/>
+      <c r="Z34" s="253"/>
+      <c r="AA34" s="253"/>
+      <c r="AB34" s="253"/>
+      <c r="AC34" s="253"/>
+      <c r="AD34" s="253"/>
       <c r="AE34" s="115"/>
       <c r="AF34" s="185">
         <v>12</v>
       </c>
-      <c r="AG34" s="267"/>
-      <c r="AH34" s="275"/>
-      <c r="AI34" s="267"/>
-      <c r="AJ34" s="276"/>
-      <c r="AK34" s="267"/>
-      <c r="AL34" s="276"/>
-      <c r="AM34" s="267"/>
-      <c r="AN34" s="276"/>
-      <c r="AO34" s="267"/>
-      <c r="AP34" s="276"/>
-      <c r="AQ34" s="267"/>
-      <c r="AR34" s="276"/>
+      <c r="AG34" s="255"/>
+      <c r="AH34" s="263"/>
+      <c r="AI34" s="255"/>
+      <c r="AJ34" s="264"/>
+      <c r="AK34" s="255"/>
+      <c r="AL34" s="264"/>
+      <c r="AM34" s="255"/>
+      <c r="AN34" s="264"/>
+      <c r="AO34" s="255"/>
+      <c r="AP34" s="264"/>
+      <c r="AQ34" s="255"/>
+      <c r="AR34" s="264"/>
       <c r="AS34" s="181"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="115"/>
-      <c r="B35" s="267"/>
-      <c r="C35" s="267"/>
-      <c r="D35" s="267"/>
-      <c r="E35" s="267"/>
-      <c r="F35" s="267"/>
-      <c r="G35" s="267"/>
-      <c r="H35" s="267"/>
-      <c r="I35" s="267"/>
-      <c r="J35" s="267"/>
-      <c r="K35" s="267"/>
-      <c r="L35" s="267"/>
-      <c r="M35" s="267"/>
-      <c r="N35" s="270"/>
-      <c r="O35" s="271"/>
-      <c r="P35" s="265"/>
-      <c r="Q35" s="265"/>
-      <c r="R35" s="265"/>
-      <c r="S35" s="265"/>
-      <c r="T35" s="267"/>
-      <c r="U35" s="267"/>
-      <c r="V35" s="267"/>
-      <c r="W35" s="272"/>
-      <c r="X35" s="267"/>
-      <c r="Y35" s="267"/>
-      <c r="Z35" s="267"/>
-      <c r="AA35" s="267"/>
-      <c r="AB35" s="267"/>
-      <c r="AC35" s="267"/>
-      <c r="AD35" s="267"/>
-      <c r="AE35" s="273"/>
-      <c r="AF35" s="274"/>
-      <c r="AG35" s="267"/>
-      <c r="AH35" s="275"/>
-      <c r="AI35" s="267"/>
-      <c r="AJ35" s="276"/>
-      <c r="AK35" s="267"/>
-      <c r="AL35" s="276"/>
-      <c r="AM35" s="267"/>
-      <c r="AN35" s="276"/>
-      <c r="AO35" s="267"/>
-      <c r="AP35" s="276"/>
-      <c r="AQ35" s="267"/>
-      <c r="AR35" s="276"/>
+      <c r="B35" s="255"/>
+      <c r="C35" s="255"/>
+      <c r="D35" s="255"/>
+      <c r="E35" s="255"/>
+      <c r="F35" s="255"/>
+      <c r="G35" s="255"/>
+      <c r="H35" s="255"/>
+      <c r="I35" s="255"/>
+      <c r="J35" s="255"/>
+      <c r="K35" s="255"/>
+      <c r="L35" s="255"/>
+      <c r="M35" s="255"/>
+      <c r="N35" s="258"/>
+      <c r="O35" s="259"/>
+      <c r="P35" s="253"/>
+      <c r="Q35" s="253"/>
+      <c r="R35" s="253"/>
+      <c r="S35" s="253"/>
+      <c r="T35" s="255"/>
+      <c r="U35" s="255"/>
+      <c r="V35" s="255"/>
+      <c r="W35" s="260"/>
+      <c r="X35" s="255"/>
+      <c r="Y35" s="255"/>
+      <c r="Z35" s="255"/>
+      <c r="AA35" s="255"/>
+      <c r="AB35" s="255"/>
+      <c r="AC35" s="255"/>
+      <c r="AD35" s="255"/>
+      <c r="AE35" s="261"/>
+      <c r="AF35" s="262"/>
+      <c r="AG35" s="255"/>
+      <c r="AH35" s="263"/>
+      <c r="AI35" s="255"/>
+      <c r="AJ35" s="264"/>
+      <c r="AK35" s="255"/>
+      <c r="AL35" s="264"/>
+      <c r="AM35" s="255"/>
+      <c r="AN35" s="264"/>
+      <c r="AO35" s="255"/>
+      <c r="AP35" s="264"/>
+      <c r="AQ35" s="255"/>
+      <c r="AR35" s="264"/>
       <c r="AS35" s="181"/>
     </row>
     <row r="36" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="115"/>
-      <c r="B36" s="267"/>
-      <c r="C36" s="267"/>
-      <c r="D36" s="267"/>
-      <c r="E36" s="267"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="267"/>
-      <c r="H36" s="267"/>
-      <c r="I36" s="267"/>
-      <c r="J36" s="267"/>
-      <c r="K36" s="267"/>
-      <c r="L36" s="267"/>
-      <c r="M36" s="267"/>
-      <c r="N36" s="270"/>
-      <c r="O36" s="251"/>
-      <c r="P36" s="267"/>
-      <c r="Q36" s="267"/>
-      <c r="R36" s="267"/>
-      <c r="S36" s="267"/>
-      <c r="T36" s="267"/>
-      <c r="U36" s="267"/>
-      <c r="V36" s="267"/>
-      <c r="W36" s="272"/>
-      <c r="X36" s="265"/>
-      <c r="Y36" s="265"/>
-      <c r="Z36" s="265"/>
-      <c r="AA36" s="265"/>
-      <c r="AB36" s="265"/>
-      <c r="AC36" s="265"/>
-      <c r="AD36" s="265"/>
-      <c r="AE36" s="273"/>
-      <c r="AF36" s="274"/>
-      <c r="AG36" s="276"/>
-      <c r="AH36" s="276"/>
-      <c r="AI36" s="276"/>
-      <c r="AJ36" s="276"/>
-      <c r="AK36" s="276"/>
-      <c r="AL36" s="276"/>
-      <c r="AM36" s="276"/>
-      <c r="AN36" s="276"/>
-      <c r="AO36" s="276"/>
-      <c r="AP36" s="276"/>
-      <c r="AQ36" s="276"/>
-      <c r="AR36" s="276"/>
+      <c r="B36" s="255"/>
+      <c r="C36" s="255"/>
+      <c r="D36" s="255"/>
+      <c r="E36" s="255"/>
+      <c r="F36" s="255"/>
+      <c r="G36" s="255"/>
+      <c r="H36" s="255"/>
+      <c r="I36" s="255"/>
+      <c r="J36" s="255"/>
+      <c r="K36" s="255"/>
+      <c r="L36" s="255"/>
+      <c r="M36" s="255"/>
+      <c r="N36" s="258"/>
+      <c r="O36" s="248"/>
+      <c r="P36" s="255"/>
+      <c r="Q36" s="255"/>
+      <c r="R36" s="255"/>
+      <c r="S36" s="255"/>
+      <c r="T36" s="255"/>
+      <c r="U36" s="255"/>
+      <c r="V36" s="255"/>
+      <c r="W36" s="260"/>
+      <c r="X36" s="253"/>
+      <c r="Y36" s="253"/>
+      <c r="Z36" s="253"/>
+      <c r="AA36" s="253"/>
+      <c r="AB36" s="253"/>
+      <c r="AC36" s="253"/>
+      <c r="AD36" s="253"/>
+      <c r="AE36" s="261"/>
+      <c r="AF36" s="262"/>
+      <c r="AG36" s="264"/>
+      <c r="AH36" s="264"/>
+      <c r="AI36" s="264"/>
+      <c r="AJ36" s="264"/>
+      <c r="AK36" s="264"/>
+      <c r="AL36" s="264"/>
+      <c r="AM36" s="264"/>
+      <c r="AN36" s="264"/>
+      <c r="AO36" s="264"/>
+      <c r="AP36" s="264"/>
+      <c r="AQ36" s="264"/>
+      <c r="AR36" s="264"/>
       <c r="AS36" s="181"/>
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37" s="115"/>
-      <c r="B37" s="267"/>
-      <c r="C37" s="267"/>
-      <c r="D37" s="267"/>
-      <c r="E37" s="267"/>
-      <c r="F37" s="267"/>
-      <c r="G37" s="267"/>
-      <c r="H37" s="267"/>
-      <c r="I37" s="267"/>
-      <c r="J37" s="267"/>
-      <c r="K37" s="267"/>
-      <c r="L37" s="267"/>
-      <c r="M37" s="267"/>
-      <c r="N37" s="270"/>
-      <c r="O37" s="271"/>
-      <c r="P37" s="265"/>
-      <c r="Q37" s="265"/>
-      <c r="R37" s="265"/>
-      <c r="S37" s="265"/>
-      <c r="T37" s="265"/>
-      <c r="U37" s="265"/>
-      <c r="V37" s="265"/>
-      <c r="W37" s="272"/>
-      <c r="X37" s="265"/>
-      <c r="Y37" s="265"/>
-      <c r="Z37" s="265"/>
-      <c r="AA37" s="265"/>
-      <c r="AB37" s="265"/>
-      <c r="AC37" s="265"/>
-      <c r="AD37" s="267"/>
-      <c r="AE37" s="273"/>
-      <c r="AF37" s="274"/>
-      <c r="AG37" s="267"/>
-      <c r="AH37" s="277"/>
-      <c r="AI37" s="267"/>
-      <c r="AJ37" s="278"/>
-      <c r="AK37" s="267"/>
-      <c r="AL37" s="278"/>
-      <c r="AM37" s="267"/>
-      <c r="AN37" s="278"/>
-      <c r="AO37" s="267"/>
-      <c r="AP37" s="278"/>
-      <c r="AQ37" s="267"/>
-      <c r="AR37" s="278"/>
+      <c r="B37" s="255"/>
+      <c r="C37" s="255"/>
+      <c r="D37" s="255"/>
+      <c r="E37" s="255"/>
+      <c r="F37" s="255"/>
+      <c r="G37" s="255"/>
+      <c r="H37" s="255"/>
+      <c r="I37" s="255"/>
+      <c r="J37" s="255"/>
+      <c r="K37" s="255"/>
+      <c r="L37" s="255"/>
+      <c r="M37" s="255"/>
+      <c r="N37" s="258"/>
+      <c r="O37" s="259"/>
+      <c r="P37" s="253"/>
+      <c r="Q37" s="253"/>
+      <c r="R37" s="253"/>
+      <c r="S37" s="253"/>
+      <c r="T37" s="253"/>
+      <c r="U37" s="253"/>
+      <c r="V37" s="253"/>
+      <c r="W37" s="260"/>
+      <c r="X37" s="253"/>
+      <c r="Y37" s="253"/>
+      <c r="Z37" s="253"/>
+      <c r="AA37" s="253"/>
+      <c r="AB37" s="253"/>
+      <c r="AC37" s="253"/>
+      <c r="AD37" s="255"/>
+      <c r="AE37" s="261"/>
+      <c r="AF37" s="262"/>
+      <c r="AG37" s="255"/>
+      <c r="AH37" s="265"/>
+      <c r="AI37" s="255"/>
+      <c r="AJ37" s="266"/>
+      <c r="AK37" s="255"/>
+      <c r="AL37" s="266"/>
+      <c r="AM37" s="255"/>
+      <c r="AN37" s="266"/>
+      <c r="AO37" s="255"/>
+      <c r="AP37" s="266"/>
+      <c r="AQ37" s="255"/>
+      <c r="AR37" s="266"/>
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38" s="115"/>
@@ -7983,55 +7981,55 @@
       <c r="AQ47" s="115"/>
     </row>
     <row r="48" spans="1:45" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="225" t="s">
+      <c r="A48" s="223" t="s">
         <v>758</v>
       </c>
-      <c r="B48" s="231"/>
-      <c r="C48" s="226"/>
-      <c r="D48" s="226"/>
-      <c r="E48" s="226"/>
-      <c r="F48" s="226"/>
-      <c r="G48" s="226"/>
-      <c r="H48" s="226"/>
+      <c r="B48" s="229"/>
+      <c r="C48" s="224"/>
+      <c r="D48" s="224"/>
+      <c r="E48" s="224"/>
+      <c r="F48" s="224"/>
+      <c r="G48" s="224"/>
+      <c r="H48" s="224"/>
       <c r="I48" s="176"/>
       <c r="J48" s="176"/>
       <c r="K48" s="176"/>
       <c r="L48" s="176"/>
       <c r="M48" s="176"/>
-      <c r="N48" s="233" t="s">
+      <c r="N48" s="231" t="s">
         <v>758</v>
       </c>
-      <c r="O48" s="205">
+      <c r="O48" s="204">
         <v>6</v>
       </c>
-      <c r="P48" s="216" t="s">
+      <c r="P48" s="215" t="s">
         <v>765</v>
       </c>
-      <c r="Q48" s="234"/>
-      <c r="R48" s="235"/>
-      <c r="S48" s="236"/>
-      <c r="T48" s="236"/>
-      <c r="U48" s="236"/>
+      <c r="Q48" s="232"/>
+      <c r="R48" s="233"/>
+      <c r="S48" s="234"/>
+      <c r="T48" s="234"/>
+      <c r="U48" s="234"/>
       <c r="V48" s="143"/>
       <c r="W48" s="143"/>
       <c r="X48" s="143"/>
       <c r="Y48" s="143"/>
       <c r="Z48" s="115"/>
-      <c r="AA48" s="232" t="s">
+      <c r="AA48" s="230" t="s">
         <v>758</v>
       </c>
-      <c r="AB48" s="217">
+      <c r="AB48" s="216">
         <v>1</v>
       </c>
-      <c r="AC48" s="216" t="s">
+      <c r="AC48" s="215" t="s">
         <v>769</v>
       </c>
-      <c r="AD48" s="236"/>
-      <c r="AE48" s="236"/>
-      <c r="AF48" s="236"/>
-      <c r="AG48" s="236"/>
-      <c r="AH48" s="215"/>
-      <c r="AI48" s="215"/>
+      <c r="AD48" s="234"/>
+      <c r="AE48" s="234"/>
+      <c r="AF48" s="234"/>
+      <c r="AG48" s="234"/>
+      <c r="AH48" s="214"/>
+      <c r="AI48" s="214"/>
       <c r="AJ48" s="115"/>
       <c r="AK48" s="115"/>
       <c r="AL48" s="115"/>
@@ -8042,32 +8040,32 @@
       <c r="AQ48" s="115"/>
     </row>
     <row r="49" spans="1:43" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="222" t="s">
+      <c r="A49" s="220" t="s">
         <v>759</v>
       </c>
-      <c r="B49" s="204">
+      <c r="B49" s="203">
         <v>120</v>
       </c>
-      <c r="C49" s="229" t="s">
+      <c r="C49" s="227" t="s">
         <v>757</v>
       </c>
-      <c r="D49" s="230"/>
-      <c r="E49" s="230"/>
-      <c r="F49" s="230"/>
-      <c r="G49" s="230"/>
-      <c r="H49" s="230"/>
+      <c r="D49" s="228"/>
+      <c r="E49" s="228"/>
+      <c r="F49" s="228"/>
+      <c r="G49" s="228"/>
+      <c r="H49" s="228"/>
       <c r="I49" s="176"/>
       <c r="J49" s="176"/>
       <c r="K49" s="176"/>
       <c r="L49" s="176"/>
       <c r="M49" s="176"/>
-      <c r="N49" s="221" t="s">
+      <c r="N49" s="219" t="s">
         <v>759</v>
       </c>
-      <c r="O49" s="243">
+      <c r="O49" s="241">
         <v>1</v>
       </c>
-      <c r="P49" s="212" t="s">
+      <c r="P49" s="211" t="s">
         <v>766</v>
       </c>
       <c r="Q49" s="142"/>
@@ -8080,13 +8078,13 @@
       <c r="X49" s="143"/>
       <c r="Y49" s="143"/>
       <c r="Z49" s="115"/>
-      <c r="AA49" s="209" t="s">
+      <c r="AA49" s="208" t="s">
         <v>759</v>
       </c>
-      <c r="AB49" s="211">
+      <c r="AB49" s="210">
         <v>66</v>
       </c>
-      <c r="AC49" s="212" t="s">
+      <c r="AC49" s="211" t="s">
         <v>764</v>
       </c>
       <c r="AD49" s="143"/>
@@ -8105,28 +8103,28 @@
       <c r="AQ49" s="115"/>
     </row>
     <row r="50" spans="1:43" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="224" t="s">
+      <c r="A50" s="222" t="s">
         <v>756</v>
       </c>
-      <c r="B50" s="231"/>
-      <c r="C50" s="201"/>
-      <c r="D50" s="202"/>
-      <c r="E50" s="202"/>
-      <c r="F50" s="202"/>
-      <c r="G50" s="202"/>
-      <c r="H50" s="202"/>
+      <c r="B50" s="229"/>
+      <c r="C50" s="200"/>
+      <c r="D50" s="201"/>
+      <c r="E50" s="201"/>
+      <c r="F50" s="201"/>
+      <c r="G50" s="201"/>
+      <c r="H50" s="201"/>
       <c r="I50" s="170"/>
       <c r="J50" s="170"/>
       <c r="K50" s="170"/>
       <c r="L50" s="170"/>
       <c r="M50" s="170"/>
-      <c r="N50" s="221" t="s">
+      <c r="N50" s="219" t="s">
         <v>760</v>
       </c>
-      <c r="O50" s="214">
+      <c r="O50" s="213">
         <v>6</v>
       </c>
-      <c r="P50" s="212" t="s">
+      <c r="P50" s="211" t="s">
         <v>767</v>
       </c>
       <c r="Q50" s="143"/>
@@ -8139,21 +8137,21 @@
       <c r="X50" s="143"/>
       <c r="Y50" s="143"/>
       <c r="Z50" s="115"/>
-      <c r="AA50" s="237" t="s">
+      <c r="AA50" s="235" t="s">
         <v>763</v>
       </c>
-      <c r="AB50" s="249">
+      <c r="AB50" s="247">
         <v>9</v>
       </c>
-      <c r="AC50" s="213" t="s">
+      <c r="AC50" s="212" t="s">
         <v>770</v>
       </c>
       <c r="AD50" s="174"/>
       <c r="AE50" s="174"/>
       <c r="AF50" s="174"/>
       <c r="AG50" s="174"/>
-      <c r="AH50" s="208"/>
-      <c r="AI50" s="208"/>
+      <c r="AH50" s="207"/>
+      <c r="AI50" s="207"/>
       <c r="AJ50" s="115"/>
       <c r="AK50" s="115"/>
       <c r="AL50" s="115"/>
@@ -8174,13 +8172,13 @@
       <c r="K51" s="170"/>
       <c r="L51" s="170"/>
       <c r="M51" s="170"/>
-      <c r="N51" s="227" t="s">
+      <c r="N51" s="225" t="s">
         <v>756</v>
       </c>
-      <c r="O51" s="206">
+      <c r="O51" s="205">
         <v>10</v>
       </c>
-      <c r="P51" s="228" t="s">
+      <c r="P51" s="226" t="s">
         <v>768</v>
       </c>
       <c r="Q51" s="143"/>
@@ -8209,7 +8207,7 @@
       <c r="AQ51" s="115"/>
     </row>
     <row r="52" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="212"/>
+      <c r="D52" s="211"/>
       <c r="E52" s="170"/>
       <c r="F52" s="170"/>
       <c r="G52" s="170"/>
@@ -8219,11 +8217,11 @@
       <c r="K52" s="170"/>
       <c r="L52" s="170"/>
       <c r="M52" s="170"/>
-      <c r="N52" s="203"/>
-      <c r="O52" s="210">
+      <c r="N52" s="202"/>
+      <c r="O52" s="209">
         <v>500</v>
       </c>
-      <c r="P52" s="213" t="s">
+      <c r="P52" s="212" t="s">
         <v>776</v>
       </c>
       <c r="Q52" s="174"/>
@@ -8297,14 +8295,14 @@
       <c r="AQ53" s="115"/>
     </row>
     <row r="54" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A54" s="212"/>
-      <c r="B54" s="212"/>
-      <c r="C54" s="212"/>
-      <c r="D54" s="212"/>
-      <c r="E54" s="212"/>
-      <c r="F54" s="212"/>
-      <c r="G54" s="212"/>
-      <c r="H54" s="212"/>
+      <c r="A54" s="211"/>
+      <c r="B54" s="211"/>
+      <c r="C54" s="211"/>
+      <c r="D54" s="211"/>
+      <c r="E54" s="211"/>
+      <c r="F54" s="211"/>
+      <c r="G54" s="211"/>
+      <c r="H54" s="211"/>
       <c r="I54" s="170"/>
       <c r="J54" s="170"/>
       <c r="K54" s="170"/>
@@ -8324,7 +8322,7 @@
       <c r="Y54" s="143"/>
       <c r="Z54" s="143"/>
       <c r="AA54" s="143"/>
-      <c r="AB54" s="219"/>
+      <c r="AB54" s="218"/>
       <c r="AC54" s="143"/>
       <c r="AD54" s="143"/>
       <c r="AE54" s="115"/>
@@ -8342,7 +8340,7 @@
       <c r="AQ54" s="115"/>
     </row>
     <row r="55" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="B55" s="195"/>
+      <c r="B55" s="194"/>
       <c r="C55" s="170"/>
       <c r="D55" s="170"/>
       <c r="E55" s="170"/>
@@ -8355,7 +8353,7 @@
       <c r="L55" s="170"/>
       <c r="M55" s="170"/>
       <c r="N55" s="115"/>
-      <c r="O55" s="207">
+      <c r="O55" s="206">
         <v>3</v>
       </c>
       <c r="P55" s="143"/>
@@ -8370,7 +8368,7 @@
       <c r="Y55" s="143"/>
       <c r="Z55" s="143"/>
       <c r="AA55" s="143"/>
-      <c r="AB55" s="218"/>
+      <c r="AB55" s="217"/>
       <c r="AC55" s="143"/>
       <c r="AD55" s="143"/>
       <c r="AE55" s="115"/>
@@ -8388,50 +8386,50 @@
       <c r="AQ55" s="115"/>
     </row>
     <row r="56" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A56" s="262">
+      <c r="A56" s="276">
         <f>SUM(B48:B50,O48:O52,AB48:AB50)</f>
         <v>719</v>
       </c>
-      <c r="B56" s="262"/>
-      <c r="C56" s="262"/>
-      <c r="D56" s="262"/>
-      <c r="E56" s="262"/>
-      <c r="F56" s="262"/>
-      <c r="G56" s="262"/>
-      <c r="H56" s="262"/>
-      <c r="I56" s="262"/>
-      <c r="J56" s="262"/>
-      <c r="K56" s="262"/>
-      <c r="L56" s="262"/>
-      <c r="M56" s="262"/>
-      <c r="N56" s="262"/>
-      <c r="O56" s="263"/>
-      <c r="P56" s="262"/>
-      <c r="Q56" s="262"/>
-      <c r="R56" s="262"/>
-      <c r="S56" s="262"/>
-      <c r="T56" s="262"/>
-      <c r="U56" s="262"/>
-      <c r="V56" s="262"/>
-      <c r="W56" s="262"/>
-      <c r="X56" s="262"/>
-      <c r="Y56" s="262"/>
-      <c r="Z56" s="262"/>
-      <c r="AA56" s="262"/>
-      <c r="AB56" s="263"/>
-      <c r="AC56" s="262"/>
-      <c r="AD56" s="262"/>
-      <c r="AE56" s="262"/>
-      <c r="AF56" s="262"/>
-      <c r="AG56" s="262"/>
-      <c r="AH56" s="262"/>
-      <c r="AI56" s="262"/>
-      <c r="AJ56" s="262"/>
-      <c r="AK56" s="262"/>
+      <c r="B56" s="276"/>
+      <c r="C56" s="276"/>
+      <c r="D56" s="276"/>
+      <c r="E56" s="276"/>
+      <c r="F56" s="276"/>
+      <c r="G56" s="276"/>
+      <c r="H56" s="276"/>
+      <c r="I56" s="276"/>
+      <c r="J56" s="276"/>
+      <c r="K56" s="276"/>
+      <c r="L56" s="276"/>
+      <c r="M56" s="276"/>
+      <c r="N56" s="276"/>
+      <c r="O56" s="277"/>
+      <c r="P56" s="276"/>
+      <c r="Q56" s="276"/>
+      <c r="R56" s="276"/>
+      <c r="S56" s="276"/>
+      <c r="T56" s="276"/>
+      <c r="U56" s="276"/>
+      <c r="V56" s="276"/>
+      <c r="W56" s="276"/>
+      <c r="X56" s="276"/>
+      <c r="Y56" s="276"/>
+      <c r="Z56" s="276"/>
+      <c r="AA56" s="276"/>
+      <c r="AB56" s="277"/>
+      <c r="AC56" s="276"/>
+      <c r="AD56" s="276"/>
+      <c r="AE56" s="276"/>
+      <c r="AF56" s="276"/>
+      <c r="AG56" s="276"/>
+      <c r="AH56" s="276"/>
+      <c r="AI56" s="276"/>
+      <c r="AJ56" s="276"/>
+      <c r="AK56" s="276"/>
     </row>
     <row r="58" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H58" s="261"/>
-      <c r="I58" s="261"/>
+      <c r="H58" s="275"/>
+      <c r="I58" s="275"/>
     </row>
     <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AA60" s="13"/>
@@ -8449,8 +8447,8 @@
       <c r="AJ66" s="131"/>
     </row>
     <row r="67" spans="13:36" x14ac:dyDescent="0.2">
-      <c r="AI67" s="255"/>
-      <c r="AJ67" s="255"/>
+      <c r="AI67" s="269"/>
+      <c r="AJ67" s="269"/>
     </row>
     <row r="68" spans="13:36" x14ac:dyDescent="0.2">
       <c r="AI68" s="113"/>

</xml_diff>

<commit_message>
Commit 5 Penyusunan Denah Wisuda USK 163
Hasil Penyusunan Denah Wisuda USK Periode 163 Hari ke 3, Jum'at 22 November 2024 ( Mengubah Warna Fkip menjadi Biru )
</commit_message>
<xml_diff>
--- a/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
+++ b/KURSIWIS. JUM'AT 22 NOVEMBER 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data Hary\Denah Wisuda 163\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D5F43F-299A-407C-A7F2-25773C6D4079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594FD7F8-BE47-42BD-8BA1-83C257CC6C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2714,12 +2714,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
-        <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="8"/>
       </patternFill>
@@ -2734,12 +2728,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -2775,6 +2763,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3426,7 +3426,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3509,16 +3509,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3530,13 +3527,13 @@
     <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3546,13 +3543,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3562,10 +3559,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3574,14 +3568,14 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="9" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3637,40 +3631,31 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3679,13 +3664,13 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3724,6 +3709,12 @@
     <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3751,14 +3742,23 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4114,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A37" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="AR48" sqref="AR48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4131,49 +4131,49 @@
     <row r="1" spans="1:46" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="270" t="s">
+      <c r="C1" s="267" t="s">
         <v>762</v>
       </c>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271"/>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
-      <c r="Y1" s="271"/>
-      <c r="Z1" s="271"/>
-      <c r="AA1" s="271"/>
-      <c r="AB1" s="271"/>
-      <c r="AC1" s="271"/>
-      <c r="AD1" s="271"/>
-      <c r="AE1" s="271"/>
-      <c r="AF1" s="271"/>
-      <c r="AG1" s="271"/>
-      <c r="AH1" s="271"/>
-      <c r="AI1" s="271"/>
-      <c r="AJ1" s="271"/>
-      <c r="AK1" s="271"/>
-      <c r="AL1" s="271"/>
-      <c r="AM1" s="271"/>
-      <c r="AN1" s="271"/>
-      <c r="AO1" s="271"/>
-      <c r="AP1" s="271"/>
-      <c r="AQ1" s="272"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="268"/>
+      <c r="N1" s="268"/>
+      <c r="O1" s="268"/>
+      <c r="P1" s="268"/>
+      <c r="Q1" s="268"/>
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="268"/>
+      <c r="V1" s="268"/>
+      <c r="W1" s="268"/>
+      <c r="X1" s="268"/>
+      <c r="Y1" s="268"/>
+      <c r="Z1" s="268"/>
+      <c r="AA1" s="268"/>
+      <c r="AB1" s="268"/>
+      <c r="AC1" s="268"/>
+      <c r="AD1" s="268"/>
+      <c r="AE1" s="268"/>
+      <c r="AF1" s="268"/>
+      <c r="AG1" s="268"/>
+      <c r="AH1" s="268"/>
+      <c r="AI1" s="268"/>
+      <c r="AJ1" s="268"/>
+      <c r="AK1" s="268"/>
+      <c r="AL1" s="268"/>
+      <c r="AM1" s="268"/>
+      <c r="AN1" s="268"/>
+      <c r="AO1" s="268"/>
+      <c r="AP1" s="268"/>
+      <c r="AQ1" s="269"/>
       <c r="AR1" s="33"/>
       <c r="AS1" s="178"/>
     </row>
@@ -4182,45 +4182,45 @@
       <c r="B2" s="33"/>
       <c r="C2" s="128"/>
       <c r="D2" s="129"/>
-      <c r="E2" s="273" t="s">
+      <c r="E2" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="273"/>
-      <c r="I2" s="273"/>
-      <c r="J2" s="273"/>
-      <c r="K2" s="273"/>
-      <c r="L2" s="273"/>
-      <c r="M2" s="273"/>
-      <c r="N2" s="273"/>
-      <c r="O2" s="273"/>
-      <c r="P2" s="273"/>
-      <c r="Q2" s="273"/>
-      <c r="R2" s="273"/>
-      <c r="S2" s="273"/>
-      <c r="T2" s="273"/>
-      <c r="U2" s="273"/>
-      <c r="V2" s="273"/>
-      <c r="W2" s="273"/>
-      <c r="X2" s="273"/>
-      <c r="Y2" s="273"/>
-      <c r="Z2" s="273"/>
-      <c r="AA2" s="273"/>
-      <c r="AB2" s="273"/>
-      <c r="AC2" s="273"/>
-      <c r="AD2" s="273"/>
-      <c r="AE2" s="273"/>
-      <c r="AF2" s="273"/>
-      <c r="AG2" s="273"/>
-      <c r="AH2" s="273"/>
-      <c r="AI2" s="273"/>
-      <c r="AJ2" s="273"/>
-      <c r="AK2" s="273"/>
-      <c r="AL2" s="273"/>
-      <c r="AM2" s="273"/>
-      <c r="AN2" s="273"/>
-      <c r="AO2" s="273"/>
+      <c r="F2" s="270"/>
+      <c r="G2" s="270"/>
+      <c r="H2" s="270"/>
+      <c r="I2" s="270"/>
+      <c r="J2" s="270"/>
+      <c r="K2" s="270"/>
+      <c r="L2" s="270"/>
+      <c r="M2" s="270"/>
+      <c r="N2" s="270"/>
+      <c r="O2" s="270"/>
+      <c r="P2" s="270"/>
+      <c r="Q2" s="270"/>
+      <c r="R2" s="270"/>
+      <c r="S2" s="270"/>
+      <c r="T2" s="270"/>
+      <c r="U2" s="270"/>
+      <c r="V2" s="270"/>
+      <c r="W2" s="270"/>
+      <c r="X2" s="270"/>
+      <c r="Y2" s="270"/>
+      <c r="Z2" s="270"/>
+      <c r="AA2" s="270"/>
+      <c r="AB2" s="270"/>
+      <c r="AC2" s="270"/>
+      <c r="AD2" s="270"/>
+      <c r="AE2" s="270"/>
+      <c r="AF2" s="270"/>
+      <c r="AG2" s="270"/>
+      <c r="AH2" s="270"/>
+      <c r="AI2" s="270"/>
+      <c r="AJ2" s="270"/>
+      <c r="AK2" s="270"/>
+      <c r="AL2" s="270"/>
+      <c r="AM2" s="270"/>
+      <c r="AN2" s="270"/>
+      <c r="AO2" s="270"/>
       <c r="AP2" s="129"/>
       <c r="AQ2" s="130"/>
       <c r="AR2" s="33"/>
@@ -4506,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="123"/>
-      <c r="C7" s="236" t="s">
+      <c r="C7" s="234" t="s">
         <v>771</v>
       </c>
       <c r="D7" s="190" t="s">
@@ -4536,13 +4536,13 @@
       <c r="L7" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="197" t="s">
+      <c r="M7" s="196" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="190" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="197" t="s">
+      <c r="O7" s="196" t="s">
         <v>21</v>
       </c>
       <c r="P7" s="190" t="s">
@@ -4888,10 +4888,10 @@
       <c r="AP9" s="190" t="s">
         <v>60</v>
       </c>
-      <c r="AQ9" s="278" t="s">
+      <c r="AQ9" s="264" t="s">
         <v>59</v>
       </c>
-      <c r="AR9" s="279" t="s">
+      <c r="AR9" s="265" t="s">
         <v>761</v>
       </c>
       <c r="AS9" s="51">
@@ -4904,10 +4904,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="147"/>
-      <c r="C10" s="237" t="s">
+      <c r="C10" s="235" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="238" t="s">
+      <c r="D10" s="236" t="s">
         <v>772</v>
       </c>
       <c r="E10" s="191" t="s">
@@ -4925,104 +4925,104 @@
       <c r="I10" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="240" t="s">
+      <c r="J10" s="279" t="s">
         <v>773</v>
       </c>
-      <c r="K10" s="239" t="s">
+      <c r="K10" s="237" t="s">
         <v>774</v>
       </c>
-      <c r="L10" s="198" t="s">
+      <c r="L10" s="197" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="198" t="s">
+      <c r="M10" s="197" t="s">
         <v>95</v>
       </c>
-      <c r="N10" s="198" t="s">
+      <c r="N10" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="O10" s="198" t="s">
+      <c r="O10" s="197" t="s">
         <v>97</v>
       </c>
-      <c r="P10" s="198" t="s">
+      <c r="P10" s="197" t="s">
         <v>98</v>
       </c>
-      <c r="Q10" s="243" t="s">
+      <c r="Q10" s="239" t="s">
         <v>775</v>
       </c>
-      <c r="R10" s="242" t="s">
+      <c r="R10" s="238" t="s">
         <v>100</v>
       </c>
-      <c r="S10" s="242" t="s">
+      <c r="S10" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="242" t="s">
+      <c r="T10" s="238" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="242" t="s">
+      <c r="U10" s="238" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="242" t="s">
+      <c r="V10" s="238" t="s">
         <v>58</v>
       </c>
       <c r="W10" s="137"/>
-      <c r="X10" s="242" t="s">
+      <c r="X10" s="238" t="s">
         <v>58</v>
       </c>
-      <c r="Y10" s="242" t="s">
+      <c r="Y10" s="238" t="s">
         <v>57</v>
       </c>
-      <c r="Z10" s="242" t="s">
+      <c r="Z10" s="238" t="s">
         <v>56</v>
       </c>
-      <c r="AA10" s="242" t="s">
+      <c r="AA10" s="238" t="s">
         <v>101</v>
       </c>
-      <c r="AB10" s="244" t="s">
+      <c r="AB10" s="275" t="s">
         <v>145</v>
       </c>
-      <c r="AC10" s="192" t="s">
+      <c r="AC10" s="276" t="s">
         <v>99</v>
       </c>
-      <c r="AD10" s="192" t="s">
+      <c r="AD10" s="276" t="s">
         <v>98</v>
       </c>
-      <c r="AE10" s="192" t="s">
+      <c r="AE10" s="276" t="s">
         <v>97</v>
       </c>
-      <c r="AF10" s="192" t="s">
+      <c r="AF10" s="276" t="s">
         <v>96</v>
       </c>
-      <c r="AG10" s="192" t="s">
+      <c r="AG10" s="276" t="s">
         <v>95</v>
       </c>
-      <c r="AH10" s="192" t="s">
+      <c r="AH10" s="276" t="s">
         <v>94</v>
       </c>
-      <c r="AI10" s="192" t="s">
+      <c r="AI10" s="276" t="s">
         <v>93</v>
       </c>
-      <c r="AJ10" s="192" t="s">
+      <c r="AJ10" s="276" t="s">
         <v>92</v>
       </c>
-      <c r="AK10" s="192" t="s">
+      <c r="AK10" s="276" t="s">
         <v>91</v>
       </c>
-      <c r="AL10" s="192" t="s">
+      <c r="AL10" s="276" t="s">
         <v>90</v>
       </c>
-      <c r="AM10" s="192" t="s">
+      <c r="AM10" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="AN10" s="192" t="s">
+      <c r="AN10" s="276" t="s">
         <v>88</v>
       </c>
-      <c r="AO10" s="192" t="s">
+      <c r="AO10" s="276" t="s">
         <v>87</v>
       </c>
-      <c r="AP10" s="192" t="s">
+      <c r="AP10" s="276" t="s">
         <v>86</v>
       </c>
-      <c r="AQ10" s="192" t="s">
+      <c r="AQ10" s="276" t="s">
         <v>85</v>
       </c>
       <c r="AR10" s="169" t="s">
@@ -5038,128 +5038,128 @@
         <v>5</v>
       </c>
       <c r="B11" s="115"/>
-      <c r="C11" s="192">
+      <c r="C11" s="276">
         <v>100</v>
       </c>
-      <c r="D11" s="192" t="s">
+      <c r="D11" s="276" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="192" t="s">
+      <c r="E11" s="276" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="192" t="s">
+      <c r="F11" s="276" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="192" t="s">
+      <c r="G11" s="276" t="s">
         <v>112</v>
       </c>
-      <c r="H11" s="192" t="s">
+      <c r="H11" s="276" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="192" t="s">
+      <c r="I11" s="276" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="192" t="s">
+      <c r="J11" s="276" t="s">
         <v>115</v>
       </c>
-      <c r="K11" s="192" t="s">
+      <c r="K11" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="L11" s="192" t="s">
+      <c r="L11" s="276" t="s">
         <v>117</v>
       </c>
-      <c r="M11" s="192" t="s">
+      <c r="M11" s="276" t="s">
         <v>118</v>
       </c>
-      <c r="N11" s="192" t="s">
+      <c r="N11" s="276" t="s">
         <v>119</v>
       </c>
-      <c r="O11" s="192" t="s">
+      <c r="O11" s="276" t="s">
         <v>120</v>
       </c>
-      <c r="P11" s="192" t="s">
+      <c r="P11" s="276" t="s">
         <v>121</v>
       </c>
-      <c r="Q11" s="192" t="s">
+      <c r="Q11" s="276" t="s">
         <v>122</v>
       </c>
-      <c r="R11" s="192" t="s">
+      <c r="R11" s="276" t="s">
         <v>123</v>
       </c>
-      <c r="S11" s="192" t="s">
+      <c r="S11" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="T11" s="192" t="s">
+      <c r="T11" s="276" t="s">
         <v>82</v>
       </c>
-      <c r="U11" s="192" t="s">
+      <c r="U11" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="V11" s="192" t="s">
+      <c r="V11" s="276" t="s">
         <v>84</v>
       </c>
       <c r="W11" s="137"/>
-      <c r="X11" s="192" t="s">
+      <c r="X11" s="276" t="s">
         <v>84</v>
       </c>
-      <c r="Y11" s="192" t="s">
+      <c r="Y11" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="Z11" s="192" t="s">
+      <c r="Z11" s="276" t="s">
         <v>82</v>
       </c>
-      <c r="AA11" s="192" t="s">
+      <c r="AA11" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="AB11" s="192" t="s">
+      <c r="AB11" s="276" t="s">
         <v>123</v>
       </c>
-      <c r="AC11" s="192" t="s">
+      <c r="AC11" s="276" t="s">
         <v>122</v>
       </c>
-      <c r="AD11" s="192" t="s">
+      <c r="AD11" s="276" t="s">
         <v>121</v>
       </c>
-      <c r="AE11" s="192" t="s">
+      <c r="AE11" s="276" t="s">
         <v>120</v>
       </c>
-      <c r="AF11" s="192" t="s">
+      <c r="AF11" s="276" t="s">
         <v>119</v>
       </c>
-      <c r="AG11" s="192" t="s">
+      <c r="AG11" s="276" t="s">
         <v>118</v>
       </c>
-      <c r="AH11" s="192" t="s">
+      <c r="AH11" s="276" t="s">
         <v>117</v>
       </c>
-      <c r="AI11" s="192" t="s">
+      <c r="AI11" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="AJ11" s="192" t="s">
+      <c r="AJ11" s="276" t="s">
         <v>115</v>
       </c>
-      <c r="AK11" s="192" t="s">
+      <c r="AK11" s="276" t="s">
         <v>114</v>
       </c>
-      <c r="AL11" s="192" t="s">
+      <c r="AL11" s="276" t="s">
         <v>113</v>
       </c>
-      <c r="AM11" s="192" t="s">
+      <c r="AM11" s="276" t="s">
         <v>112</v>
       </c>
-      <c r="AN11" s="192" t="s">
+      <c r="AN11" s="276" t="s">
         <v>111</v>
       </c>
-      <c r="AO11" s="192" t="s">
+      <c r="AO11" s="276" t="s">
         <v>110</v>
       </c>
-      <c r="AP11" s="192" t="s">
+      <c r="AP11" s="276" t="s">
         <v>109</v>
       </c>
-      <c r="AQ11" s="192" t="s">
+      <c r="AQ11" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="AR11" s="195" t="s">
+      <c r="AR11" s="194" t="s">
         <v>537</v>
       </c>
       <c r="AS11" s="51">
@@ -5171,126 +5171,126 @@
       <c r="A12" s="133">
         <v>6</v>
       </c>
-      <c r="B12" s="249"/>
-      <c r="C12" s="192">
+      <c r="B12" s="244"/>
+      <c r="C12" s="276">
         <v>120</v>
       </c>
-      <c r="D12" s="192">
+      <c r="D12" s="276">
         <v>119</v>
       </c>
-      <c r="E12" s="192">
+      <c r="E12" s="276">
         <v>118</v>
       </c>
-      <c r="F12" s="192">
+      <c r="F12" s="276">
         <v>117</v>
       </c>
-      <c r="G12" s="192">
+      <c r="G12" s="276">
         <v>116</v>
       </c>
-      <c r="H12" s="192">
+      <c r="H12" s="276">
         <v>115</v>
       </c>
-      <c r="I12" s="192">
+      <c r="I12" s="276">
         <v>114</v>
       </c>
-      <c r="J12" s="192">
+      <c r="J12" s="276">
         <v>113</v>
       </c>
-      <c r="K12" s="192">
+      <c r="K12" s="276">
         <v>112</v>
       </c>
-      <c r="L12" s="192">
+      <c r="L12" s="276">
         <v>111</v>
       </c>
-      <c r="M12" s="192">
+      <c r="M12" s="276">
         <v>110</v>
       </c>
-      <c r="N12" s="192">
+      <c r="N12" s="276">
         <v>109</v>
       </c>
-      <c r="O12" s="192">
+      <c r="O12" s="276">
         <v>108</v>
       </c>
-      <c r="P12" s="192">
+      <c r="P12" s="276">
         <v>107</v>
       </c>
-      <c r="Q12" s="192">
+      <c r="Q12" s="276">
         <v>106</v>
       </c>
-      <c r="R12" s="192">
+      <c r="R12" s="276">
         <v>105</v>
       </c>
-      <c r="S12" s="192">
+      <c r="S12" s="276">
         <v>104</v>
       </c>
-      <c r="T12" s="192">
+      <c r="T12" s="276">
         <v>103</v>
       </c>
-      <c r="U12" s="192">
+      <c r="U12" s="276">
         <v>102</v>
       </c>
-      <c r="V12" s="192">
+      <c r="V12" s="276">
         <v>101</v>
       </c>
       <c r="W12" s="183"/>
-      <c r="X12" s="192">
+      <c r="X12" s="276">
         <v>101</v>
       </c>
-      <c r="Y12" s="192" t="s">
+      <c r="Y12" s="276" t="s">
         <v>106</v>
       </c>
-      <c r="Z12" s="192">
+      <c r="Z12" s="276">
         <v>102</v>
       </c>
-      <c r="AA12" s="192" t="s">
+      <c r="AA12" s="276" t="s">
         <v>105</v>
       </c>
-      <c r="AB12" s="192">
+      <c r="AB12" s="276">
         <v>103</v>
       </c>
-      <c r="AC12" s="192" t="s">
+      <c r="AC12" s="276" t="s">
         <v>104</v>
       </c>
-      <c r="AD12" s="192">
+      <c r="AD12" s="276">
         <v>104</v>
       </c>
-      <c r="AE12" s="192" t="s">
+      <c r="AE12" s="276" t="s">
         <v>103</v>
       </c>
-      <c r="AF12" s="192">
+      <c r="AF12" s="276">
         <v>105</v>
       </c>
-      <c r="AG12" s="192" t="s">
+      <c r="AG12" s="276" t="s">
         <v>144</v>
       </c>
-      <c r="AH12" s="192">
+      <c r="AH12" s="276">
         <v>106</v>
       </c>
-      <c r="AI12" s="192" t="s">
+      <c r="AI12" s="276" t="s">
         <v>143</v>
       </c>
-      <c r="AJ12" s="192">
+      <c r="AJ12" s="276">
         <v>107</v>
       </c>
-      <c r="AK12" s="192" t="s">
+      <c r="AK12" s="276" t="s">
         <v>142</v>
       </c>
-      <c r="AL12" s="192">
+      <c r="AL12" s="276">
         <v>108</v>
       </c>
-      <c r="AM12" s="192" t="s">
+      <c r="AM12" s="276" t="s">
         <v>141</v>
       </c>
-      <c r="AN12" s="192">
+      <c r="AN12" s="276">
         <v>109</v>
       </c>
-      <c r="AO12" s="192" t="s">
+      <c r="AO12" s="276" t="s">
         <v>140</v>
       </c>
-      <c r="AP12" s="192">
+      <c r="AP12" s="276">
         <v>110</v>
       </c>
-      <c r="AQ12" s="192" t="s">
+      <c r="AQ12" s="276" t="s">
         <v>139</v>
       </c>
       <c r="AR12" s="119"/>
@@ -5304,125 +5304,125 @@
         <v>7</v>
       </c>
       <c r="B13" s="119"/>
-      <c r="C13" s="192">
+      <c r="C13" s="276">
         <v>140</v>
       </c>
-      <c r="D13" s="192">
+      <c r="D13" s="276">
         <v>139</v>
       </c>
-      <c r="E13" s="192">
+      <c r="E13" s="276">
         <v>138</v>
       </c>
-      <c r="F13" s="192">
+      <c r="F13" s="276">
         <v>137</v>
       </c>
-      <c r="G13" s="192">
+      <c r="G13" s="276">
         <v>136</v>
       </c>
-      <c r="H13" s="192">
+      <c r="H13" s="276">
         <v>135</v>
       </c>
-      <c r="I13" s="192">
+      <c r="I13" s="276">
         <v>134</v>
       </c>
-      <c r="J13" s="192">
+      <c r="J13" s="276">
         <v>133</v>
       </c>
-      <c r="K13" s="192">
+      <c r="K13" s="276">
         <v>132</v>
       </c>
-      <c r="L13" s="192">
+      <c r="L13" s="276">
         <v>131</v>
       </c>
-      <c r="M13" s="192">
+      <c r="M13" s="276">
         <v>130</v>
       </c>
-      <c r="N13" s="192">
+      <c r="N13" s="276">
         <v>129</v>
       </c>
-      <c r="O13" s="192">
+      <c r="O13" s="276">
         <v>128</v>
       </c>
-      <c r="P13" s="192">
+      <c r="P13" s="276">
         <v>127</v>
       </c>
-      <c r="Q13" s="192">
+      <c r="Q13" s="276">
         <v>126</v>
       </c>
-      <c r="R13" s="192">
+      <c r="R13" s="276">
         <v>125</v>
       </c>
-      <c r="S13" s="192">
+      <c r="S13" s="276">
         <v>124</v>
       </c>
-      <c r="T13" s="192">
+      <c r="T13" s="276">
         <v>123</v>
       </c>
-      <c r="U13" s="192">
+      <c r="U13" s="276">
         <v>122</v>
       </c>
-      <c r="V13" s="192">
+      <c r="V13" s="276">
         <v>121</v>
       </c>
       <c r="W13" s="137"/>
-      <c r="X13" s="192">
+      <c r="X13" s="276">
         <v>121</v>
       </c>
-      <c r="Y13" s="192">
+      <c r="Y13" s="276">
         <v>122</v>
       </c>
-      <c r="Z13" s="192">
+      <c r="Z13" s="276">
         <v>123</v>
       </c>
-      <c r="AA13" s="192">
+      <c r="AA13" s="276">
         <v>124</v>
       </c>
-      <c r="AB13" s="192">
+      <c r="AB13" s="276">
         <v>125</v>
       </c>
-      <c r="AC13" s="192">
+      <c r="AC13" s="276">
         <v>126</v>
       </c>
-      <c r="AD13" s="192">
+      <c r="AD13" s="276">
         <v>127</v>
       </c>
-      <c r="AE13" s="192">
+      <c r="AE13" s="276">
         <v>128</v>
       </c>
-      <c r="AF13" s="192">
+      <c r="AF13" s="276">
         <v>129</v>
       </c>
-      <c r="AG13" s="192">
+      <c r="AG13" s="276">
         <v>130</v>
       </c>
-      <c r="AH13" s="192">
+      <c r="AH13" s="276">
         <v>131</v>
       </c>
-      <c r="AI13" s="192">
+      <c r="AI13" s="276">
         <v>132</v>
       </c>
-      <c r="AJ13" s="192">
+      <c r="AJ13" s="276">
         <v>133</v>
       </c>
-      <c r="AK13" s="192">
+      <c r="AK13" s="276">
         <v>134</v>
       </c>
-      <c r="AL13" s="192">
+      <c r="AL13" s="276">
         <v>135</v>
       </c>
-      <c r="AM13" s="192">
+      <c r="AM13" s="276">
         <v>136</v>
       </c>
-      <c r="AN13" s="192">
+      <c r="AN13" s="276">
         <v>137</v>
       </c>
-      <c r="AO13" s="192">
+      <c r="AO13" s="276">
         <v>138</v>
       </c>
-      <c r="AP13" s="192">
+      <c r="AP13" s="276">
         <v>139</v>
       </c>
-      <c r="AQ13" s="192">
+      <c r="AQ13" s="276">
         <v>140</v>
       </c>
       <c r="AR13" s="119"/>
@@ -5436,125 +5436,125 @@
         <v>8</v>
       </c>
       <c r="B14" s="119"/>
-      <c r="C14" s="192">
+      <c r="C14" s="276">
         <v>160</v>
       </c>
-      <c r="D14" s="192">
+      <c r="D14" s="276">
         <v>159</v>
       </c>
-      <c r="E14" s="192">
+      <c r="E14" s="276">
         <v>158</v>
       </c>
-      <c r="F14" s="192">
+      <c r="F14" s="276">
         <v>157</v>
       </c>
-      <c r="G14" s="192">
+      <c r="G14" s="276">
         <v>156</v>
       </c>
-      <c r="H14" s="192">
+      <c r="H14" s="276">
         <v>155</v>
       </c>
-      <c r="I14" s="192">
+      <c r="I14" s="276">
         <v>154</v>
       </c>
-      <c r="J14" s="192">
+      <c r="J14" s="276">
         <v>153</v>
       </c>
-      <c r="K14" s="192">
+      <c r="K14" s="276">
         <v>152</v>
       </c>
-      <c r="L14" s="192">
+      <c r="L14" s="276">
         <v>151</v>
       </c>
-      <c r="M14" s="192">
+      <c r="M14" s="276">
         <v>150</v>
       </c>
-      <c r="N14" s="192">
+      <c r="N14" s="276">
         <v>149</v>
       </c>
-      <c r="O14" s="192">
+      <c r="O14" s="276">
         <v>148</v>
       </c>
-      <c r="P14" s="192">
+      <c r="P14" s="276">
         <v>147</v>
       </c>
-      <c r="Q14" s="192">
+      <c r="Q14" s="276">
         <v>146</v>
       </c>
-      <c r="R14" s="192">
+      <c r="R14" s="276">
         <v>145</v>
       </c>
-      <c r="S14" s="192">
+      <c r="S14" s="276">
         <v>144</v>
       </c>
-      <c r="T14" s="192">
+      <c r="T14" s="276">
         <v>143</v>
       </c>
-      <c r="U14" s="192">
+      <c r="U14" s="276">
         <v>142</v>
       </c>
-      <c r="V14" s="192">
+      <c r="V14" s="276">
         <v>141</v>
       </c>
       <c r="W14" s="137"/>
-      <c r="X14" s="192" t="s">
+      <c r="X14" s="276" t="s">
         <v>153</v>
       </c>
-      <c r="Y14" s="192" t="s">
+      <c r="Y14" s="276" t="s">
         <v>152</v>
       </c>
-      <c r="Z14" s="192" t="s">
+      <c r="Z14" s="276" t="s">
         <v>151</v>
       </c>
-      <c r="AA14" s="192" t="s">
+      <c r="AA14" s="276" t="s">
         <v>150</v>
       </c>
-      <c r="AB14" s="192" t="s">
+      <c r="AB14" s="276" t="s">
         <v>149</v>
       </c>
-      <c r="AC14" s="192" t="s">
+      <c r="AC14" s="276" t="s">
         <v>148</v>
       </c>
-      <c r="AD14" s="192" t="s">
+      <c r="AD14" s="276" t="s">
         <v>147</v>
       </c>
-      <c r="AE14" s="192" t="s">
+      <c r="AE14" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="AF14" s="192" t="s">
+      <c r="AF14" s="276" t="s">
         <v>187</v>
       </c>
-      <c r="AG14" s="192" t="s">
+      <c r="AG14" s="276" t="s">
         <v>186</v>
       </c>
-      <c r="AH14" s="192" t="s">
+      <c r="AH14" s="276" t="s">
         <v>185</v>
       </c>
-      <c r="AI14" s="192" t="s">
+      <c r="AI14" s="276" t="s">
         <v>184</v>
       </c>
-      <c r="AJ14" s="192" t="s">
+      <c r="AJ14" s="276" t="s">
         <v>183</v>
       </c>
-      <c r="AK14" s="192" t="s">
+      <c r="AK14" s="276" t="s">
         <v>182</v>
       </c>
-      <c r="AL14" s="192" t="s">
+      <c r="AL14" s="276" t="s">
         <v>181</v>
       </c>
-      <c r="AM14" s="192" t="s">
+      <c r="AM14" s="276" t="s">
         <v>180</v>
       </c>
-      <c r="AN14" s="192" t="s">
+      <c r="AN14" s="276" t="s">
         <v>179</v>
       </c>
-      <c r="AO14" s="192" t="s">
+      <c r="AO14" s="276" t="s">
         <v>178</v>
       </c>
-      <c r="AP14" s="192" t="s">
+      <c r="AP14" s="276" t="s">
         <v>177</v>
       </c>
-      <c r="AQ14" s="192" t="s">
+      <c r="AQ14" s="276" t="s">
         <v>176</v>
       </c>
       <c r="AR14" s="119"/>
@@ -5568,125 +5568,125 @@
         <v>9</v>
       </c>
       <c r="B15" s="119"/>
-      <c r="C15" s="192" t="s">
+      <c r="C15" s="276" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="192" t="s">
+      <c r="D15" s="276" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="192" t="s">
+      <c r="E15" s="276" t="s">
         <v>200</v>
       </c>
-      <c r="F15" s="192" t="s">
+      <c r="F15" s="276" t="s">
         <v>201</v>
       </c>
-      <c r="G15" s="192" t="s">
+      <c r="G15" s="276" t="s">
         <v>202</v>
       </c>
-      <c r="H15" s="192" t="s">
+      <c r="H15" s="276" t="s">
         <v>203</v>
       </c>
-      <c r="I15" s="192" t="s">
+      <c r="I15" s="276" t="s">
         <v>204</v>
       </c>
-      <c r="J15" s="192" t="s">
+      <c r="J15" s="276" t="s">
         <v>205</v>
       </c>
-      <c r="K15" s="192" t="s">
+      <c r="K15" s="276" t="s">
         <v>206</v>
       </c>
-      <c r="L15" s="192" t="s">
+      <c r="L15" s="276" t="s">
         <v>207</v>
       </c>
-      <c r="M15" s="192" t="s">
+      <c r="M15" s="276" t="s">
         <v>208</v>
       </c>
-      <c r="N15" s="192" t="s">
+      <c r="N15" s="276" t="s">
         <v>209</v>
       </c>
-      <c r="O15" s="192" t="s">
+      <c r="O15" s="276" t="s">
         <v>168</v>
       </c>
-      <c r="P15" s="192" t="s">
+      <c r="P15" s="276" t="s">
         <v>169</v>
       </c>
-      <c r="Q15" s="192" t="s">
+      <c r="Q15" s="276" t="s">
         <v>170</v>
       </c>
-      <c r="R15" s="192" t="s">
+      <c r="R15" s="276" t="s">
         <v>171</v>
       </c>
-      <c r="S15" s="192" t="s">
+      <c r="S15" s="276" t="s">
         <v>172</v>
       </c>
-      <c r="T15" s="192" t="s">
+      <c r="T15" s="276" t="s">
         <v>173</v>
       </c>
-      <c r="U15" s="192" t="s">
+      <c r="U15" s="276" t="s">
         <v>174</v>
       </c>
-      <c r="V15" s="192" t="s">
+      <c r="V15" s="276" t="s">
         <v>175</v>
       </c>
       <c r="W15" s="137"/>
-      <c r="X15" s="192" t="s">
+      <c r="X15" s="276" t="s">
         <v>175</v>
       </c>
-      <c r="Y15" s="192" t="s">
+      <c r="Y15" s="276" t="s">
         <v>174</v>
       </c>
-      <c r="Z15" s="192" t="s">
+      <c r="Z15" s="276" t="s">
         <v>173</v>
       </c>
-      <c r="AA15" s="192" t="s">
+      <c r="AA15" s="276" t="s">
         <v>172</v>
       </c>
-      <c r="AB15" s="192" t="s">
+      <c r="AB15" s="276" t="s">
         <v>171</v>
       </c>
-      <c r="AC15" s="192" t="s">
+      <c r="AC15" s="276" t="s">
         <v>170</v>
       </c>
-      <c r="AD15" s="192" t="s">
+      <c r="AD15" s="276" t="s">
         <v>169</v>
       </c>
-      <c r="AE15" s="192" t="s">
+      <c r="AE15" s="276" t="s">
         <v>168</v>
       </c>
-      <c r="AF15" s="192" t="s">
+      <c r="AF15" s="276" t="s">
         <v>209</v>
       </c>
-      <c r="AG15" s="192" t="s">
+      <c r="AG15" s="276" t="s">
         <v>208</v>
       </c>
-      <c r="AH15" s="192" t="s">
+      <c r="AH15" s="276" t="s">
         <v>207</v>
       </c>
-      <c r="AI15" s="192" t="s">
+      <c r="AI15" s="276" t="s">
         <v>206</v>
       </c>
-      <c r="AJ15" s="192" t="s">
+      <c r="AJ15" s="276" t="s">
         <v>205</v>
       </c>
-      <c r="AK15" s="192" t="s">
+      <c r="AK15" s="276" t="s">
         <v>204</v>
       </c>
-      <c r="AL15" s="192" t="s">
+      <c r="AL15" s="276" t="s">
         <v>203</v>
       </c>
-      <c r="AM15" s="192" t="s">
+      <c r="AM15" s="276" t="s">
         <v>202</v>
       </c>
-      <c r="AN15" s="192" t="s">
+      <c r="AN15" s="276" t="s">
         <v>201</v>
       </c>
-      <c r="AO15" s="192" t="s">
+      <c r="AO15" s="276" t="s">
         <v>200</v>
       </c>
-      <c r="AP15" s="192" t="s">
+      <c r="AP15" s="276" t="s">
         <v>199</v>
       </c>
-      <c r="AQ15" s="192" t="s">
+      <c r="AQ15" s="276" t="s">
         <v>198</v>
       </c>
       <c r="AR15" s="123"/>
@@ -5700,125 +5700,125 @@
         <v>10</v>
       </c>
       <c r="B16" s="124"/>
-      <c r="C16" s="192">
+      <c r="C16" s="276">
         <v>200</v>
       </c>
-      <c r="D16" s="192">
+      <c r="D16" s="276">
         <v>199</v>
       </c>
-      <c r="E16" s="192" t="s">
+      <c r="E16" s="276" t="s">
         <v>224</v>
       </c>
-      <c r="F16" s="192" t="s">
+      <c r="F16" s="276" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="192" t="s">
+      <c r="G16" s="276" t="s">
         <v>226</v>
       </c>
-      <c r="H16" s="192" t="s">
+      <c r="H16" s="276" t="s">
         <v>227</v>
       </c>
-      <c r="I16" s="192" t="s">
+      <c r="I16" s="276" t="s">
         <v>228</v>
       </c>
-      <c r="J16" s="192" t="s">
+      <c r="J16" s="276" t="s">
         <v>229</v>
       </c>
-      <c r="K16" s="192" t="s">
+      <c r="K16" s="276" t="s">
         <v>230</v>
       </c>
-      <c r="L16" s="192" t="s">
+      <c r="L16" s="276" t="s">
         <v>231</v>
       </c>
-      <c r="M16" s="192" t="s">
+      <c r="M16" s="276" t="s">
         <v>232</v>
       </c>
-      <c r="N16" s="192" t="s">
+      <c r="N16" s="276" t="s">
         <v>189</v>
       </c>
-      <c r="O16" s="192" t="s">
+      <c r="O16" s="276" t="s">
         <v>190</v>
       </c>
-      <c r="P16" s="192" t="s">
+      <c r="P16" s="276" t="s">
         <v>191</v>
       </c>
-      <c r="Q16" s="192" t="s">
+      <c r="Q16" s="276" t="s">
         <v>192</v>
       </c>
-      <c r="R16" s="192" t="s">
+      <c r="R16" s="276" t="s">
         <v>193</v>
       </c>
-      <c r="S16" s="192" t="s">
+      <c r="S16" s="276" t="s">
         <v>194</v>
       </c>
-      <c r="T16" s="192" t="s">
+      <c r="T16" s="276" t="s">
         <v>195</v>
       </c>
-      <c r="U16" s="192" t="s">
+      <c r="U16" s="276" t="s">
         <v>196</v>
       </c>
-      <c r="V16" s="192" t="s">
+      <c r="V16" s="276" t="s">
         <v>197</v>
       </c>
       <c r="W16" s="150"/>
-      <c r="X16" s="192">
+      <c r="X16" s="276">
         <v>181</v>
       </c>
-      <c r="Y16" s="192">
+      <c r="Y16" s="276">
         <v>182</v>
       </c>
-      <c r="Z16" s="192">
+      <c r="Z16" s="276">
         <v>183</v>
       </c>
-      <c r="AA16" s="192">
+      <c r="AA16" s="276">
         <v>184</v>
       </c>
-      <c r="AB16" s="192">
+      <c r="AB16" s="276">
         <v>185</v>
       </c>
-      <c r="AC16" s="192">
+      <c r="AC16" s="276">
         <v>186</v>
       </c>
-      <c r="AD16" s="192">
+      <c r="AD16" s="276">
         <v>187</v>
       </c>
-      <c r="AE16" s="192">
+      <c r="AE16" s="276">
         <v>188</v>
       </c>
-      <c r="AF16" s="192">
+      <c r="AF16" s="276">
         <v>189</v>
       </c>
-      <c r="AG16" s="192">
+      <c r="AG16" s="276">
         <v>190</v>
       </c>
-      <c r="AH16" s="192">
+      <c r="AH16" s="276">
         <v>191</v>
       </c>
-      <c r="AI16" s="192">
+      <c r="AI16" s="276">
         <v>192</v>
       </c>
-      <c r="AJ16" s="192">
+      <c r="AJ16" s="276">
         <v>193</v>
       </c>
-      <c r="AK16" s="192">
+      <c r="AK16" s="276">
         <v>194</v>
       </c>
-      <c r="AL16" s="192">
+      <c r="AL16" s="276">
         <v>195</v>
       </c>
-      <c r="AM16" s="192">
+      <c r="AM16" s="276">
         <v>196</v>
       </c>
-      <c r="AN16" s="192">
+      <c r="AN16" s="276">
         <v>197</v>
       </c>
-      <c r="AO16" s="192">
+      <c r="AO16" s="276">
         <v>198</v>
       </c>
-      <c r="AP16" s="192">
+      <c r="AP16" s="276">
         <v>199</v>
       </c>
-      <c r="AQ16" s="192">
+      <c r="AQ16" s="276">
         <v>200</v>
       </c>
       <c r="AR16" s="119"/>
@@ -5832,125 +5832,125 @@
         <v>11</v>
       </c>
       <c r="B17" s="119"/>
-      <c r="C17" s="192">
+      <c r="C17" s="276">
         <v>220</v>
       </c>
-      <c r="D17" s="192">
+      <c r="D17" s="276">
         <v>219</v>
       </c>
-      <c r="E17" s="192">
+      <c r="E17" s="276">
         <v>218</v>
       </c>
-      <c r="F17" s="192">
+      <c r="F17" s="276">
         <v>217</v>
       </c>
-      <c r="G17" s="192">
+      <c r="G17" s="276">
         <v>216</v>
       </c>
-      <c r="H17" s="192">
+      <c r="H17" s="276">
         <v>215</v>
       </c>
-      <c r="I17" s="192">
+      <c r="I17" s="276">
         <v>214</v>
       </c>
-      <c r="J17" s="192">
+      <c r="J17" s="276">
         <v>213</v>
       </c>
-      <c r="K17" s="192">
+      <c r="K17" s="276">
         <v>212</v>
       </c>
-      <c r="L17" s="192">
+      <c r="L17" s="276">
         <v>211</v>
       </c>
-      <c r="M17" s="192">
+      <c r="M17" s="276">
         <v>210</v>
       </c>
-      <c r="N17" s="192">
+      <c r="N17" s="276">
         <v>209</v>
       </c>
-      <c r="O17" s="192">
+      <c r="O17" s="276">
         <v>208</v>
       </c>
-      <c r="P17" s="192">
+      <c r="P17" s="276">
         <v>207</v>
       </c>
-      <c r="Q17" s="192">
+      <c r="Q17" s="276">
         <v>206</v>
       </c>
-      <c r="R17" s="192">
+      <c r="R17" s="276">
         <v>205</v>
       </c>
-      <c r="S17" s="192">
+      <c r="S17" s="276">
         <v>204</v>
       </c>
-      <c r="T17" s="192">
+      <c r="T17" s="276">
         <v>203</v>
       </c>
-      <c r="U17" s="192">
+      <c r="U17" s="276">
         <v>202</v>
       </c>
-      <c r="V17" s="192">
+      <c r="V17" s="276">
         <v>201</v>
       </c>
       <c r="W17" s="137"/>
-      <c r="X17" s="192" t="s">
+      <c r="X17" s="276" t="s">
         <v>221</v>
       </c>
-      <c r="Y17" s="192" t="s">
+      <c r="Y17" s="276" t="s">
         <v>220</v>
       </c>
-      <c r="Z17" s="192" t="s">
+      <c r="Z17" s="276" t="s">
         <v>219</v>
       </c>
-      <c r="AA17" s="192" t="s">
+      <c r="AA17" s="276" t="s">
         <v>218</v>
       </c>
-      <c r="AB17" s="192" t="s">
+      <c r="AB17" s="276" t="s">
         <v>217</v>
       </c>
-      <c r="AC17" s="192" t="s">
+      <c r="AC17" s="276" t="s">
         <v>216</v>
       </c>
-      <c r="AD17" s="192" t="s">
+      <c r="AD17" s="276" t="s">
         <v>215</v>
       </c>
-      <c r="AE17" s="192" t="s">
+      <c r="AE17" s="276" t="s">
         <v>214</v>
       </c>
-      <c r="AF17" s="192" t="s">
+      <c r="AF17" s="276" t="s">
         <v>213</v>
       </c>
-      <c r="AG17" s="192" t="s">
+      <c r="AG17" s="276" t="s">
         <v>212</v>
       </c>
-      <c r="AH17" s="192" t="s">
+      <c r="AH17" s="276" t="s">
         <v>250</v>
       </c>
-      <c r="AI17" s="192" t="s">
+      <c r="AI17" s="276" t="s">
         <v>249</v>
       </c>
-      <c r="AJ17" s="192" t="s">
+      <c r="AJ17" s="276" t="s">
         <v>248</v>
       </c>
-      <c r="AK17" s="192" t="s">
+      <c r="AK17" s="276" t="s">
         <v>247</v>
       </c>
-      <c r="AL17" s="192" t="s">
+      <c r="AL17" s="276" t="s">
         <v>246</v>
       </c>
-      <c r="AM17" s="192" t="s">
+      <c r="AM17" s="276" t="s">
         <v>245</v>
       </c>
-      <c r="AN17" s="192" t="s">
+      <c r="AN17" s="276" t="s">
         <v>244</v>
       </c>
-      <c r="AO17" s="192" t="s">
+      <c r="AO17" s="276" t="s">
         <v>243</v>
       </c>
-      <c r="AP17" s="192" t="s">
+      <c r="AP17" s="276" t="s">
         <v>242</v>
       </c>
-      <c r="AQ17" s="192" t="s">
+      <c r="AQ17" s="276" t="s">
         <v>241</v>
       </c>
       <c r="AR17" s="119"/>
@@ -5964,128 +5964,128 @@
         <v>12</v>
       </c>
       <c r="B18" s="119"/>
-      <c r="C18" s="192">
+      <c r="C18" s="276">
         <v>240</v>
       </c>
-      <c r="D18" s="192">
+      <c r="D18" s="276">
         <v>239</v>
       </c>
-      <c r="E18" s="192">
+      <c r="E18" s="276">
         <v>238</v>
       </c>
-      <c r="F18" s="192">
+      <c r="F18" s="276">
         <v>237</v>
       </c>
-      <c r="G18" s="192">
+      <c r="G18" s="276">
         <v>236</v>
       </c>
-      <c r="H18" s="192">
+      <c r="H18" s="276">
         <v>235</v>
       </c>
-      <c r="I18" s="192">
+      <c r="I18" s="276">
         <v>234</v>
       </c>
-      <c r="J18" s="192">
+      <c r="J18" s="276">
         <v>233</v>
       </c>
-      <c r="K18" s="192">
+      <c r="K18" s="276">
         <v>232</v>
       </c>
-      <c r="L18" s="192">
+      <c r="L18" s="276">
         <v>231</v>
       </c>
-      <c r="M18" s="192">
+      <c r="M18" s="276">
         <v>230</v>
       </c>
-      <c r="N18" s="192">
+      <c r="N18" s="276">
         <v>229</v>
       </c>
-      <c r="O18" s="192">
+      <c r="O18" s="276">
         <v>228</v>
       </c>
-      <c r="P18" s="192">
+      <c r="P18" s="276">
         <v>227</v>
       </c>
-      <c r="Q18" s="192">
+      <c r="Q18" s="276">
         <v>226</v>
       </c>
-      <c r="R18" s="192">
+      <c r="R18" s="276">
         <v>225</v>
       </c>
-      <c r="S18" s="192">
+      <c r="S18" s="276">
         <v>224</v>
       </c>
-      <c r="T18" s="192">
+      <c r="T18" s="276">
         <v>223</v>
       </c>
-      <c r="U18" s="192">
+      <c r="U18" s="276">
         <v>222</v>
       </c>
-      <c r="V18" s="192">
+      <c r="V18" s="276">
         <v>221</v>
       </c>
       <c r="W18" s="137"/>
-      <c r="X18" s="192" t="s">
+      <c r="X18" s="276" t="s">
         <v>240</v>
       </c>
-      <c r="Y18" s="192" t="s">
+      <c r="Y18" s="276" t="s">
         <v>239</v>
       </c>
-      <c r="Z18" s="192" t="s">
+      <c r="Z18" s="276" t="s">
         <v>238</v>
       </c>
-      <c r="AA18" s="192" t="s">
+      <c r="AA18" s="276" t="s">
         <v>237</v>
       </c>
-      <c r="AB18" s="192" t="s">
+      <c r="AB18" s="276" t="s">
         <v>251</v>
       </c>
-      <c r="AC18" s="192" t="s">
+      <c r="AC18" s="276" t="s">
         <v>252</v>
       </c>
-      <c r="AD18" s="192" t="s">
+      <c r="AD18" s="276" t="s">
         <v>253</v>
       </c>
-      <c r="AE18" s="192" t="s">
+      <c r="AE18" s="276" t="s">
         <v>236</v>
       </c>
-      <c r="AF18" s="192" t="s">
+      <c r="AF18" s="276" t="s">
         <v>235</v>
       </c>
-      <c r="AG18" s="192" t="s">
+      <c r="AG18" s="276" t="s">
         <v>234</v>
       </c>
-      <c r="AH18" s="192" t="s">
+      <c r="AH18" s="276" t="s">
         <v>233</v>
       </c>
-      <c r="AI18" s="192" t="s">
+      <c r="AI18" s="276" t="s">
         <v>276</v>
       </c>
-      <c r="AJ18" s="192" t="s">
+      <c r="AJ18" s="276" t="s">
         <v>275</v>
       </c>
-      <c r="AK18" s="192" t="s">
+      <c r="AK18" s="276" t="s">
         <v>274</v>
       </c>
-      <c r="AL18" s="192" t="s">
+      <c r="AL18" s="276" t="s">
         <v>273</v>
       </c>
-      <c r="AM18" s="192" t="s">
+      <c r="AM18" s="276" t="s">
         <v>272</v>
       </c>
-      <c r="AN18" s="192" t="s">
+      <c r="AN18" s="276" t="s">
         <v>271</v>
       </c>
-      <c r="AO18" s="192" t="s">
+      <c r="AO18" s="276" t="s">
         <v>270</v>
       </c>
-      <c r="AP18" s="192" t="s">
+      <c r="AP18" s="276" t="s">
         <v>269</v>
       </c>
-      <c r="AQ18" s="280" t="s">
+      <c r="AQ18" s="278" t="s">
         <v>268</v>
       </c>
-      <c r="AR18" s="279" t="s">
+      <c r="AR18" s="265" t="s">
         <v>779</v>
       </c>
       <c r="AS18" s="51">
@@ -6098,125 +6098,125 @@
         <v>13</v>
       </c>
       <c r="B19" s="119"/>
-      <c r="C19" s="192">
+      <c r="C19" s="276">
         <v>260</v>
       </c>
-      <c r="D19" s="192">
+      <c r="D19" s="276">
         <v>259</v>
       </c>
-      <c r="E19" s="192">
+      <c r="E19" s="276">
         <v>258</v>
       </c>
-      <c r="F19" s="192">
+      <c r="F19" s="276">
         <v>257</v>
       </c>
-      <c r="G19" s="192">
+      <c r="G19" s="276">
         <v>256</v>
       </c>
-      <c r="H19" s="192">
+      <c r="H19" s="276">
         <v>255</v>
       </c>
-      <c r="I19" s="192">
+      <c r="I19" s="276">
         <v>254</v>
       </c>
-      <c r="J19" s="192">
+      <c r="J19" s="276">
         <v>253</v>
       </c>
-      <c r="K19" s="192">
+      <c r="K19" s="276">
         <v>252</v>
       </c>
-      <c r="L19" s="192">
+      <c r="L19" s="276">
         <v>251</v>
       </c>
-      <c r="M19" s="192">
+      <c r="M19" s="276">
         <v>250</v>
       </c>
-      <c r="N19" s="192">
+      <c r="N19" s="276">
         <v>249</v>
       </c>
-      <c r="O19" s="192">
+      <c r="O19" s="276">
         <v>248</v>
       </c>
-      <c r="P19" s="192">
+      <c r="P19" s="276">
         <v>247</v>
       </c>
-      <c r="Q19" s="192">
+      <c r="Q19" s="276">
         <v>246</v>
       </c>
-      <c r="R19" s="192">
+      <c r="R19" s="276">
         <v>245</v>
       </c>
-      <c r="S19" s="192">
+      <c r="S19" s="276">
         <v>244</v>
       </c>
-      <c r="T19" s="192">
+      <c r="T19" s="276">
         <v>243</v>
       </c>
-      <c r="U19" s="192">
+      <c r="U19" s="276">
         <v>242</v>
       </c>
-      <c r="V19" s="192">
+      <c r="V19" s="276">
         <v>241</v>
       </c>
       <c r="W19" s="137"/>
-      <c r="X19" s="192">
+      <c r="X19" s="276">
         <v>241</v>
       </c>
-      <c r="Y19" s="192">
+      <c r="Y19" s="276">
         <v>242</v>
       </c>
-      <c r="Z19" s="192">
+      <c r="Z19" s="276">
         <v>243</v>
       </c>
-      <c r="AA19" s="192">
+      <c r="AA19" s="276">
         <v>244</v>
       </c>
-      <c r="AB19" s="192">
+      <c r="AB19" s="276">
         <v>245</v>
       </c>
-      <c r="AC19" s="192">
+      <c r="AC19" s="276">
         <v>246</v>
       </c>
-      <c r="AD19" s="192">
+      <c r="AD19" s="276">
         <v>247</v>
       </c>
-      <c r="AE19" s="192">
+      <c r="AE19" s="276">
         <v>248</v>
       </c>
-      <c r="AF19" s="192">
+      <c r="AF19" s="276">
         <v>249</v>
       </c>
-      <c r="AG19" s="192">
+      <c r="AG19" s="276">
         <v>250</v>
       </c>
-      <c r="AH19" s="192">
+      <c r="AH19" s="276">
         <v>251</v>
       </c>
-      <c r="AI19" s="192">
+      <c r="AI19" s="276">
         <v>252</v>
       </c>
-      <c r="AJ19" s="192">
+      <c r="AJ19" s="276">
         <v>253</v>
       </c>
-      <c r="AK19" s="192">
+      <c r="AK19" s="276">
         <v>254</v>
       </c>
-      <c r="AL19" s="192">
+      <c r="AL19" s="276">
         <v>255</v>
       </c>
-      <c r="AM19" s="192">
+      <c r="AM19" s="276">
         <v>256</v>
       </c>
-      <c r="AN19" s="192">
+      <c r="AN19" s="276">
         <v>257</v>
       </c>
-      <c r="AO19" s="192">
+      <c r="AO19" s="276">
         <v>258</v>
       </c>
-      <c r="AP19" s="192">
+      <c r="AP19" s="276">
         <v>259</v>
       </c>
-      <c r="AQ19" s="192">
+      <c r="AQ19" s="276">
         <v>260</v>
       </c>
       <c r="AR19" s="177" t="s">
@@ -6231,129 +6231,129 @@
       <c r="A20" s="133">
         <v>14</v>
       </c>
-      <c r="B20" s="196"/>
-      <c r="C20" s="192">
+      <c r="B20" s="195"/>
+      <c r="C20" s="276">
         <v>280</v>
       </c>
-      <c r="D20" s="192">
+      <c r="D20" s="276">
         <v>279</v>
       </c>
-      <c r="E20" s="192">
+      <c r="E20" s="276">
         <v>278</v>
       </c>
-      <c r="F20" s="192">
+      <c r="F20" s="276">
         <v>277</v>
       </c>
-      <c r="G20" s="192">
+      <c r="G20" s="276">
         <v>276</v>
       </c>
-      <c r="H20" s="192">
+      <c r="H20" s="276">
         <v>275</v>
       </c>
-      <c r="I20" s="192">
+      <c r="I20" s="276">
         <v>274</v>
       </c>
-      <c r="J20" s="192">
+      <c r="J20" s="276">
         <v>273</v>
       </c>
-      <c r="K20" s="192">
+      <c r="K20" s="276">
         <v>272</v>
       </c>
-      <c r="L20" s="192">
+      <c r="L20" s="276">
         <v>271</v>
       </c>
-      <c r="M20" s="192">
+      <c r="M20" s="276">
         <v>270</v>
       </c>
-      <c r="N20" s="192">
+      <c r="N20" s="276">
         <v>269</v>
       </c>
-      <c r="O20" s="192">
+      <c r="O20" s="276">
         <v>268</v>
       </c>
-      <c r="P20" s="192">
+      <c r="P20" s="276">
         <v>267</v>
       </c>
-      <c r="Q20" s="192">
+      <c r="Q20" s="276">
         <v>266</v>
       </c>
-      <c r="R20" s="192">
+      <c r="R20" s="276">
         <v>265</v>
       </c>
-      <c r="S20" s="192">
+      <c r="S20" s="276">
         <v>264</v>
       </c>
-      <c r="T20" s="192">
+      <c r="T20" s="276">
         <v>263</v>
       </c>
-      <c r="U20" s="192">
+      <c r="U20" s="276">
         <v>262</v>
       </c>
-      <c r="V20" s="192">
+      <c r="V20" s="276">
         <v>261</v>
       </c>
       <c r="W20" s="151"/>
-      <c r="X20" s="192">
+      <c r="X20" s="276">
         <v>261</v>
       </c>
-      <c r="Y20" s="192">
+      <c r="Y20" s="276">
         <v>262</v>
       </c>
-      <c r="Z20" s="192">
+      <c r="Z20" s="276">
         <v>263</v>
       </c>
-      <c r="AA20" s="192">
+      <c r="AA20" s="276">
         <v>264</v>
       </c>
-      <c r="AB20" s="192">
+      <c r="AB20" s="276">
         <v>265</v>
       </c>
-      <c r="AC20" s="192">
+      <c r="AC20" s="276">
         <v>266</v>
       </c>
-      <c r="AD20" s="192">
+      <c r="AD20" s="276">
         <v>267</v>
       </c>
-      <c r="AE20" s="192">
+      <c r="AE20" s="276">
         <v>268</v>
       </c>
-      <c r="AF20" s="192">
+      <c r="AF20" s="276">
         <v>269</v>
       </c>
-      <c r="AG20" s="192">
+      <c r="AG20" s="276">
         <v>270</v>
       </c>
-      <c r="AH20" s="192">
+      <c r="AH20" s="276">
         <v>271</v>
       </c>
-      <c r="AI20" s="192">
+      <c r="AI20" s="276">
         <v>272</v>
       </c>
-      <c r="AJ20" s="192">
+      <c r="AJ20" s="276">
         <v>273</v>
       </c>
-      <c r="AK20" s="192">
+      <c r="AK20" s="276">
         <v>274</v>
       </c>
-      <c r="AL20" s="192">
+      <c r="AL20" s="276">
         <v>275</v>
       </c>
-      <c r="AM20" s="192">
+      <c r="AM20" s="276">
         <v>276</v>
       </c>
-      <c r="AN20" s="192">
+      <c r="AN20" s="276">
         <v>277</v>
       </c>
-      <c r="AO20" s="192">
+      <c r="AO20" s="276">
         <v>278</v>
       </c>
-      <c r="AP20" s="192">
+      <c r="AP20" s="276">
         <v>279</v>
       </c>
-      <c r="AQ20" s="192">
+      <c r="AQ20" s="276">
         <v>280</v>
       </c>
-      <c r="AR20" s="195" t="s">
+      <c r="AR20" s="194" t="s">
         <v>460</v>
       </c>
       <c r="AS20" s="51">
@@ -6366,125 +6366,125 @@
         <v>15</v>
       </c>
       <c r="B21" s="119"/>
-      <c r="C21" s="192">
+      <c r="C21" s="276">
         <v>300</v>
       </c>
-      <c r="D21" s="192">
+      <c r="D21" s="276">
         <v>299</v>
       </c>
-      <c r="E21" s="192">
+      <c r="E21" s="276">
         <v>298</v>
       </c>
-      <c r="F21" s="192">
+      <c r="F21" s="276">
         <v>297</v>
       </c>
-      <c r="G21" s="192">
+      <c r="G21" s="276">
         <v>296</v>
       </c>
-      <c r="H21" s="192">
+      <c r="H21" s="276">
         <v>295</v>
       </c>
-      <c r="I21" s="192">
+      <c r="I21" s="276">
         <v>294</v>
       </c>
-      <c r="J21" s="192">
+      <c r="J21" s="276">
         <v>293</v>
       </c>
-      <c r="K21" s="192">
+      <c r="K21" s="276">
         <v>292</v>
       </c>
-      <c r="L21" s="192">
+      <c r="L21" s="276">
         <v>291</v>
       </c>
-      <c r="M21" s="192">
+      <c r="M21" s="276">
         <v>290</v>
       </c>
-      <c r="N21" s="192">
+      <c r="N21" s="276">
         <v>289</v>
       </c>
-      <c r="O21" s="192">
+      <c r="O21" s="276">
         <v>288</v>
       </c>
-      <c r="P21" s="192">
+      <c r="P21" s="276">
         <v>287</v>
       </c>
-      <c r="Q21" s="192">
+      <c r="Q21" s="276">
         <v>286</v>
       </c>
-      <c r="R21" s="192">
+      <c r="R21" s="276">
         <v>285</v>
       </c>
-      <c r="S21" s="192">
+      <c r="S21" s="276">
         <v>284</v>
       </c>
-      <c r="T21" s="192">
+      <c r="T21" s="276">
         <v>283</v>
       </c>
-      <c r="U21" s="192">
+      <c r="U21" s="276">
         <v>282</v>
       </c>
-      <c r="V21" s="192">
+      <c r="V21" s="276">
         <v>281</v>
       </c>
       <c r="W21" s="118"/>
-      <c r="X21" s="192">
+      <c r="X21" s="276">
         <v>281</v>
       </c>
-      <c r="Y21" s="192">
+      <c r="Y21" s="276">
         <v>282</v>
       </c>
-      <c r="Z21" s="192">
+      <c r="Z21" s="276">
         <v>283</v>
       </c>
-      <c r="AA21" s="192">
+      <c r="AA21" s="276">
         <v>284</v>
       </c>
-      <c r="AB21" s="192">
+      <c r="AB21" s="276">
         <v>285</v>
       </c>
-      <c r="AC21" s="192">
+      <c r="AC21" s="276">
         <v>286</v>
       </c>
-      <c r="AD21" s="192">
+      <c r="AD21" s="276">
         <v>287</v>
       </c>
-      <c r="AE21" s="192">
+      <c r="AE21" s="276">
         <v>288</v>
       </c>
-      <c r="AF21" s="192">
+      <c r="AF21" s="276">
         <v>289</v>
       </c>
-      <c r="AG21" s="192">
+      <c r="AG21" s="276">
         <v>290</v>
       </c>
-      <c r="AH21" s="192">
+      <c r="AH21" s="276">
         <v>291</v>
       </c>
-      <c r="AI21" s="192">
+      <c r="AI21" s="276">
         <v>292</v>
       </c>
-      <c r="AJ21" s="192">
+      <c r="AJ21" s="276">
         <v>293</v>
       </c>
-      <c r="AK21" s="192">
+      <c r="AK21" s="276">
         <v>294</v>
       </c>
-      <c r="AL21" s="192">
+      <c r="AL21" s="276">
         <v>295</v>
       </c>
-      <c r="AM21" s="192">
+      <c r="AM21" s="276">
         <v>296</v>
       </c>
-      <c r="AN21" s="192">
+      <c r="AN21" s="276">
         <v>297</v>
       </c>
-      <c r="AO21" s="192">
+      <c r="AO21" s="276">
         <v>298</v>
       </c>
-      <c r="AP21" s="192">
+      <c r="AP21" s="276">
         <v>299</v>
       </c>
-      <c r="AQ21" s="192">
+      <c r="AQ21" s="276">
         <v>300</v>
       </c>
       <c r="AR21" s="119"/>
@@ -6507,11 +6507,11 @@
       <c r="K22" s="113"/>
       <c r="L22" s="113"/>
       <c r="M22" s="113"/>
-      <c r="N22" s="274" t="s">
+      <c r="N22" s="271" t="s">
         <v>575</v>
       </c>
-      <c r="O22" s="274"/>
-      <c r="P22" s="274"/>
+      <c r="O22" s="271"/>
+      <c r="P22" s="271"/>
       <c r="Q22" s="113"/>
       <c r="R22" s="113"/>
       <c r="S22" s="113"/>
@@ -6525,11 +6525,11 @@
       <c r="AA22" s="113"/>
       <c r="AB22" s="113"/>
       <c r="AC22" s="113"/>
-      <c r="AD22" s="274" t="s">
+      <c r="AD22" s="271" t="s">
         <v>575</v>
       </c>
-      <c r="AE22" s="274"/>
-      <c r="AF22" s="274"/>
+      <c r="AE22" s="271"/>
+      <c r="AF22" s="271"/>
       <c r="AG22" s="113"/>
       <c r="AH22" s="113"/>
       <c r="AI22" s="113"/>
@@ -6545,19 +6545,19 @@
       <c r="AS22" s="178"/>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A23" s="221"/>
-      <c r="B23" s="253"/>
-      <c r="C23" s="253"/>
-      <c r="D23" s="253"/>
-      <c r="E23" s="253"/>
-      <c r="F23" s="253"/>
-      <c r="G23" s="253"/>
-      <c r="H23" s="253"/>
-      <c r="I23" s="253"/>
-      <c r="J23" s="253"/>
-      <c r="K23" s="253"/>
-      <c r="L23" s="254"/>
-      <c r="M23" s="254"/>
+      <c r="A23" s="219"/>
+      <c r="B23" s="248"/>
+      <c r="C23" s="248"/>
+      <c r="D23" s="248"/>
+      <c r="E23" s="248"/>
+      <c r="F23" s="248"/>
+      <c r="G23" s="248"/>
+      <c r="H23" s="248"/>
+      <c r="I23" s="248"/>
+      <c r="J23" s="248"/>
+      <c r="K23" s="248"/>
+      <c r="L23" s="249"/>
+      <c r="M23" s="249"/>
       <c r="N23" s="154">
         <v>1</v>
       </c>
@@ -6601,34 +6601,34 @@
       <c r="AF23" s="156">
         <v>1</v>
       </c>
-      <c r="AG23" s="254"/>
-      <c r="AH23" s="254"/>
-      <c r="AI23" s="255"/>
-      <c r="AJ23" s="255"/>
-      <c r="AK23" s="255"/>
-      <c r="AL23" s="255"/>
-      <c r="AM23" s="255"/>
-      <c r="AN23" s="255"/>
-      <c r="AO23" s="255"/>
-      <c r="AP23" s="255"/>
-      <c r="AQ23" s="255"/>
-      <c r="AR23" s="255"/>
+      <c r="AG23" s="249"/>
+      <c r="AH23" s="249"/>
+      <c r="AI23" s="250"/>
+      <c r="AJ23" s="250"/>
+      <c r="AK23" s="250"/>
+      <c r="AL23" s="250"/>
+      <c r="AM23" s="250"/>
+      <c r="AN23" s="250"/>
+      <c r="AO23" s="250"/>
+      <c r="AP23" s="250"/>
+      <c r="AQ23" s="250"/>
+      <c r="AR23" s="250"/>
       <c r="AS23" s="178"/>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="123"/>
-      <c r="B24" s="255"/>
-      <c r="C24" s="255"/>
-      <c r="D24" s="255"/>
-      <c r="E24" s="255"/>
-      <c r="F24" s="255"/>
-      <c r="G24" s="255"/>
-      <c r="H24" s="255"/>
-      <c r="I24" s="255"/>
-      <c r="J24" s="255"/>
-      <c r="K24" s="255"/>
-      <c r="L24" s="254"/>
-      <c r="M24" s="254"/>
+      <c r="B24" s="250"/>
+      <c r="C24" s="250"/>
+      <c r="D24" s="250"/>
+      <c r="E24" s="250"/>
+      <c r="F24" s="250"/>
+      <c r="G24" s="250"/>
+      <c r="H24" s="250"/>
+      <c r="I24" s="250"/>
+      <c r="J24" s="250"/>
+      <c r="K24" s="250"/>
+      <c r="L24" s="249"/>
+      <c r="M24" s="249"/>
       <c r="N24" s="154">
         <v>2</v>
       </c>
@@ -6652,34 +6652,34 @@
       <c r="AF24" s="156">
         <v>2</v>
       </c>
-      <c r="AG24" s="254"/>
-      <c r="AH24" s="254"/>
-      <c r="AI24" s="255"/>
-      <c r="AJ24" s="255"/>
-      <c r="AK24" s="255"/>
-      <c r="AL24" s="255"/>
-      <c r="AM24" s="255"/>
-      <c r="AN24" s="255"/>
-      <c r="AO24" s="255"/>
-      <c r="AP24" s="255"/>
-      <c r="AQ24" s="255"/>
-      <c r="AR24" s="255"/>
+      <c r="AG24" s="249"/>
+      <c r="AH24" s="249"/>
+      <c r="AI24" s="250"/>
+      <c r="AJ24" s="250"/>
+      <c r="AK24" s="250"/>
+      <c r="AL24" s="250"/>
+      <c r="AM24" s="250"/>
+      <c r="AN24" s="250"/>
+      <c r="AO24" s="250"/>
+      <c r="AP24" s="250"/>
+      <c r="AQ24" s="250"/>
+      <c r="AR24" s="250"/>
       <c r="AS24" s="178"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="124"/>
-      <c r="B25" s="255"/>
-      <c r="C25" s="255"/>
-      <c r="D25" s="255"/>
-      <c r="E25" s="255"/>
-      <c r="F25" s="255"/>
-      <c r="G25" s="255"/>
-      <c r="H25" s="255"/>
-      <c r="I25" s="255"/>
-      <c r="J25" s="255"/>
-      <c r="K25" s="255"/>
-      <c r="L25" s="254"/>
-      <c r="M25" s="254"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="249"/>
+      <c r="M25" s="249"/>
       <c r="N25" s="154">
         <v>3</v>
       </c>
@@ -6703,857 +6703,857 @@
       <c r="AF25" s="156">
         <v>3</v>
       </c>
-      <c r="AG25" s="254"/>
-      <c r="AH25" s="254"/>
-      <c r="AI25" s="255"/>
-      <c r="AJ25" s="255"/>
-      <c r="AK25" s="255"/>
-      <c r="AL25" s="255"/>
-      <c r="AM25" s="255"/>
-      <c r="AN25" s="255"/>
-      <c r="AO25" s="255"/>
-      <c r="AP25" s="255"/>
-      <c r="AQ25" s="255"/>
-      <c r="AR25" s="255"/>
+      <c r="AG25" s="249"/>
+      <c r="AH25" s="249"/>
+      <c r="AI25" s="250"/>
+      <c r="AJ25" s="250"/>
+      <c r="AK25" s="250"/>
+      <c r="AL25" s="250"/>
+      <c r="AM25" s="250"/>
+      <c r="AN25" s="250"/>
+      <c r="AO25" s="250"/>
+      <c r="AP25" s="250"/>
+      <c r="AQ25" s="250"/>
+      <c r="AR25" s="250"/>
       <c r="AS25" s="178"/>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="123"/>
-      <c r="B26" s="256"/>
-      <c r="C26" s="256"/>
-      <c r="D26" s="256"/>
-      <c r="E26" s="256"/>
-      <c r="F26" s="256"/>
-      <c r="G26" s="256"/>
-      <c r="H26" s="256"/>
-      <c r="I26" s="256"/>
-      <c r="J26" s="256"/>
-      <c r="K26" s="256"/>
-      <c r="L26" s="256"/>
-      <c r="M26" s="256"/>
+      <c r="B26" s="251"/>
+      <c r="C26" s="251"/>
+      <c r="D26" s="251"/>
+      <c r="E26" s="251"/>
+      <c r="F26" s="251"/>
+      <c r="G26" s="251"/>
+      <c r="H26" s="251"/>
+      <c r="I26" s="251"/>
+      <c r="J26" s="251"/>
+      <c r="K26" s="251"/>
+      <c r="L26" s="251"/>
+      <c r="M26" s="251"/>
       <c r="N26" s="154">
         <v>4</v>
       </c>
       <c r="O26" s="113"/>
-      <c r="P26" s="192">
+      <c r="P26" s="276">
         <v>307</v>
       </c>
-      <c r="Q26" s="192">
+      <c r="Q26" s="276">
         <v>306</v>
       </c>
-      <c r="R26" s="192">
+      <c r="R26" s="276">
         <v>305</v>
       </c>
-      <c r="S26" s="192">
+      <c r="S26" s="276">
         <v>304</v>
       </c>
-      <c r="T26" s="192">
+      <c r="T26" s="276">
         <v>303</v>
       </c>
-      <c r="U26" s="192">
+      <c r="U26" s="276">
         <v>302</v>
       </c>
-      <c r="V26" s="192">
+      <c r="V26" s="276">
         <v>301</v>
       </c>
       <c r="W26" s="161"/>
-      <c r="X26" s="192">
+      <c r="X26" s="276">
         <v>301</v>
       </c>
-      <c r="Y26" s="192">
+      <c r="Y26" s="276">
         <v>302</v>
       </c>
-      <c r="Z26" s="192">
+      <c r="Z26" s="276">
         <v>303</v>
       </c>
-      <c r="AA26" s="192">
+      <c r="AA26" s="276">
         <v>304</v>
       </c>
-      <c r="AB26" s="192">
+      <c r="AB26" s="276">
         <v>305</v>
       </c>
-      <c r="AC26" s="192">
+      <c r="AC26" s="276">
         <v>306</v>
       </c>
-      <c r="AD26" s="192">
+      <c r="AD26" s="276">
         <v>307</v>
       </c>
       <c r="AE26" s="113"/>
       <c r="AF26" s="156">
         <v>4</v>
       </c>
-      <c r="AG26" s="255"/>
-      <c r="AH26" s="267"/>
-      <c r="AI26" s="255"/>
-      <c r="AJ26" s="267"/>
-      <c r="AK26" s="255"/>
-      <c r="AL26" s="267"/>
-      <c r="AM26" s="255"/>
-      <c r="AN26" s="267"/>
-      <c r="AO26" s="255"/>
-      <c r="AP26" s="267"/>
-      <c r="AQ26" s="255"/>
-      <c r="AR26" s="267"/>
+      <c r="AG26" s="250"/>
+      <c r="AH26" s="262"/>
+      <c r="AI26" s="250"/>
+      <c r="AJ26" s="262"/>
+      <c r="AK26" s="250"/>
+      <c r="AL26" s="262"/>
+      <c r="AM26" s="250"/>
+      <c r="AN26" s="262"/>
+      <c r="AO26" s="250"/>
+      <c r="AP26" s="262"/>
+      <c r="AQ26" s="250"/>
+      <c r="AR26" s="262"/>
       <c r="AS26" s="178"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="115"/>
-      <c r="B27" s="256"/>
-      <c r="C27" s="256"/>
-      <c r="D27" s="256"/>
-      <c r="E27" s="256"/>
-      <c r="F27" s="256"/>
-      <c r="G27" s="256"/>
-      <c r="H27" s="256"/>
-      <c r="I27" s="256"/>
-      <c r="J27" s="256"/>
-      <c r="K27" s="256"/>
-      <c r="L27" s="256"/>
-      <c r="M27" s="256"/>
+      <c r="B27" s="251"/>
+      <c r="C27" s="251"/>
+      <c r="D27" s="251"/>
+      <c r="E27" s="251"/>
+      <c r="F27" s="251"/>
+      <c r="G27" s="251"/>
+      <c r="H27" s="251"/>
+      <c r="I27" s="251"/>
+      <c r="J27" s="251"/>
+      <c r="K27" s="251"/>
+      <c r="L27" s="251"/>
+      <c r="M27" s="251"/>
       <c r="N27" s="154">
         <v>5</v>
       </c>
       <c r="O27" s="113"/>
-      <c r="P27" s="192">
+      <c r="P27" s="276">
         <v>314</v>
       </c>
-      <c r="Q27" s="192">
+      <c r="Q27" s="276">
         <v>313</v>
       </c>
-      <c r="R27" s="192">
+      <c r="R27" s="276">
         <v>312</v>
       </c>
-      <c r="S27" s="192">
+      <c r="S27" s="276">
         <v>311</v>
       </c>
-      <c r="T27" s="192">
+      <c r="T27" s="276">
         <v>310</v>
       </c>
-      <c r="U27" s="192">
+      <c r="U27" s="276">
         <v>309</v>
       </c>
-      <c r="V27" s="192">
+      <c r="V27" s="276">
         <v>308</v>
       </c>
       <c r="W27" s="153"/>
-      <c r="X27" s="192">
+      <c r="X27" s="276">
         <v>308</v>
       </c>
-      <c r="Y27" s="192">
+      <c r="Y27" s="276">
         <v>309</v>
       </c>
-      <c r="Z27" s="192">
+      <c r="Z27" s="276">
         <v>310</v>
       </c>
-      <c r="AA27" s="192">
+      <c r="AA27" s="276">
         <v>311</v>
       </c>
-      <c r="AB27" s="192">
+      <c r="AB27" s="276">
         <v>312</v>
       </c>
-      <c r="AC27" s="192">
+      <c r="AC27" s="276">
         <v>313</v>
       </c>
-      <c r="AD27" s="192">
+      <c r="AD27" s="276">
         <v>314</v>
       </c>
       <c r="AE27" s="113"/>
       <c r="AF27" s="156">
         <v>5</v>
       </c>
-      <c r="AG27" s="255"/>
-      <c r="AH27" s="267"/>
-      <c r="AI27" s="255"/>
-      <c r="AJ27" s="255"/>
-      <c r="AK27" s="255"/>
-      <c r="AL27" s="255"/>
-      <c r="AM27" s="255"/>
-      <c r="AN27" s="255"/>
-      <c r="AO27" s="268"/>
-      <c r="AP27" s="255"/>
-      <c r="AQ27" s="255"/>
-      <c r="AR27" s="255"/>
+      <c r="AG27" s="250"/>
+      <c r="AH27" s="262"/>
+      <c r="AI27" s="250"/>
+      <c r="AJ27" s="250"/>
+      <c r="AK27" s="250"/>
+      <c r="AL27" s="250"/>
+      <c r="AM27" s="250"/>
+      <c r="AN27" s="250"/>
+      <c r="AO27" s="263"/>
+      <c r="AP27" s="250"/>
+      <c r="AQ27" s="250"/>
+      <c r="AR27" s="250"/>
       <c r="AS27" s="178"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="119"/>
-      <c r="B28" s="256"/>
-      <c r="C28" s="256"/>
-      <c r="D28" s="256"/>
-      <c r="E28" s="256"/>
-      <c r="F28" s="256"/>
-      <c r="G28" s="256"/>
-      <c r="H28" s="256"/>
-      <c r="I28" s="256"/>
-      <c r="J28" s="256"/>
-      <c r="K28" s="256"/>
-      <c r="L28" s="256"/>
-      <c r="M28" s="256"/>
+      <c r="B28" s="251"/>
+      <c r="C28" s="251"/>
+      <c r="D28" s="251"/>
+      <c r="E28" s="251"/>
+      <c r="F28" s="251"/>
+      <c r="G28" s="251"/>
+      <c r="H28" s="251"/>
+      <c r="I28" s="251"/>
+      <c r="J28" s="251"/>
+      <c r="K28" s="251"/>
+      <c r="L28" s="251"/>
+      <c r="M28" s="251"/>
       <c r="N28" s="154">
         <v>6</v>
       </c>
       <c r="O28" s="113"/>
-      <c r="P28" s="192">
+      <c r="P28" s="276">
         <v>321</v>
       </c>
-      <c r="Q28" s="192">
+      <c r="Q28" s="276">
         <v>320</v>
       </c>
-      <c r="R28" s="192">
+      <c r="R28" s="276">
         <v>319</v>
       </c>
-      <c r="S28" s="192">
+      <c r="S28" s="276">
         <v>318</v>
       </c>
-      <c r="T28" s="192">
+      <c r="T28" s="276">
         <v>317</v>
       </c>
-      <c r="U28" s="192">
+      <c r="U28" s="276">
         <v>316</v>
       </c>
-      <c r="V28" s="192">
+      <c r="V28" s="276">
         <v>315</v>
       </c>
       <c r="W28" s="153"/>
-      <c r="X28" s="192">
+      <c r="X28" s="276">
         <v>315</v>
       </c>
-      <c r="Y28" s="192">
+      <c r="Y28" s="276">
         <v>316</v>
       </c>
-      <c r="Z28" s="192">
+      <c r="Z28" s="276">
         <v>317</v>
       </c>
-      <c r="AA28" s="192">
+      <c r="AA28" s="276">
         <v>318</v>
       </c>
-      <c r="AB28" s="192">
+      <c r="AB28" s="276">
         <v>319</v>
       </c>
-      <c r="AC28" s="192">
+      <c r="AC28" s="276">
         <v>320</v>
       </c>
-      <c r="AD28" s="192">
+      <c r="AD28" s="276">
         <v>321</v>
       </c>
       <c r="AE28" s="158"/>
       <c r="AF28" s="156">
         <v>6</v>
       </c>
-      <c r="AG28" s="255"/>
-      <c r="AH28" s="267"/>
-      <c r="AI28" s="255"/>
-      <c r="AJ28" s="255"/>
-      <c r="AK28" s="255"/>
-      <c r="AL28" s="255"/>
-      <c r="AM28" s="255"/>
-      <c r="AN28" s="255"/>
-      <c r="AO28" s="255"/>
-      <c r="AP28" s="255"/>
-      <c r="AQ28" s="255"/>
-      <c r="AR28" s="255"/>
+      <c r="AG28" s="250"/>
+      <c r="AH28" s="262"/>
+      <c r="AI28" s="250"/>
+      <c r="AJ28" s="250"/>
+      <c r="AK28" s="250"/>
+      <c r="AL28" s="250"/>
+      <c r="AM28" s="250"/>
+      <c r="AN28" s="250"/>
+      <c r="AO28" s="250"/>
+      <c r="AP28" s="250"/>
+      <c r="AQ28" s="250"/>
+      <c r="AR28" s="250"/>
       <c r="AS28" s="179"/>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="127"/>
-      <c r="B29" s="257"/>
-      <c r="C29" s="257"/>
-      <c r="D29" s="257"/>
-      <c r="E29" s="257"/>
-      <c r="F29" s="257"/>
-      <c r="G29" s="257"/>
-      <c r="H29" s="257"/>
-      <c r="I29" s="257"/>
-      <c r="J29" s="257"/>
-      <c r="K29" s="257"/>
-      <c r="L29" s="257"/>
-      <c r="M29" s="257"/>
+      <c r="B29" s="252"/>
+      <c r="C29" s="252"/>
+      <c r="D29" s="252"/>
+      <c r="E29" s="252"/>
+      <c r="F29" s="252"/>
+      <c r="G29" s="252"/>
+      <c r="H29" s="252"/>
+      <c r="I29" s="252"/>
+      <c r="J29" s="252"/>
+      <c r="K29" s="252"/>
+      <c r="L29" s="252"/>
+      <c r="M29" s="252"/>
       <c r="N29" s="154">
         <v>7</v>
       </c>
       <c r="O29" s="113"/>
-      <c r="P29" s="192">
+      <c r="P29" s="276">
         <v>328</v>
       </c>
-      <c r="Q29" s="192">
+      <c r="Q29" s="276">
         <v>327</v>
       </c>
-      <c r="R29" s="237">
+      <c r="R29" s="235">
         <v>326</v>
       </c>
-      <c r="S29" s="245" t="s">
+      <c r="S29" s="240" t="s">
         <v>778</v>
       </c>
-      <c r="T29" s="250" t="s">
+      <c r="T29" s="245" t="s">
         <v>364</v>
       </c>
-      <c r="U29" s="193">
+      <c r="U29" s="192">
         <v>323</v>
       </c>
-      <c r="V29" s="193">
+      <c r="V29" s="192">
         <v>322</v>
       </c>
       <c r="W29" s="153"/>
-      <c r="X29" s="193">
+      <c r="X29" s="192">
         <v>322</v>
       </c>
-      <c r="Y29" s="193">
+      <c r="Y29" s="192">
         <v>323</v>
       </c>
-      <c r="Z29" s="193">
+      <c r="Z29" s="192">
         <v>324</v>
       </c>
-      <c r="AA29" s="193">
+      <c r="AA29" s="192">
         <v>325</v>
       </c>
-      <c r="AB29" s="193">
+      <c r="AB29" s="192">
         <v>326</v>
       </c>
-      <c r="AC29" s="193">
+      <c r="AC29" s="192">
         <v>327</v>
       </c>
-      <c r="AD29" s="193">
+      <c r="AD29" s="192">
         <v>328</v>
       </c>
       <c r="AE29" s="113"/>
       <c r="AF29" s="156">
         <v>7</v>
       </c>
-      <c r="AG29" s="264"/>
-      <c r="AH29" s="263"/>
-      <c r="AI29" s="264"/>
-      <c r="AJ29" s="263"/>
-      <c r="AK29" s="264"/>
-      <c r="AL29" s="263"/>
-      <c r="AM29" s="264"/>
-      <c r="AN29" s="263"/>
-      <c r="AO29" s="264"/>
-      <c r="AP29" s="263"/>
-      <c r="AQ29" s="264"/>
-      <c r="AR29" s="263"/>
+      <c r="AG29" s="259"/>
+      <c r="AH29" s="258"/>
+      <c r="AI29" s="259"/>
+      <c r="AJ29" s="258"/>
+      <c r="AK29" s="259"/>
+      <c r="AL29" s="258"/>
+      <c r="AM29" s="259"/>
+      <c r="AN29" s="258"/>
+      <c r="AO29" s="259"/>
+      <c r="AP29" s="258"/>
+      <c r="AQ29" s="259"/>
+      <c r="AR29" s="258"/>
       <c r="AS29" s="178"/>
     </row>
     <row r="30" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="115"/>
-      <c r="B30" s="255"/>
-      <c r="C30" s="255"/>
-      <c r="D30" s="255"/>
-      <c r="E30" s="255"/>
-      <c r="F30" s="255"/>
-      <c r="G30" s="255"/>
-      <c r="H30" s="255"/>
-      <c r="I30" s="255"/>
-      <c r="J30" s="255"/>
-      <c r="K30" s="255"/>
-      <c r="L30" s="255"/>
-      <c r="M30" s="255"/>
+      <c r="B30" s="250"/>
+      <c r="C30" s="250"/>
+      <c r="D30" s="250"/>
+      <c r="E30" s="250"/>
+      <c r="F30" s="250"/>
+      <c r="G30" s="250"/>
+      <c r="H30" s="250"/>
+      <c r="I30" s="250"/>
+      <c r="J30" s="250"/>
+      <c r="K30" s="250"/>
+      <c r="L30" s="250"/>
+      <c r="M30" s="250"/>
       <c r="N30" s="113">
         <v>8</v>
       </c>
-      <c r="O30" s="248"/>
-      <c r="P30" s="251">
+      <c r="O30" s="243"/>
+      <c r="P30" s="246">
         <v>335</v>
       </c>
-      <c r="Q30" s="193">
+      <c r="Q30" s="192">
         <v>334</v>
       </c>
-      <c r="R30" s="193">
+      <c r="R30" s="192">
         <v>333</v>
       </c>
-      <c r="S30" s="193">
+      <c r="S30" s="192">
         <v>332</v>
       </c>
-      <c r="T30" s="193">
+      <c r="T30" s="192">
         <v>331</v>
       </c>
-      <c r="U30" s="193">
+      <c r="U30" s="192">
         <v>330</v>
       </c>
-      <c r="V30" s="193">
+      <c r="V30" s="192">
         <v>329</v>
       </c>
       <c r="W30" s="162"/>
-      <c r="X30" s="193">
+      <c r="X30" s="192">
         <v>329</v>
       </c>
-      <c r="Y30" s="193">
+      <c r="Y30" s="192">
         <v>330</v>
       </c>
-      <c r="Z30" s="193">
+      <c r="Z30" s="192">
         <v>331</v>
       </c>
-      <c r="AA30" s="193">
+      <c r="AA30" s="192">
         <v>332</v>
       </c>
-      <c r="AB30" s="193">
+      <c r="AB30" s="192">
         <v>333</v>
       </c>
-      <c r="AC30" s="193">
+      <c r="AC30" s="192">
         <v>334</v>
       </c>
-      <c r="AD30" s="193">
+      <c r="AD30" s="192">
         <v>335</v>
       </c>
       <c r="AE30" s="113"/>
       <c r="AF30" s="159">
         <v>8</v>
       </c>
-      <c r="AG30" s="255"/>
-      <c r="AH30" s="267"/>
-      <c r="AI30" s="255"/>
-      <c r="AJ30" s="255"/>
-      <c r="AK30" s="255"/>
-      <c r="AL30" s="255"/>
-      <c r="AM30" s="255"/>
-      <c r="AN30" s="255"/>
-      <c r="AO30" s="255"/>
-      <c r="AP30" s="255"/>
-      <c r="AQ30" s="255"/>
-      <c r="AR30" s="255"/>
+      <c r="AG30" s="250"/>
+      <c r="AH30" s="262"/>
+      <c r="AI30" s="250"/>
+      <c r="AJ30" s="250"/>
+      <c r="AK30" s="250"/>
+      <c r="AL30" s="250"/>
+      <c r="AM30" s="250"/>
+      <c r="AN30" s="250"/>
+      <c r="AO30" s="250"/>
+      <c r="AP30" s="250"/>
+      <c r="AQ30" s="250"/>
+      <c r="AR30" s="250"/>
     </row>
     <row r="31" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="115"/>
-      <c r="B31" s="255"/>
-      <c r="C31" s="255"/>
-      <c r="D31" s="255"/>
-      <c r="E31" s="255"/>
-      <c r="F31" s="255"/>
-      <c r="G31" s="255"/>
-      <c r="H31" s="255"/>
-      <c r="I31" s="255"/>
-      <c r="J31" s="255"/>
-      <c r="K31" s="255"/>
-      <c r="L31" s="255"/>
-      <c r="M31" s="255"/>
+      <c r="B31" s="250"/>
+      <c r="C31" s="250"/>
+      <c r="D31" s="250"/>
+      <c r="E31" s="250"/>
+      <c r="F31" s="250"/>
+      <c r="G31" s="250"/>
+      <c r="H31" s="250"/>
+      <c r="I31" s="250"/>
+      <c r="J31" s="250"/>
+      <c r="K31" s="250"/>
+      <c r="L31" s="250"/>
+      <c r="M31" s="250"/>
       <c r="N31" s="154">
         <v>9</v>
       </c>
       <c r="O31" s="125"/>
-      <c r="P31" s="193">
+      <c r="P31" s="192">
         <v>342</v>
       </c>
-      <c r="Q31" s="193">
+      <c r="Q31" s="192">
         <v>341</v>
       </c>
-      <c r="R31" s="193">
+      <c r="R31" s="192">
         <v>340</v>
       </c>
-      <c r="S31" s="193">
+      <c r="S31" s="192">
         <v>339</v>
       </c>
-      <c r="T31" s="193">
+      <c r="T31" s="192">
         <v>338</v>
       </c>
-      <c r="U31" s="193">
+      <c r="U31" s="192">
         <v>337</v>
       </c>
-      <c r="V31" s="193">
+      <c r="V31" s="192">
         <v>336</v>
       </c>
       <c r="W31" s="163"/>
-      <c r="X31" s="193">
+      <c r="X31" s="192">
         <v>336</v>
       </c>
-      <c r="Y31" s="193">
+      <c r="Y31" s="192">
         <v>337</v>
       </c>
-      <c r="Z31" s="193">
+      <c r="Z31" s="192">
         <v>338</v>
       </c>
-      <c r="AA31" s="193">
+      <c r="AA31" s="192">
         <v>339</v>
       </c>
-      <c r="AB31" s="193">
+      <c r="AB31" s="192">
         <v>340</v>
       </c>
-      <c r="AC31" s="193">
+      <c r="AC31" s="192">
         <v>341</v>
       </c>
-      <c r="AD31" s="193">
+      <c r="AD31" s="192">
         <v>342</v>
       </c>
       <c r="AE31" s="115"/>
       <c r="AF31" s="185">
         <v>9</v>
       </c>
-      <c r="AG31" s="255"/>
-      <c r="AH31" s="267"/>
-      <c r="AI31" s="255"/>
-      <c r="AJ31" s="255"/>
-      <c r="AK31" s="255"/>
-      <c r="AL31" s="255"/>
-      <c r="AM31" s="255"/>
-      <c r="AN31" s="255"/>
-      <c r="AO31" s="255"/>
-      <c r="AP31" s="255"/>
-      <c r="AQ31" s="255"/>
-      <c r="AR31" s="255"/>
+      <c r="AG31" s="250"/>
+      <c r="AH31" s="262"/>
+      <c r="AI31" s="250"/>
+      <c r="AJ31" s="250"/>
+      <c r="AK31" s="250"/>
+      <c r="AL31" s="250"/>
+      <c r="AM31" s="250"/>
+      <c r="AN31" s="250"/>
+      <c r="AO31" s="250"/>
+      <c r="AP31" s="250"/>
+      <c r="AQ31" s="250"/>
+      <c r="AR31" s="250"/>
     </row>
     <row r="32" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="115"/>
-      <c r="B32" s="255"/>
-      <c r="C32" s="255"/>
-      <c r="D32" s="255"/>
-      <c r="E32" s="255"/>
-      <c r="F32" s="255"/>
-      <c r="G32" s="255"/>
-      <c r="H32" s="255"/>
-      <c r="I32" s="255"/>
-      <c r="J32" s="255"/>
-      <c r="K32" s="255"/>
-      <c r="L32" s="255"/>
-      <c r="M32" s="255"/>
+      <c r="B32" s="250"/>
+      <c r="C32" s="250"/>
+      <c r="D32" s="250"/>
+      <c r="E32" s="250"/>
+      <c r="F32" s="250"/>
+      <c r="G32" s="250"/>
+      <c r="H32" s="250"/>
+      <c r="I32" s="250"/>
+      <c r="J32" s="250"/>
+      <c r="K32" s="250"/>
+      <c r="L32" s="250"/>
+      <c r="M32" s="250"/>
       <c r="N32" s="184">
         <v>10</v>
       </c>
       <c r="O32" s="115"/>
-      <c r="P32" s="193">
+      <c r="P32" s="192">
         <v>349</v>
       </c>
-      <c r="Q32" s="193">
+      <c r="Q32" s="192">
         <v>348</v>
       </c>
-      <c r="R32" s="193">
+      <c r="R32" s="192">
         <v>347</v>
       </c>
-      <c r="S32" s="193">
+      <c r="S32" s="192">
         <v>346</v>
       </c>
-      <c r="T32" s="193">
+      <c r="T32" s="192">
         <v>345</v>
       </c>
-      <c r="U32" s="193">
+      <c r="U32" s="192">
         <v>344</v>
       </c>
-      <c r="V32" s="193">
+      <c r="V32" s="192">
         <v>343</v>
       </c>
       <c r="W32" s="163"/>
-      <c r="X32" s="193">
+      <c r="X32" s="192">
         <v>343</v>
       </c>
-      <c r="Y32" s="193">
+      <c r="Y32" s="192">
         <v>344</v>
       </c>
-      <c r="Z32" s="193">
+      <c r="Z32" s="192">
         <v>345</v>
       </c>
-      <c r="AA32" s="193">
+      <c r="AA32" s="192">
         <v>346</v>
       </c>
-      <c r="AB32" s="193">
+      <c r="AB32" s="192">
         <v>347</v>
       </c>
-      <c r="AC32" s="193">
+      <c r="AC32" s="192">
         <v>348</v>
       </c>
-      <c r="AD32" s="193">
+      <c r="AD32" s="192">
         <v>349</v>
       </c>
       <c r="AE32" s="115"/>
       <c r="AF32" s="185">
         <v>10</v>
       </c>
-      <c r="AG32" s="255"/>
-      <c r="AH32" s="267"/>
-      <c r="AI32" s="255"/>
-      <c r="AJ32" s="255"/>
-      <c r="AK32" s="255"/>
-      <c r="AL32" s="255"/>
-      <c r="AM32" s="255"/>
-      <c r="AN32" s="255"/>
-      <c r="AO32" s="255"/>
-      <c r="AP32" s="255"/>
-      <c r="AQ32" s="255"/>
-      <c r="AR32" s="255"/>
+      <c r="AG32" s="250"/>
+      <c r="AH32" s="262"/>
+      <c r="AI32" s="250"/>
+      <c r="AJ32" s="250"/>
+      <c r="AK32" s="250"/>
+      <c r="AL32" s="250"/>
+      <c r="AM32" s="250"/>
+      <c r="AN32" s="250"/>
+      <c r="AO32" s="250"/>
+      <c r="AP32" s="250"/>
+      <c r="AQ32" s="250"/>
+      <c r="AR32" s="250"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
-      <c r="B33" s="255"/>
-      <c r="C33" s="255"/>
-      <c r="D33" s="255"/>
-      <c r="E33" s="255"/>
-      <c r="F33" s="255"/>
-      <c r="G33" s="255"/>
-      <c r="H33" s="255"/>
-      <c r="I33" s="255"/>
-      <c r="J33" s="255"/>
-      <c r="K33" s="255"/>
-      <c r="L33" s="255"/>
-      <c r="M33" s="255"/>
+      <c r="B33" s="250"/>
+      <c r="C33" s="250"/>
+      <c r="D33" s="250"/>
+      <c r="E33" s="250"/>
+      <c r="F33" s="250"/>
+      <c r="G33" s="250"/>
+      <c r="H33" s="250"/>
+      <c r="I33" s="250"/>
+      <c r="J33" s="250"/>
+      <c r="K33" s="250"/>
+      <c r="L33" s="250"/>
+      <c r="M33" s="250"/>
       <c r="N33" s="186">
         <v>11</v>
       </c>
       <c r="O33" s="115"/>
-      <c r="P33" s="193">
+      <c r="P33" s="192">
         <v>356</v>
       </c>
-      <c r="Q33" s="193">
+      <c r="Q33" s="192">
         <v>355</v>
       </c>
-      <c r="R33" s="193">
+      <c r="R33" s="192">
         <v>354</v>
       </c>
-      <c r="S33" s="193">
+      <c r="S33" s="192">
         <v>353</v>
       </c>
-      <c r="T33" s="193">
+      <c r="T33" s="192">
         <v>352</v>
       </c>
-      <c r="U33" s="193">
+      <c r="U33" s="192">
         <v>351</v>
       </c>
-      <c r="V33" s="193">
+      <c r="V33" s="192">
         <v>350</v>
       </c>
       <c r="W33" s="163"/>
-      <c r="X33" s="252">
+      <c r="X33" s="247">
         <v>350</v>
       </c>
-      <c r="Y33" s="252">
+      <c r="Y33" s="247">
         <v>351</v>
       </c>
-      <c r="Z33" s="193">
+      <c r="Z33" s="192">
         <v>352</v>
       </c>
-      <c r="AA33" s="193">
+      <c r="AA33" s="192">
         <v>353</v>
       </c>
-      <c r="AB33" s="193">
+      <c r="AB33" s="192">
         <v>354</v>
       </c>
-      <c r="AC33" s="193">
+      <c r="AC33" s="192">
         <v>355</v>
       </c>
-      <c r="AD33" s="193">
+      <c r="AD33" s="192">
         <v>356</v>
       </c>
       <c r="AE33" s="115"/>
       <c r="AF33" s="185">
         <v>11</v>
       </c>
-      <c r="AG33" s="255"/>
-      <c r="AH33" s="263"/>
-      <c r="AI33" s="255"/>
-      <c r="AJ33" s="264"/>
-      <c r="AK33" s="255"/>
-      <c r="AL33" s="264"/>
-      <c r="AM33" s="255"/>
-      <c r="AN33" s="264"/>
-      <c r="AO33" s="255"/>
-      <c r="AP33" s="264"/>
-      <c r="AQ33" s="255"/>
-      <c r="AR33" s="264"/>
+      <c r="AG33" s="250"/>
+      <c r="AH33" s="258"/>
+      <c r="AI33" s="250"/>
+      <c r="AJ33" s="259"/>
+      <c r="AK33" s="250"/>
+      <c r="AL33" s="259"/>
+      <c r="AM33" s="250"/>
+      <c r="AN33" s="259"/>
+      <c r="AO33" s="250"/>
+      <c r="AP33" s="259"/>
+      <c r="AQ33" s="250"/>
+      <c r="AR33" s="259"/>
       <c r="AS33" s="181"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="115"/>
-      <c r="B34" s="255"/>
-      <c r="C34" s="255"/>
-      <c r="D34" s="255"/>
-      <c r="E34" s="255"/>
-      <c r="F34" s="255"/>
-      <c r="G34" s="255"/>
-      <c r="H34" s="255"/>
-      <c r="I34" s="255"/>
-      <c r="J34" s="255"/>
-      <c r="K34" s="255"/>
-      <c r="L34" s="255"/>
-      <c r="M34" s="255"/>
+      <c r="B34" s="250"/>
+      <c r="C34" s="250"/>
+      <c r="D34" s="250"/>
+      <c r="E34" s="250"/>
+      <c r="F34" s="250"/>
+      <c r="G34" s="250"/>
+      <c r="H34" s="250"/>
+      <c r="I34" s="250"/>
+      <c r="J34" s="250"/>
+      <c r="K34" s="250"/>
+      <c r="L34" s="250"/>
+      <c r="M34" s="250"/>
       <c r="N34" s="186">
         <v>12</v>
       </c>
       <c r="O34" s="141"/>
-      <c r="P34" s="246" t="s">
+      <c r="P34" s="241" t="s">
         <v>777</v>
       </c>
-      <c r="Q34" s="199">
+      <c r="Q34" s="198">
         <v>362</v>
       </c>
-      <c r="R34" s="199">
+      <c r="R34" s="198">
         <v>361</v>
       </c>
-      <c r="S34" s="199">
+      <c r="S34" s="198">
         <v>360</v>
       </c>
-      <c r="T34" s="199">
+      <c r="T34" s="198">
         <v>359</v>
       </c>
-      <c r="U34" s="199">
+      <c r="U34" s="198">
         <v>358</v>
       </c>
-      <c r="V34" s="199">
+      <c r="V34" s="198">
         <v>357</v>
       </c>
       <c r="W34" s="166"/>
-      <c r="X34" s="199">
+      <c r="X34" s="198">
         <v>357</v>
       </c>
-      <c r="Y34" s="199">
+      <c r="Y34" s="198">
         <v>358</v>
       </c>
-      <c r="Z34" s="253"/>
-      <c r="AA34" s="253"/>
-      <c r="AB34" s="253"/>
-      <c r="AC34" s="253"/>
-      <c r="AD34" s="253"/>
+      <c r="Z34" s="248"/>
+      <c r="AA34" s="248"/>
+      <c r="AB34" s="248"/>
+      <c r="AC34" s="248"/>
+      <c r="AD34" s="248"/>
       <c r="AE34" s="115"/>
       <c r="AF34" s="185">
         <v>12</v>
       </c>
-      <c r="AG34" s="255"/>
-      <c r="AH34" s="263"/>
-      <c r="AI34" s="255"/>
-      <c r="AJ34" s="264"/>
-      <c r="AK34" s="255"/>
-      <c r="AL34" s="264"/>
-      <c r="AM34" s="255"/>
-      <c r="AN34" s="264"/>
-      <c r="AO34" s="255"/>
-      <c r="AP34" s="264"/>
-      <c r="AQ34" s="255"/>
-      <c r="AR34" s="264"/>
+      <c r="AG34" s="250"/>
+      <c r="AH34" s="258"/>
+      <c r="AI34" s="250"/>
+      <c r="AJ34" s="259"/>
+      <c r="AK34" s="250"/>
+      <c r="AL34" s="259"/>
+      <c r="AM34" s="250"/>
+      <c r="AN34" s="259"/>
+      <c r="AO34" s="250"/>
+      <c r="AP34" s="259"/>
+      <c r="AQ34" s="250"/>
+      <c r="AR34" s="259"/>
       <c r="AS34" s="181"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="115"/>
-      <c r="B35" s="255"/>
-      <c r="C35" s="255"/>
-      <c r="D35" s="255"/>
-      <c r="E35" s="255"/>
-      <c r="F35" s="255"/>
-      <c r="G35" s="255"/>
-      <c r="H35" s="255"/>
-      <c r="I35" s="255"/>
-      <c r="J35" s="255"/>
-      <c r="K35" s="255"/>
-      <c r="L35" s="255"/>
-      <c r="M35" s="255"/>
-      <c r="N35" s="258"/>
-      <c r="O35" s="259"/>
-      <c r="P35" s="253"/>
-      <c r="Q35" s="253"/>
-      <c r="R35" s="253"/>
-      <c r="S35" s="253"/>
-      <c r="T35" s="255"/>
-      <c r="U35" s="255"/>
-      <c r="V35" s="255"/>
-      <c r="W35" s="260"/>
-      <c r="X35" s="255"/>
-      <c r="Y35" s="255"/>
-      <c r="Z35" s="255"/>
-      <c r="AA35" s="255"/>
-      <c r="AB35" s="255"/>
-      <c r="AC35" s="255"/>
-      <c r="AD35" s="255"/>
-      <c r="AE35" s="261"/>
-      <c r="AF35" s="262"/>
-      <c r="AG35" s="255"/>
-      <c r="AH35" s="263"/>
-      <c r="AI35" s="255"/>
-      <c r="AJ35" s="264"/>
-      <c r="AK35" s="255"/>
-      <c r="AL35" s="264"/>
-      <c r="AM35" s="255"/>
-      <c r="AN35" s="264"/>
-      <c r="AO35" s="255"/>
-      <c r="AP35" s="264"/>
-      <c r="AQ35" s="255"/>
-      <c r="AR35" s="264"/>
+      <c r="B35" s="250"/>
+      <c r="C35" s="250"/>
+      <c r="D35" s="250"/>
+      <c r="E35" s="250"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="250"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="250"/>
+      <c r="L35" s="250"/>
+      <c r="M35" s="250"/>
+      <c r="N35" s="253"/>
+      <c r="O35" s="254"/>
+      <c r="P35" s="248"/>
+      <c r="Q35" s="248"/>
+      <c r="R35" s="248"/>
+      <c r="S35" s="248"/>
+      <c r="T35" s="250"/>
+      <c r="U35" s="250"/>
+      <c r="V35" s="250"/>
+      <c r="W35" s="255"/>
+      <c r="X35" s="250"/>
+      <c r="Y35" s="250"/>
+      <c r="Z35" s="250"/>
+      <c r="AA35" s="250"/>
+      <c r="AB35" s="250"/>
+      <c r="AC35" s="250"/>
+      <c r="AD35" s="250"/>
+      <c r="AE35" s="256"/>
+      <c r="AF35" s="257"/>
+      <c r="AG35" s="250"/>
+      <c r="AH35" s="258"/>
+      <c r="AI35" s="250"/>
+      <c r="AJ35" s="259"/>
+      <c r="AK35" s="250"/>
+      <c r="AL35" s="259"/>
+      <c r="AM35" s="250"/>
+      <c r="AN35" s="259"/>
+      <c r="AO35" s="250"/>
+      <c r="AP35" s="259"/>
+      <c r="AQ35" s="250"/>
+      <c r="AR35" s="259"/>
       <c r="AS35" s="181"/>
     </row>
     <row r="36" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="115"/>
-      <c r="B36" s="255"/>
-      <c r="C36" s="255"/>
-      <c r="D36" s="255"/>
-      <c r="E36" s="255"/>
-      <c r="F36" s="255"/>
-      <c r="G36" s="255"/>
-      <c r="H36" s="255"/>
-      <c r="I36" s="255"/>
-      <c r="J36" s="255"/>
-      <c r="K36" s="255"/>
-      <c r="L36" s="255"/>
-      <c r="M36" s="255"/>
-      <c r="N36" s="258"/>
-      <c r="O36" s="248"/>
-      <c r="P36" s="255"/>
-      <c r="Q36" s="255"/>
-      <c r="R36" s="255"/>
-      <c r="S36" s="255"/>
-      <c r="T36" s="255"/>
-      <c r="U36" s="255"/>
-      <c r="V36" s="255"/>
-      <c r="W36" s="260"/>
-      <c r="X36" s="253"/>
-      <c r="Y36" s="253"/>
-      <c r="Z36" s="253"/>
-      <c r="AA36" s="253"/>
-      <c r="AB36" s="253"/>
-      <c r="AC36" s="253"/>
-      <c r="AD36" s="253"/>
-      <c r="AE36" s="261"/>
-      <c r="AF36" s="262"/>
-      <c r="AG36" s="264"/>
-      <c r="AH36" s="264"/>
-      <c r="AI36" s="264"/>
-      <c r="AJ36" s="264"/>
-      <c r="AK36" s="264"/>
-      <c r="AL36" s="264"/>
-      <c r="AM36" s="264"/>
-      <c r="AN36" s="264"/>
-      <c r="AO36" s="264"/>
-      <c r="AP36" s="264"/>
-      <c r="AQ36" s="264"/>
-      <c r="AR36" s="264"/>
+      <c r="B36" s="250"/>
+      <c r="C36" s="250"/>
+      <c r="D36" s="250"/>
+      <c r="E36" s="250"/>
+      <c r="F36" s="250"/>
+      <c r="G36" s="250"/>
+      <c r="H36" s="250"/>
+      <c r="I36" s="250"/>
+      <c r="J36" s="250"/>
+      <c r="K36" s="250"/>
+      <c r="L36" s="250"/>
+      <c r="M36" s="250"/>
+      <c r="N36" s="253"/>
+      <c r="O36" s="243"/>
+      <c r="P36" s="250"/>
+      <c r="Q36" s="250"/>
+      <c r="R36" s="250"/>
+      <c r="S36" s="250"/>
+      <c r="T36" s="250"/>
+      <c r="U36" s="250"/>
+      <c r="V36" s="250"/>
+      <c r="W36" s="255"/>
+      <c r="X36" s="248"/>
+      <c r="Y36" s="248"/>
+      <c r="Z36" s="248"/>
+      <c r="AA36" s="248"/>
+      <c r="AB36" s="248"/>
+      <c r="AC36" s="248"/>
+      <c r="AD36" s="248"/>
+      <c r="AE36" s="256"/>
+      <c r="AF36" s="257"/>
+      <c r="AG36" s="259"/>
+      <c r="AH36" s="259"/>
+      <c r="AI36" s="259"/>
+      <c r="AJ36" s="259"/>
+      <c r="AK36" s="259"/>
+      <c r="AL36" s="259"/>
+      <c r="AM36" s="259"/>
+      <c r="AN36" s="259"/>
+      <c r="AO36" s="259"/>
+      <c r="AP36" s="259"/>
+      <c r="AQ36" s="259"/>
+      <c r="AR36" s="259"/>
       <c r="AS36" s="181"/>
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37" s="115"/>
-      <c r="B37" s="255"/>
-      <c r="C37" s="255"/>
-      <c r="D37" s="255"/>
-      <c r="E37" s="255"/>
-      <c r="F37" s="255"/>
-      <c r="G37" s="255"/>
-      <c r="H37" s="255"/>
-      <c r="I37" s="255"/>
-      <c r="J37" s="255"/>
-      <c r="K37" s="255"/>
-      <c r="L37" s="255"/>
-      <c r="M37" s="255"/>
-      <c r="N37" s="258"/>
-      <c r="O37" s="259"/>
-      <c r="P37" s="253"/>
-      <c r="Q37" s="253"/>
-      <c r="R37" s="253"/>
-      <c r="S37" s="253"/>
-      <c r="T37" s="253"/>
-      <c r="U37" s="253"/>
-      <c r="V37" s="253"/>
-      <c r="W37" s="260"/>
-      <c r="X37" s="253"/>
-      <c r="Y37" s="253"/>
-      <c r="Z37" s="253"/>
-      <c r="AA37" s="253"/>
-      <c r="AB37" s="253"/>
-      <c r="AC37" s="253"/>
-      <c r="AD37" s="255"/>
-      <c r="AE37" s="261"/>
-      <c r="AF37" s="262"/>
-      <c r="AG37" s="255"/>
-      <c r="AH37" s="265"/>
-      <c r="AI37" s="255"/>
-      <c r="AJ37" s="266"/>
-      <c r="AK37" s="255"/>
-      <c r="AL37" s="266"/>
-      <c r="AM37" s="255"/>
-      <c r="AN37" s="266"/>
-      <c r="AO37" s="255"/>
-      <c r="AP37" s="266"/>
-      <c r="AQ37" s="255"/>
-      <c r="AR37" s="266"/>
+      <c r="B37" s="250"/>
+      <c r="C37" s="250"/>
+      <c r="D37" s="250"/>
+      <c r="E37" s="250"/>
+      <c r="F37" s="250"/>
+      <c r="G37" s="250"/>
+      <c r="H37" s="250"/>
+      <c r="I37" s="250"/>
+      <c r="J37" s="250"/>
+      <c r="K37" s="250"/>
+      <c r="L37" s="250"/>
+      <c r="M37" s="250"/>
+      <c r="N37" s="253"/>
+      <c r="O37" s="254"/>
+      <c r="P37" s="248"/>
+      <c r="Q37" s="248"/>
+      <c r="R37" s="248"/>
+      <c r="S37" s="248"/>
+      <c r="T37" s="248"/>
+      <c r="U37" s="248"/>
+      <c r="V37" s="248"/>
+      <c r="W37" s="255"/>
+      <c r="X37" s="248"/>
+      <c r="Y37" s="248"/>
+      <c r="Z37" s="248"/>
+      <c r="AA37" s="248"/>
+      <c r="AB37" s="248"/>
+      <c r="AC37" s="248"/>
+      <c r="AD37" s="250"/>
+      <c r="AE37" s="256"/>
+      <c r="AF37" s="257"/>
+      <c r="AG37" s="250"/>
+      <c r="AH37" s="260"/>
+      <c r="AI37" s="250"/>
+      <c r="AJ37" s="261"/>
+      <c r="AK37" s="250"/>
+      <c r="AL37" s="261"/>
+      <c r="AM37" s="250"/>
+      <c r="AN37" s="261"/>
+      <c r="AO37" s="250"/>
+      <c r="AP37" s="261"/>
+      <c r="AQ37" s="250"/>
+      <c r="AR37" s="261"/>
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38" s="115"/>
@@ -7981,55 +7981,55 @@
       <c r="AQ47" s="115"/>
     </row>
     <row r="48" spans="1:45" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="223" t="s">
+      <c r="A48" s="221" t="s">
         <v>758</v>
       </c>
-      <c r="B48" s="229"/>
-      <c r="C48" s="224"/>
-      <c r="D48" s="224"/>
-      <c r="E48" s="224"/>
-      <c r="F48" s="224"/>
-      <c r="G48" s="224"/>
-      <c r="H48" s="224"/>
+      <c r="B48" s="227"/>
+      <c r="C48" s="222"/>
+      <c r="D48" s="222"/>
+      <c r="E48" s="222"/>
+      <c r="F48" s="222"/>
+      <c r="G48" s="222"/>
+      <c r="H48" s="222"/>
       <c r="I48" s="176"/>
       <c r="J48" s="176"/>
       <c r="K48" s="176"/>
       <c r="L48" s="176"/>
       <c r="M48" s="176"/>
-      <c r="N48" s="231" t="s">
+      <c r="N48" s="229" t="s">
         <v>758</v>
       </c>
-      <c r="O48" s="204">
+      <c r="O48" s="203">
         <v>6</v>
       </c>
-      <c r="P48" s="215" t="s">
+      <c r="P48" s="213" t="s">
         <v>765</v>
       </c>
-      <c r="Q48" s="232"/>
-      <c r="R48" s="233"/>
-      <c r="S48" s="234"/>
-      <c r="T48" s="234"/>
-      <c r="U48" s="234"/>
+      <c r="Q48" s="230"/>
+      <c r="R48" s="231"/>
+      <c r="S48" s="232"/>
+      <c r="T48" s="232"/>
+      <c r="U48" s="232"/>
       <c r="V48" s="143"/>
       <c r="W48" s="143"/>
       <c r="X48" s="143"/>
       <c r="Y48" s="143"/>
       <c r="Z48" s="115"/>
-      <c r="AA48" s="230" t="s">
+      <c r="AA48" s="228" t="s">
         <v>758</v>
       </c>
-      <c r="AB48" s="216">
+      <c r="AB48" s="214">
         <v>1</v>
       </c>
-      <c r="AC48" s="215" t="s">
+      <c r="AC48" s="213" t="s">
         <v>769</v>
       </c>
-      <c r="AD48" s="234"/>
-      <c r="AE48" s="234"/>
-      <c r="AF48" s="234"/>
-      <c r="AG48" s="234"/>
-      <c r="AH48" s="214"/>
-      <c r="AI48" s="214"/>
+      <c r="AD48" s="232"/>
+      <c r="AE48" s="232"/>
+      <c r="AF48" s="232"/>
+      <c r="AG48" s="232"/>
+      <c r="AH48" s="212"/>
+      <c r="AI48" s="212"/>
       <c r="AJ48" s="115"/>
       <c r="AK48" s="115"/>
       <c r="AL48" s="115"/>
@@ -8040,32 +8040,32 @@
       <c r="AQ48" s="115"/>
     </row>
     <row r="49" spans="1:43" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="220" t="s">
+      <c r="A49" s="218" t="s">
         <v>759</v>
       </c>
-      <c r="B49" s="203">
+      <c r="B49" s="202">
         <v>120</v>
       </c>
-      <c r="C49" s="227" t="s">
+      <c r="C49" s="225" t="s">
         <v>757</v>
       </c>
-      <c r="D49" s="228"/>
-      <c r="E49" s="228"/>
-      <c r="F49" s="228"/>
-      <c r="G49" s="228"/>
-      <c r="H49" s="228"/>
+      <c r="D49" s="226"/>
+      <c r="E49" s="226"/>
+      <c r="F49" s="226"/>
+      <c r="G49" s="226"/>
+      <c r="H49" s="226"/>
       <c r="I49" s="176"/>
       <c r="J49" s="176"/>
       <c r="K49" s="176"/>
       <c r="L49" s="176"/>
       <c r="M49" s="176"/>
-      <c r="N49" s="219" t="s">
+      <c r="N49" s="217" t="s">
         <v>759</v>
       </c>
-      <c r="O49" s="241">
+      <c r="O49" s="280">
         <v>1</v>
       </c>
-      <c r="P49" s="211" t="s">
+      <c r="P49" s="209" t="s">
         <v>766</v>
       </c>
       <c r="Q49" s="142"/>
@@ -8078,13 +8078,13 @@
       <c r="X49" s="143"/>
       <c r="Y49" s="143"/>
       <c r="Z49" s="115"/>
-      <c r="AA49" s="208" t="s">
+      <c r="AA49" s="207" t="s">
         <v>759</v>
       </c>
-      <c r="AB49" s="210">
+      <c r="AB49" s="208">
         <v>66</v>
       </c>
-      <c r="AC49" s="211" t="s">
+      <c r="AC49" s="209" t="s">
         <v>764</v>
       </c>
       <c r="AD49" s="143"/>
@@ -8103,28 +8103,28 @@
       <c r="AQ49" s="115"/>
     </row>
     <row r="50" spans="1:43" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="222" t="s">
+      <c r="A50" s="220" t="s">
         <v>756</v>
       </c>
-      <c r="B50" s="229"/>
-      <c r="C50" s="200"/>
-      <c r="D50" s="201"/>
-      <c r="E50" s="201"/>
-      <c r="F50" s="201"/>
-      <c r="G50" s="201"/>
-      <c r="H50" s="201"/>
+      <c r="B50" s="227"/>
+      <c r="C50" s="199"/>
+      <c r="D50" s="200"/>
+      <c r="E50" s="200"/>
+      <c r="F50" s="200"/>
+      <c r="G50" s="200"/>
+      <c r="H50" s="200"/>
       <c r="I50" s="170"/>
       <c r="J50" s="170"/>
       <c r="K50" s="170"/>
       <c r="L50" s="170"/>
       <c r="M50" s="170"/>
-      <c r="N50" s="219" t="s">
+      <c r="N50" s="217" t="s">
         <v>760</v>
       </c>
-      <c r="O50" s="213">
+      <c r="O50" s="211">
         <v>6</v>
       </c>
-      <c r="P50" s="211" t="s">
+      <c r="P50" s="209" t="s">
         <v>767</v>
       </c>
       <c r="Q50" s="143"/>
@@ -8137,21 +8137,21 @@
       <c r="X50" s="143"/>
       <c r="Y50" s="143"/>
       <c r="Z50" s="115"/>
-      <c r="AA50" s="235" t="s">
+      <c r="AA50" s="233" t="s">
         <v>763</v>
       </c>
-      <c r="AB50" s="247">
+      <c r="AB50" s="242">
         <v>9</v>
       </c>
-      <c r="AC50" s="212" t="s">
+      <c r="AC50" s="210" t="s">
         <v>770</v>
       </c>
       <c r="AD50" s="174"/>
       <c r="AE50" s="174"/>
       <c r="AF50" s="174"/>
       <c r="AG50" s="174"/>
-      <c r="AH50" s="207"/>
-      <c r="AI50" s="207"/>
+      <c r="AH50" s="206"/>
+      <c r="AI50" s="206"/>
       <c r="AJ50" s="115"/>
       <c r="AK50" s="115"/>
       <c r="AL50" s="115"/>
@@ -8172,13 +8172,13 @@
       <c r="K51" s="170"/>
       <c r="L51" s="170"/>
       <c r="M51" s="170"/>
-      <c r="N51" s="225" t="s">
+      <c r="N51" s="223" t="s">
         <v>756</v>
       </c>
-      <c r="O51" s="205">
+      <c r="O51" s="204">
         <v>10</v>
       </c>
-      <c r="P51" s="226" t="s">
+      <c r="P51" s="224" t="s">
         <v>768</v>
       </c>
       <c r="Q51" s="143"/>
@@ -8207,7 +8207,7 @@
       <c r="AQ51" s="115"/>
     </row>
     <row r="52" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="211"/>
+      <c r="D52" s="209"/>
       <c r="E52" s="170"/>
       <c r="F52" s="170"/>
       <c r="G52" s="170"/>
@@ -8217,11 +8217,11 @@
       <c r="K52" s="170"/>
       <c r="L52" s="170"/>
       <c r="M52" s="170"/>
-      <c r="N52" s="202"/>
-      <c r="O52" s="209">
+      <c r="N52" s="201"/>
+      <c r="O52" s="277">
         <v>500</v>
       </c>
-      <c r="P52" s="212" t="s">
+      <c r="P52" s="210" t="s">
         <v>776</v>
       </c>
       <c r="Q52" s="174"/>
@@ -8295,14 +8295,14 @@
       <c r="AQ53" s="115"/>
     </row>
     <row r="54" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A54" s="211"/>
-      <c r="B54" s="211"/>
-      <c r="C54" s="211"/>
-      <c r="D54" s="211"/>
-      <c r="E54" s="211"/>
-      <c r="F54" s="211"/>
-      <c r="G54" s="211"/>
-      <c r="H54" s="211"/>
+      <c r="A54" s="209"/>
+      <c r="B54" s="209"/>
+      <c r="C54" s="209"/>
+      <c r="D54" s="209"/>
+      <c r="E54" s="209"/>
+      <c r="F54" s="209"/>
+      <c r="G54" s="209"/>
+      <c r="H54" s="209"/>
       <c r="I54" s="170"/>
       <c r="J54" s="170"/>
       <c r="K54" s="170"/>
@@ -8322,7 +8322,7 @@
       <c r="Y54" s="143"/>
       <c r="Z54" s="143"/>
       <c r="AA54" s="143"/>
-      <c r="AB54" s="218"/>
+      <c r="AB54" s="216"/>
       <c r="AC54" s="143"/>
       <c r="AD54" s="143"/>
       <c r="AE54" s="115"/>
@@ -8340,7 +8340,7 @@
       <c r="AQ54" s="115"/>
     </row>
     <row r="55" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="B55" s="194"/>
+      <c r="B55" s="193"/>
       <c r="C55" s="170"/>
       <c r="D55" s="170"/>
       <c r="E55" s="170"/>
@@ -8353,7 +8353,7 @@
       <c r="L55" s="170"/>
       <c r="M55" s="170"/>
       <c r="N55" s="115"/>
-      <c r="O55" s="206">
+      <c r="O55" s="205">
         <v>3</v>
       </c>
       <c r="P55" s="143"/>
@@ -8368,7 +8368,7 @@
       <c r="Y55" s="143"/>
       <c r="Z55" s="143"/>
       <c r="AA55" s="143"/>
-      <c r="AB55" s="217"/>
+      <c r="AB55" s="215"/>
       <c r="AC55" s="143"/>
       <c r="AD55" s="143"/>
       <c r="AE55" s="115"/>
@@ -8386,50 +8386,50 @@
       <c r="AQ55" s="115"/>
     </row>
     <row r="56" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A56" s="276">
+      <c r="A56" s="273">
         <f>SUM(B48:B50,O48:O52,AB48:AB50)</f>
         <v>719</v>
       </c>
-      <c r="B56" s="276"/>
-      <c r="C56" s="276"/>
-      <c r="D56" s="276"/>
-      <c r="E56" s="276"/>
-      <c r="F56" s="276"/>
-      <c r="G56" s="276"/>
-      <c r="H56" s="276"/>
-      <c r="I56" s="276"/>
-      <c r="J56" s="276"/>
-      <c r="K56" s="276"/>
-      <c r="L56" s="276"/>
-      <c r="M56" s="276"/>
-      <c r="N56" s="276"/>
-      <c r="O56" s="277"/>
-      <c r="P56" s="276"/>
-      <c r="Q56" s="276"/>
-      <c r="R56" s="276"/>
-      <c r="S56" s="276"/>
-      <c r="T56" s="276"/>
-      <c r="U56" s="276"/>
-      <c r="V56" s="276"/>
-      <c r="W56" s="276"/>
-      <c r="X56" s="276"/>
-      <c r="Y56" s="276"/>
-      <c r="Z56" s="276"/>
-      <c r="AA56" s="276"/>
-      <c r="AB56" s="277"/>
-      <c r="AC56" s="276"/>
-      <c r="AD56" s="276"/>
-      <c r="AE56" s="276"/>
-      <c r="AF56" s="276"/>
-      <c r="AG56" s="276"/>
-      <c r="AH56" s="276"/>
-      <c r="AI56" s="276"/>
-      <c r="AJ56" s="276"/>
-      <c r="AK56" s="276"/>
+      <c r="B56" s="273"/>
+      <c r="C56" s="273"/>
+      <c r="D56" s="273"/>
+      <c r="E56" s="273"/>
+      <c r="F56" s="273"/>
+      <c r="G56" s="273"/>
+      <c r="H56" s="273"/>
+      <c r="I56" s="273"/>
+      <c r="J56" s="273"/>
+      <c r="K56" s="273"/>
+      <c r="L56" s="273"/>
+      <c r="M56" s="273"/>
+      <c r="N56" s="273"/>
+      <c r="O56" s="274"/>
+      <c r="P56" s="273"/>
+      <c r="Q56" s="273"/>
+      <c r="R56" s="273"/>
+      <c r="S56" s="273"/>
+      <c r="T56" s="273"/>
+      <c r="U56" s="273"/>
+      <c r="V56" s="273"/>
+      <c r="W56" s="273"/>
+      <c r="X56" s="273"/>
+      <c r="Y56" s="273"/>
+      <c r="Z56" s="273"/>
+      <c r="AA56" s="273"/>
+      <c r="AB56" s="274"/>
+      <c r="AC56" s="273"/>
+      <c r="AD56" s="273"/>
+      <c r="AE56" s="273"/>
+      <c r="AF56" s="273"/>
+      <c r="AG56" s="273"/>
+      <c r="AH56" s="273"/>
+      <c r="AI56" s="273"/>
+      <c r="AJ56" s="273"/>
+      <c r="AK56" s="273"/>
     </row>
     <row r="58" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H58" s="275"/>
-      <c r="I58" s="275"/>
+      <c r="H58" s="272"/>
+      <c r="I58" s="272"/>
     </row>
     <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AA60" s="13"/>
@@ -8447,8 +8447,8 @@
       <c r="AJ66" s="131"/>
     </row>
     <row r="67" spans="13:36" x14ac:dyDescent="0.2">
-      <c r="AI67" s="269"/>
-      <c r="AJ67" s="269"/>
+      <c r="AI67" s="266"/>
+      <c r="AJ67" s="266"/>
     </row>
     <row r="68" spans="13:36" x14ac:dyDescent="0.2">
       <c r="AI68" s="113"/>

</xml_diff>